<commit_message>
Alien disguises (missing parts and power up)
Former-commit-id: e5722972f0b2d42fef6450520e1289f7985df17f
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="424">
   <si>
     <t>[sku]</t>
   </si>
@@ -1218,6 +1218,84 @@
   </si>
   <si>
     <t>TID_DRAGON_DARK_4_DESC</t>
+  </si>
+  <si>
+    <t>dragon_alien_0</t>
+  </si>
+  <si>
+    <t>dragon_alien_1</t>
+  </si>
+  <si>
+    <t>dragon_alien_2</t>
+  </si>
+  <si>
+    <t>dragon_alien_3</t>
+  </si>
+  <si>
+    <t>dragon_alien_4</t>
+  </si>
+  <si>
+    <t>dragon_alien</t>
+  </si>
+  <si>
+    <t>icon_alien_0</t>
+  </si>
+  <si>
+    <t>icon_alien_1</t>
+  </si>
+  <si>
+    <t>icon_alien_2</t>
+  </si>
+  <si>
+    <t>icon_alien_3</t>
+  </si>
+  <si>
+    <t>icon_alien_4</t>
+  </si>
+  <si>
+    <t>TID_SKIN_ALIEN_0_NAME</t>
+  </si>
+  <si>
+    <t>TID_SKIN_ALIEN_1_NAME</t>
+  </si>
+  <si>
+    <t>TID_SKIN_ALIEN_2_NAME</t>
+  </si>
+  <si>
+    <t>TID_SKIN_ALIEN_3_NAME</t>
+  </si>
+  <si>
+    <t>TID_SKIN_ALIEN_4_NAME</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_ALIEN_0_DESC</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_ALIEN_1_DESC</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_ALIEN_2_DESC</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_ALIEN_3_DESC</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_ALIEN_4_DESC</t>
+  </si>
+  <si>
+    <t>aliendragon_default</t>
+  </si>
+  <si>
+    <t>aliendragon_skin_1</t>
+  </si>
+  <si>
+    <t>aliendragon_skin_2</t>
+  </si>
+  <si>
+    <t>aliendragon_skin_3</t>
+  </si>
+  <si>
+    <t>aliendragon_skin_4</t>
   </si>
 </sst>
 </file>
@@ -2578,8 +2656,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="disguisesDefinitions6" displayName="disguisesDefinitions6" ref="B4:T62" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19">
-  <autoFilter ref="B4:T62"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="disguisesDefinitions6" displayName="disguisesDefinitions6" ref="B4:T67" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19">
+  <autoFilter ref="B4:T67"/>
   <sortState ref="B5:T46">
     <sortCondition ref="T4:T46"/>
   </sortState>
@@ -2874,10 +2952,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="B1:T62"/>
+  <dimension ref="B1:T67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R19" sqref="R19"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="R69" sqref="R69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5858,7 +5936,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="62" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="31" t="s">
         <v>3</v>
       </c>
@@ -5868,7 +5946,7 @@
       <c r="D62" s="32" t="s">
         <v>234</v>
       </c>
-      <c r="E62" s="47" t="s">
+      <c r="E62" s="55" t="s">
         <v>246</v>
       </c>
       <c r="F62" s="34">
@@ -5880,10 +5958,10 @@
       <c r="H62" s="35">
         <v>45</v>
       </c>
-      <c r="I62" s="48">
+      <c r="I62" s="42">
         <v>10</v>
       </c>
-      <c r="J62" s="48"/>
+      <c r="J62" s="42"/>
       <c r="K62" s="28" t="s">
         <v>247</v>
       </c>
@@ -5907,6 +5985,241 @@
       </c>
       <c r="T62" s="23">
         <v>58</v>
+      </c>
+    </row>
+    <row r="63" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B63" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C63" s="15" t="s">
+        <v>398</v>
+      </c>
+      <c r="D63" s="15" t="s">
+        <v>403</v>
+      </c>
+      <c r="E63" s="47"/>
+      <c r="F63" s="17">
+        <v>0</v>
+      </c>
+      <c r="G63" s="18">
+        <v>0</v>
+      </c>
+      <c r="H63" s="18">
+        <v>0</v>
+      </c>
+      <c r="I63" s="48">
+        <v>0</v>
+      </c>
+      <c r="J63" s="48"/>
+      <c r="K63" s="19" t="s">
+        <v>404</v>
+      </c>
+      <c r="L63" s="19" t="s">
+        <v>398</v>
+      </c>
+      <c r="M63" s="19"/>
+      <c r="N63" s="19"/>
+      <c r="O63" s="20"/>
+      <c r="P63" s="20"/>
+      <c r="Q63" s="21" t="s">
+        <v>409</v>
+      </c>
+      <c r="R63" s="22" t="s">
+        <v>414</v>
+      </c>
+      <c r="S63" s="22" t="s">
+        <v>419</v>
+      </c>
+      <c r="T63" s="23">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="64" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B64" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C64" s="32" t="s">
+        <v>399</v>
+      </c>
+      <c r="D64" s="32" t="s">
+        <v>403</v>
+      </c>
+      <c r="E64" s="49"/>
+      <c r="F64" s="34">
+        <v>1</v>
+      </c>
+      <c r="G64" s="35">
+        <v>350000</v>
+      </c>
+      <c r="H64" s="35">
+        <v>0</v>
+      </c>
+      <c r="I64" s="50">
+        <v>1</v>
+      </c>
+      <c r="J64" s="35"/>
+      <c r="K64" s="36" t="s">
+        <v>405</v>
+      </c>
+      <c r="L64" s="36" t="s">
+        <v>399</v>
+      </c>
+      <c r="M64" s="36"/>
+      <c r="N64" s="36"/>
+      <c r="O64" s="28"/>
+      <c r="P64" s="28"/>
+      <c r="Q64" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="R64" s="38" t="s">
+        <v>415</v>
+      </c>
+      <c r="S64" s="38" t="s">
+        <v>420</v>
+      </c>
+      <c r="T64" s="23">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B65" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C65" s="32" t="s">
+        <v>400</v>
+      </c>
+      <c r="D65" s="32" t="s">
+        <v>403</v>
+      </c>
+      <c r="E65" s="51"/>
+      <c r="F65" s="34">
+        <v>2</v>
+      </c>
+      <c r="G65" s="35">
+        <v>350000</v>
+      </c>
+      <c r="H65" s="35">
+        <v>0</v>
+      </c>
+      <c r="I65" s="35">
+        <v>4</v>
+      </c>
+      <c r="J65" s="35"/>
+      <c r="K65" s="36" t="s">
+        <v>406</v>
+      </c>
+      <c r="L65" s="36" t="s">
+        <v>400</v>
+      </c>
+      <c r="M65" s="36"/>
+      <c r="N65" s="36"/>
+      <c r="O65" s="28"/>
+      <c r="P65" s="28"/>
+      <c r="Q65" s="37" t="s">
+        <v>411</v>
+      </c>
+      <c r="R65" s="38" t="s">
+        <v>416</v>
+      </c>
+      <c r="S65" s="38" t="s">
+        <v>421</v>
+      </c>
+      <c r="T65" s="23">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="66" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B66" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C66" s="32" t="s">
+        <v>401</v>
+      </c>
+      <c r="D66" s="32" t="s">
+        <v>403</v>
+      </c>
+      <c r="E66" s="51"/>
+      <c r="F66" s="34">
+        <v>3</v>
+      </c>
+      <c r="G66" s="35">
+        <v>350000</v>
+      </c>
+      <c r="H66" s="35">
+        <v>0</v>
+      </c>
+      <c r="I66" s="27">
+        <v>7</v>
+      </c>
+      <c r="J66" s="27"/>
+      <c r="K66" s="28" t="s">
+        <v>407</v>
+      </c>
+      <c r="L66" s="28" t="s">
+        <v>401</v>
+      </c>
+      <c r="M66" s="28"/>
+      <c r="N66" s="28"/>
+      <c r="O66" s="28"/>
+      <c r="P66" s="28"/>
+      <c r="Q66" s="37" t="s">
+        <v>412</v>
+      </c>
+      <c r="R66" s="38" t="s">
+        <v>417</v>
+      </c>
+      <c r="S66" s="38" t="s">
+        <v>422</v>
+      </c>
+      <c r="T66" s="23">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="67" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B67" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C67" s="32" t="s">
+        <v>402</v>
+      </c>
+      <c r="D67" s="32" t="s">
+        <v>403</v>
+      </c>
+      <c r="E67" s="47"/>
+      <c r="F67" s="34">
+        <v>4</v>
+      </c>
+      <c r="G67" s="35">
+        <v>0</v>
+      </c>
+      <c r="H67" s="35">
+        <v>45</v>
+      </c>
+      <c r="I67" s="48">
+        <v>10</v>
+      </c>
+      <c r="J67" s="48"/>
+      <c r="K67" s="28" t="s">
+        <v>408</v>
+      </c>
+      <c r="L67" s="28" t="s">
+        <v>402</v>
+      </c>
+      <c r="M67" s="28"/>
+      <c r="N67" s="28"/>
+      <c r="O67" s="28"/>
+      <c r="P67" s="28"/>
+      <c r="Q67" s="37" t="s">
+        <v>413</v>
+      </c>
+      <c r="R67" s="38" t="s">
+        <v>418</v>
+      </c>
+      <c r="S67" s="38" t="s">
+        <v>423</v>
+      </c>
+      <c r="T67" s="23">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed power ups, as last alien disguise is just for xmas, a season one
Former-commit-id: e68c2cae726694ba59e1a142753a06d1beb33db3
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="427">
   <si>
     <t>[sku]</t>
   </si>
@@ -1296,6 +1296,15 @@
   </si>
   <si>
     <t>aliendragon_skin_4</t>
+  </si>
+  <si>
+    <t>xmas</t>
+  </si>
+  <si>
+    <t>disguise_dive_coins</t>
+  </si>
+  <si>
+    <t>disguise_dive</t>
   </si>
 </sst>
 </file>
@@ -2954,8 +2963,8 @@
   </sheetPr>
   <dimension ref="B1:T67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G75" sqref="G75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6094,7 +6103,7 @@
         <v>403</v>
       </c>
       <c r="E65" s="51" t="s">
-        <v>240</v>
+        <v>426</v>
       </c>
       <c r="F65" s="34">
         <v>2</v>
@@ -6143,16 +6152,16 @@
         <v>403</v>
       </c>
       <c r="E66" s="51" t="s">
-        <v>265</v>
+        <v>425</v>
       </c>
       <c r="F66" s="34">
         <v>3</v>
       </c>
       <c r="G66" s="35">
-        <v>350000</v>
+        <v>0</v>
       </c>
       <c r="H66" s="35">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="I66" s="27">
         <v>7</v>
@@ -6201,12 +6210,14 @@
         <v>0</v>
       </c>
       <c r="H67" s="35">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="I67" s="48">
-        <v>10</v>
-      </c>
-      <c r="J67" s="48"/>
+        <v>0</v>
+      </c>
+      <c r="J67" s="27" t="s">
+        <v>424</v>
+      </c>
       <c r="K67" s="28" t="s">
         <v>408</v>
       </c>

</xml_diff>

<commit_message>
Some disguises parts and texts
Former-commit-id: e6c40968b41f92cb1cdd84301f724a230301de11
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="430">
   <si>
     <t>[sku]</t>
   </si>
@@ -1305,6 +1305,15 @@
   </si>
   <si>
     <t>disguise_dive</t>
+  </si>
+  <si>
+    <t>PF_F_Breather;PF_F_Helmet;PF_F_Shoulder_L;PF_F_Shoulder_R</t>
+  </si>
+  <si>
+    <t>PF_GR_Arm_L;PF_GR_Arm_R;PF_GR_Ears;PF_GR_Eyes;PF_GR_Leg_L;PF_GR_Leg_R;PF_GR_Shoulder_L;PF_GR_Shoulder_R</t>
+  </si>
+  <si>
+    <t>PF_GRI_Feet_L;PF_GRI_Feet_R;PF_GRI_Hat;PF_GRI_Waist</t>
   </si>
 </sst>
 </file>
@@ -2964,7 +2973,7 @@
   <dimension ref="B1:T67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G75" sqref="G75"/>
+      <selection activeCell="O69" sqref="O69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6077,7 +6086,9 @@
       </c>
       <c r="M64" s="36"/>
       <c r="N64" s="36"/>
-      <c r="O64" s="28"/>
+      <c r="O64" s="28" t="s">
+        <v>427</v>
+      </c>
       <c r="P64" s="28"/>
       <c r="Q64" s="37" t="s">
         <v>410</v>
@@ -6126,7 +6137,9 @@
       </c>
       <c r="M65" s="36"/>
       <c r="N65" s="36"/>
-      <c r="O65" s="28"/>
+      <c r="O65" s="28" t="s">
+        <v>428</v>
+      </c>
       <c r="P65" s="28"/>
       <c r="Q65" s="37" t="s">
         <v>411</v>
@@ -6226,7 +6239,9 @@
       </c>
       <c r="M67" s="28"/>
       <c r="N67" s="28"/>
-      <c r="O67" s="28"/>
+      <c r="O67" s="28" t="s">
+        <v>429</v>
+      </c>
       <c r="P67" s="28"/>
       <c r="Q67" s="37" t="s">
         <v>413</v>

</xml_diff>

<commit_message>
Adding disguise 3, parts
Former-commit-id: f2ee722bc78748d6921766228c6b4a9e6b5beead
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="431">
   <si>
     <t>[sku]</t>
   </si>
@@ -1314,6 +1314,9 @@
   </si>
   <si>
     <t>PF_GRI_Feet_L;PF_GRI_Feet_R;PF_GRI_Hat;PF_GRI_Waist</t>
+  </si>
+  <si>
+    <t>PF_PR_Arm_L;PF_PR_Arm_R;PF_PR_Head;PF_PR_Shoulder_L;PF_PR_Shoulder_R;PF_PR_Tail_L;PF_PR_Tail_R;PF_PR_Waist</t>
   </si>
 </sst>
 </file>
@@ -2972,8 +2975,8 @@
   </sheetPr>
   <dimension ref="B1:T67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H70" sqref="H70"/>
+    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="O67" sqref="O67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6188,7 +6191,9 @@
       </c>
       <c r="M66" s="28"/>
       <c r="N66" s="28"/>
-      <c r="O66" s="28"/>
+      <c r="O66" s="28" t="s">
+        <v>430</v>
+      </c>
       <c r="P66" s="28"/>
       <c r="Q66" s="37" t="s">
         <v>412</v>

</xml_diff>

<commit_message>
LNY Skins added in content for Blaze and Umbra
Former-commit-id: 2395cf4a57497e6c26fb11a9b40779fafa396746
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="443">
   <si>
     <t>[sku]</t>
   </si>
@@ -836,9 +836,6 @@
     <t>darkdragon_skin_3</t>
   </si>
   <si>
-    <t>darkdragon_skin_4</t>
-  </si>
-  <si>
     <t>FX_PF_DarkDragon_Skin00_FlamesHead;FX_PF_DarkDragon_Skin00_FlamesNeck;FX_PF_DarkDragon_Skin00_FlamesSpine;FX_PF_DarkDragon_Skin00_Wings_Left;FX_PF_DarkDragon_Skin00_Wings_Right</t>
   </si>
   <si>
@@ -1317,6 +1314,45 @@
   </si>
   <si>
     <t>PF_PR_Arm_L;PF_PR_Arm_R;PF_PR_Head;PF_PR_Shoulder_L;PF_PR_Shoulder_R;PF_PR_Tail_L;PF_PR_Tail_R;PF_PR_Waist</t>
+  </si>
+  <si>
+    <t>dragon_classic_6</t>
+  </si>
+  <si>
+    <t>free_revive</t>
+  </si>
+  <si>
+    <t>icon_classic_6</t>
+  </si>
+  <si>
+    <t>chineseNewYear</t>
+  </si>
+  <si>
+    <t>classic_chineseNewYear</t>
+  </si>
+  <si>
+    <t>TID_SKIN_LNY_CLASSIC_NAME</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_CLASSIC_6_DESC</t>
+  </si>
+  <si>
+    <t>dragon_dark_5</t>
+  </si>
+  <si>
+    <t>transform_gold</t>
+  </si>
+  <si>
+    <t>icon_dark_5</t>
+  </si>
+  <si>
+    <t>TID_SKIN_LNY_DARK_NAME</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_DARK_5_DESC</t>
+  </si>
+  <si>
+    <t>darkdragon_skin_chineseNewYear</t>
   </si>
 </sst>
 </file>
@@ -1456,7 +1492,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1708,11 +1744,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
@@ -1888,6 +1954,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2677,8 +2752,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="disguisesDefinitions6" displayName="disguisesDefinitions6" ref="B4:T67" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19">
-  <autoFilter ref="B4:T67"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="disguisesDefinitions6" displayName="disguisesDefinitions6" ref="B4:T69" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19">
+  <autoFilter ref="B4:T69"/>
   <sortState ref="B5:T46">
     <sortCondition ref="T4:T46"/>
   </sortState>
@@ -2973,10 +3048,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="B1:T67"/>
+  <dimension ref="B1:T69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
-      <selection activeCell="O67" sqref="O67"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2988,13 +3063,13 @@
     <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
     <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="73" customWidth="1"/>
     <col min="16" max="16" width="29" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="38.7109375" customWidth="1"/>
     <col min="18" max="18" width="37.85546875" customWidth="1"/>
     <col min="19" max="19" width="38.7109375" customWidth="1"/>
   </cols>
@@ -3065,7 +3140,7 @@
         <v>22</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K4" s="11" t="s">
         <v>1</v>
@@ -3133,10 +3208,10 @@
       <c r="O5" s="20"/>
       <c r="P5" s="20"/>
       <c r="Q5" s="21" t="s">
+        <v>294</v>
+      </c>
+      <c r="R5" s="22" t="s">
         <v>295</v>
-      </c>
-      <c r="R5" s="22" t="s">
-        <v>296</v>
       </c>
       <c r="S5" s="22" t="s">
         <v>30</v>
@@ -3184,10 +3259,10 @@
       </c>
       <c r="P6" s="28"/>
       <c r="Q6" s="29" t="s">
+        <v>296</v>
+      </c>
+      <c r="R6" s="30" t="s">
         <v>297</v>
-      </c>
-      <c r="R6" s="30" t="s">
-        <v>298</v>
       </c>
       <c r="S6" s="30" t="s">
         <v>33</v>
@@ -3231,10 +3306,10 @@
       <c r="O7" s="20"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="21" t="s">
+        <v>298</v>
+      </c>
+      <c r="R7" s="22" t="s">
         <v>299</v>
-      </c>
-      <c r="R7" s="22" t="s">
-        <v>300</v>
       </c>
       <c r="S7" s="22" t="s">
         <v>35</v>
@@ -3282,10 +3357,10 @@
       </c>
       <c r="P8" s="58"/>
       <c r="Q8" s="37" t="s">
+        <v>300</v>
+      </c>
+      <c r="R8" s="38" t="s">
         <v>301</v>
-      </c>
-      <c r="R8" s="38" t="s">
-        <v>302</v>
       </c>
       <c r="S8" s="38" t="s">
         <v>38</v>
@@ -3333,10 +3408,10 @@
       </c>
       <c r="P9" s="43"/>
       <c r="Q9" s="29" t="s">
+        <v>302</v>
+      </c>
+      <c r="R9" s="30" t="s">
         <v>303</v>
-      </c>
-      <c r="R9" s="30" t="s">
-        <v>304</v>
       </c>
       <c r="S9" s="30" t="s">
         <v>41</v>
@@ -3380,10 +3455,10 @@
       <c r="O10" s="28"/>
       <c r="P10" s="28"/>
       <c r="Q10" s="21" t="s">
+        <v>304</v>
+      </c>
+      <c r="R10" s="22" t="s">
         <v>305</v>
-      </c>
-      <c r="R10" s="22" t="s">
-        <v>306</v>
       </c>
       <c r="S10" s="22" t="s">
         <v>43</v>
@@ -3431,10 +3506,10 @@
       </c>
       <c r="P11" s="28"/>
       <c r="Q11" s="37" t="s">
+        <v>306</v>
+      </c>
+      <c r="R11" s="38" t="s">
         <v>307</v>
-      </c>
-      <c r="R11" s="38" t="s">
-        <v>308</v>
       </c>
       <c r="S11" s="38" t="s">
         <v>46</v>
@@ -3480,10 +3555,10 @@
       </c>
       <c r="P12" s="43"/>
       <c r="Q12" s="44" t="s">
+        <v>308</v>
+      </c>
+      <c r="R12" s="45" t="s">
         <v>309</v>
-      </c>
-      <c r="R12" s="45" t="s">
-        <v>310</v>
       </c>
       <c r="S12" s="45" t="s">
         <v>49</v>
@@ -3527,10 +3602,10 @@
       <c r="O13" s="28"/>
       <c r="P13" s="28"/>
       <c r="Q13" s="37" t="s">
+        <v>310</v>
+      </c>
+      <c r="R13" s="38" t="s">
         <v>311</v>
-      </c>
-      <c r="R13" s="38" t="s">
-        <v>312</v>
       </c>
       <c r="S13" s="38" t="s">
         <v>51</v>
@@ -3578,10 +3653,10 @@
       </c>
       <c r="P14" s="28"/>
       <c r="Q14" s="37" t="s">
+        <v>312</v>
+      </c>
+      <c r="R14" s="38" t="s">
         <v>313</v>
-      </c>
-      <c r="R14" s="38" t="s">
-        <v>314</v>
       </c>
       <c r="S14" s="38" t="s">
         <v>53</v>
@@ -3629,10 +3704,10 @@
       </c>
       <c r="P15" s="28"/>
       <c r="Q15" s="59" t="s">
+        <v>314</v>
+      </c>
+      <c r="R15" s="59" t="s">
         <v>315</v>
-      </c>
-      <c r="R15" s="59" t="s">
-        <v>316</v>
       </c>
       <c r="S15" s="59" t="s">
         <v>56</v>
@@ -3680,10 +3755,10 @@
       </c>
       <c r="P16" s="28"/>
       <c r="Q16" s="29" t="s">
+        <v>316</v>
+      </c>
+      <c r="R16" s="30" t="s">
         <v>317</v>
-      </c>
-      <c r="R16" s="30" t="s">
-        <v>318</v>
       </c>
       <c r="S16" s="30" t="s">
         <v>59</v>
@@ -3727,10 +3802,10 @@
       <c r="O17" s="20"/>
       <c r="P17" s="20"/>
       <c r="Q17" s="21" t="s">
+        <v>318</v>
+      </c>
+      <c r="R17" s="22" t="s">
         <v>319</v>
-      </c>
-      <c r="R17" s="22" t="s">
-        <v>320</v>
       </c>
       <c r="S17" s="22" t="s">
         <v>61</v>
@@ -3778,10 +3853,10 @@
       </c>
       <c r="P18" s="28"/>
       <c r="Q18" s="37" t="s">
+        <v>320</v>
+      </c>
+      <c r="R18" s="38" t="s">
         <v>321</v>
-      </c>
-      <c r="R18" s="38" t="s">
-        <v>322</v>
       </c>
       <c r="S18" s="38" t="s">
         <v>65</v>
@@ -3829,10 +3904,10 @@
       </c>
       <c r="P19" s="28"/>
       <c r="Q19" s="37" t="s">
+        <v>322</v>
+      </c>
+      <c r="R19" s="38" t="s">
         <v>323</v>
-      </c>
-      <c r="R19" s="38" t="s">
-        <v>324</v>
       </c>
       <c r="S19" s="38" t="s">
         <v>67</v>
@@ -3880,10 +3955,10 @@
       </c>
       <c r="P20" s="28"/>
       <c r="Q20" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="R20" s="30" t="s">
         <v>325</v>
-      </c>
-      <c r="R20" s="30" t="s">
-        <v>326</v>
       </c>
       <c r="S20" s="30" t="s">
         <v>70</v>
@@ -3929,10 +4004,10 @@
       </c>
       <c r="P21" s="20"/>
       <c r="Q21" s="21" t="s">
+        <v>326</v>
+      </c>
+      <c r="R21" s="22" t="s">
         <v>327</v>
-      </c>
-      <c r="R21" s="22" t="s">
-        <v>328</v>
       </c>
       <c r="S21" s="22" t="s">
         <v>73</v>
@@ -3980,10 +4055,10 @@
       </c>
       <c r="P22" s="28"/>
       <c r="Q22" s="37" t="s">
+        <v>328</v>
+      </c>
+      <c r="R22" s="38" t="s">
         <v>329</v>
-      </c>
-      <c r="R22" s="38" t="s">
-        <v>330</v>
       </c>
       <c r="S22" s="38" t="s">
         <v>76</v>
@@ -4031,10 +4106,10 @@
       </c>
       <c r="P23" s="28"/>
       <c r="Q23" s="37" t="s">
+        <v>330</v>
+      </c>
+      <c r="R23" s="38" t="s">
         <v>331</v>
-      </c>
-      <c r="R23" s="38" t="s">
-        <v>332</v>
       </c>
       <c r="S23" s="38" t="s">
         <v>79</v>
@@ -4082,10 +4157,10 @@
       </c>
       <c r="P24" s="28"/>
       <c r="Q24" s="29" t="s">
+        <v>332</v>
+      </c>
+      <c r="R24" s="30" t="s">
         <v>333</v>
-      </c>
-      <c r="R24" s="30" t="s">
-        <v>334</v>
       </c>
       <c r="S24" s="30" t="s">
         <v>82</v>
@@ -4129,10 +4204,10 @@
       <c r="O25" s="20"/>
       <c r="P25" s="20"/>
       <c r="Q25" s="21" t="s">
+        <v>334</v>
+      </c>
+      <c r="R25" s="22" t="s">
         <v>335</v>
-      </c>
-      <c r="R25" s="22" t="s">
-        <v>336</v>
       </c>
       <c r="S25" s="22" t="s">
         <v>84</v>
@@ -4180,10 +4255,10 @@
       </c>
       <c r="P26" s="28"/>
       <c r="Q26" s="37" t="s">
+        <v>336</v>
+      </c>
+      <c r="R26" s="38" t="s">
         <v>337</v>
-      </c>
-      <c r="R26" s="38" t="s">
-        <v>338</v>
       </c>
       <c r="S26" s="38" t="s">
         <v>87</v>
@@ -4231,10 +4306,10 @@
       </c>
       <c r="P27" s="28"/>
       <c r="Q27" s="37" t="s">
+        <v>338</v>
+      </c>
+      <c r="R27" s="38" t="s">
         <v>339</v>
-      </c>
-      <c r="R27" s="38" t="s">
-        <v>340</v>
       </c>
       <c r="S27" s="38" t="s">
         <v>90</v>
@@ -4282,10 +4357,10 @@
       </c>
       <c r="P28" s="28"/>
       <c r="Q28" s="37" t="s">
+        <v>340</v>
+      </c>
+      <c r="R28" s="38" t="s">
         <v>341</v>
-      </c>
-      <c r="R28" s="38" t="s">
-        <v>342</v>
       </c>
       <c r="S28" s="38" t="s">
         <v>93</v>
@@ -4333,10 +4408,10 @@
       </c>
       <c r="P29" s="28"/>
       <c r="Q29" s="59" t="s">
+        <v>342</v>
+      </c>
+      <c r="R29" s="59" t="s">
         <v>343</v>
-      </c>
-      <c r="R29" s="59" t="s">
-        <v>344</v>
       </c>
       <c r="S29" s="59" t="s">
         <v>96</v>
@@ -4345,18 +4420,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="2:20" s="46" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B30" s="24" t="s">
         <v>3</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D30" s="23" t="s">
         <v>11</v>
       </c>
       <c r="E30" s="51" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F30" s="26">
         <v>5</v>
@@ -4372,125 +4447,123 @@
         <v>181</v>
       </c>
       <c r="K30" s="28" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L30" s="28" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="M30" s="28"/>
       <c r="N30" s="28"/>
       <c r="O30" s="28" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="P30" s="28"/>
       <c r="Q30" s="29" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="R30" s="30" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="S30" s="30" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="T30" s="23">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B31" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31" s="16"/>
-      <c r="F31" s="17">
-        <v>0</v>
-      </c>
-      <c r="G31" s="18">
-        <v>0</v>
-      </c>
-      <c r="H31" s="18">
-        <v>0</v>
-      </c>
-      <c r="I31" s="18">
-        <v>0</v>
-      </c>
-      <c r="J31" s="18"/>
-      <c r="K31" s="19" t="s">
-        <v>208</v>
-      </c>
-      <c r="L31" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="M31" s="19"/>
-      <c r="N31" s="19"/>
-      <c r="O31" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="P31" s="20"/>
-      <c r="Q31" s="21" t="s">
-        <v>346</v>
-      </c>
-      <c r="R31" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="S31" s="22" t="s">
-        <v>99</v>
+    <row r="31" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>430</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="61" t="s">
+        <v>431</v>
+      </c>
+      <c r="F31" s="26">
+        <v>6</v>
+      </c>
+      <c r="G31" s="27">
+        <v>0</v>
+      </c>
+      <c r="H31" s="27">
+        <v>65</v>
+      </c>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27" t="s">
+        <v>433</v>
+      </c>
+      <c r="K31" s="28" t="s">
+        <v>432</v>
+      </c>
+      <c r="L31" s="28" t="s">
+        <v>430</v>
+      </c>
+      <c r="M31" s="28"/>
+      <c r="N31" s="28"/>
+      <c r="O31" s="28"/>
+      <c r="P31" s="28"/>
+      <c r="Q31" s="29" t="s">
+        <v>435</v>
+      </c>
+      <c r="R31" s="30" t="s">
+        <v>436</v>
+      </c>
+      <c r="S31" s="30" t="s">
+        <v>434</v>
       </c>
       <c r="T31" s="23">
         <v>27</v>
       </c>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B32" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="C32" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="D32" s="32" t="s">
+      <c r="B32" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D32" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E32" s="52" t="s">
-        <v>248</v>
-      </c>
-      <c r="F32" s="34">
-        <v>1</v>
-      </c>
-      <c r="G32" s="35">
-        <v>80000</v>
-      </c>
-      <c r="H32" s="35">
-        <v>0</v>
-      </c>
-      <c r="I32" s="35">
-        <v>1</v>
-      </c>
-      <c r="J32" s="35"/>
-      <c r="K32" s="36" t="s">
-        <v>209</v>
-      </c>
-      <c r="L32" s="36" t="s">
-        <v>100</v>
-      </c>
-      <c r="M32" s="36"/>
-      <c r="N32" s="36"/>
-      <c r="O32" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="P32" s="28"/>
-      <c r="Q32" s="37" t="s">
-        <v>348</v>
-      </c>
-      <c r="R32" s="38" t="s">
-        <v>349</v>
-      </c>
-      <c r="S32" s="38" t="s">
-        <v>102</v>
+      <c r="E32" s="16"/>
+      <c r="F32" s="17">
+        <v>0</v>
+      </c>
+      <c r="G32" s="18">
+        <v>0</v>
+      </c>
+      <c r="H32" s="18">
+        <v>0</v>
+      </c>
+      <c r="I32" s="18">
+        <v>0</v>
+      </c>
+      <c r="J32" s="18"/>
+      <c r="K32" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="L32" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="P32" s="20"/>
+      <c r="Q32" s="21" t="s">
+        <v>345</v>
+      </c>
+      <c r="R32" s="22" t="s">
+        <v>346</v>
+      </c>
+      <c r="S32" s="22" t="s">
+        <v>99</v>
       </c>
       <c r="T32" s="23">
         <v>28</v>
@@ -4501,16 +4574,16 @@
         <v>3</v>
       </c>
       <c r="C33" s="32" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D33" s="32" t="s">
         <v>12</v>
       </c>
       <c r="E33" s="52" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="F33" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G33" s="35">
         <v>80000</v>
@@ -4519,29 +4592,29 @@
         <v>0</v>
       </c>
       <c r="I33" s="35">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J33" s="35"/>
       <c r="K33" s="36" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="L33" s="36" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="M33" s="36"/>
       <c r="N33" s="36"/>
       <c r="O33" s="28" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="P33" s="28"/>
       <c r="Q33" s="37" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="R33" s="38" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="S33" s="38" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="T33" s="23">
         <v>29</v>
@@ -4552,16 +4625,16 @@
         <v>3</v>
       </c>
       <c r="C34" s="32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D34" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E34" s="51" t="s">
-        <v>259</v>
+      <c r="E34" s="52" t="s">
+        <v>257</v>
       </c>
       <c r="F34" s="34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G34" s="35">
         <v>80000</v>
@@ -4570,127 +4643,131 @@
         <v>0</v>
       </c>
       <c r="I34" s="35">
-        <v>7</v>
-      </c>
-      <c r="J34" s="27"/>
-      <c r="K34" s="28" t="s">
-        <v>211</v>
-      </c>
-      <c r="L34" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="M34" s="28"/>
-      <c r="N34" s="28"/>
+        <v>4</v>
+      </c>
+      <c r="J34" s="35"/>
+      <c r="K34" s="36" t="s">
+        <v>210</v>
+      </c>
+      <c r="L34" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="M34" s="36"/>
+      <c r="N34" s="36"/>
       <c r="O34" s="28" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="P34" s="28"/>
       <c r="Q34" s="37" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="R34" s="38" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="S34" s="38" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="T34" s="23">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="C35" s="40" t="s">
-        <v>109</v>
-      </c>
-      <c r="D35" s="40" t="s">
+    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B35" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="D35" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E35" s="55" t="s">
-        <v>260</v>
-      </c>
-      <c r="F35" s="41">
-        <v>4</v>
-      </c>
-      <c r="G35" s="42">
-        <v>0</v>
-      </c>
-      <c r="H35" s="42">
-        <v>45</v>
-      </c>
-      <c r="I35" s="42">
-        <v>10</v>
-      </c>
-      <c r="J35" s="42"/>
-      <c r="K35" s="43" t="s">
-        <v>212</v>
-      </c>
-      <c r="L35" s="43" t="s">
-        <v>109</v>
-      </c>
-      <c r="M35" s="43"/>
-      <c r="N35" s="43"/>
-      <c r="O35" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="P35" s="43"/>
-      <c r="Q35" s="44" t="s">
-        <v>354</v>
-      </c>
-      <c r="R35" s="45" t="s">
-        <v>355</v>
-      </c>
-      <c r="S35" s="45" t="s">
-        <v>111</v>
+      <c r="E35" s="51" t="s">
+        <v>259</v>
+      </c>
+      <c r="F35" s="34">
+        <v>3</v>
+      </c>
+      <c r="G35" s="35">
+        <v>80000</v>
+      </c>
+      <c r="H35" s="35">
+        <v>0</v>
+      </c>
+      <c r="I35" s="35">
+        <v>7</v>
+      </c>
+      <c r="J35" s="27"/>
+      <c r="K35" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="L35" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="M35" s="28"/>
+      <c r="N35" s="28"/>
+      <c r="O35" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="P35" s="28"/>
+      <c r="Q35" s="37" t="s">
+        <v>351</v>
+      </c>
+      <c r="R35" s="38" t="s">
+        <v>352</v>
+      </c>
+      <c r="S35" s="38" t="s">
+        <v>108</v>
       </c>
       <c r="T35" s="23">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B36" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C36" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="D36" s="23" t="s">
-        <v>141</v>
-      </c>
-      <c r="E36" s="25"/>
-      <c r="F36" s="26">
-        <v>0</v>
-      </c>
-      <c r="G36" s="27">
-        <v>0</v>
-      </c>
-      <c r="H36" s="27">
-        <v>0</v>
-      </c>
-      <c r="I36" s="27">
-        <v>0</v>
-      </c>
-      <c r="J36" s="27"/>
-      <c r="K36" s="28" t="s">
-        <v>213</v>
-      </c>
-      <c r="L36" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="M36" s="28"/>
-      <c r="N36" s="28"/>
-      <c r="O36" s="28"/>
-      <c r="P36" s="28"/>
-      <c r="Q36" s="29" t="s">
-        <v>142</v>
-      </c>
-      <c r="R36" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="S36" s="30" t="s">
-        <v>152</v>
+    <row r="36" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="40" t="s">
+        <v>109</v>
+      </c>
+      <c r="D36" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="55" t="s">
+        <v>260</v>
+      </c>
+      <c r="F36" s="41">
+        <v>4</v>
+      </c>
+      <c r="G36" s="42">
+        <v>0</v>
+      </c>
+      <c r="H36" s="42">
+        <v>45</v>
+      </c>
+      <c r="I36" s="42">
+        <v>10</v>
+      </c>
+      <c r="J36" s="42"/>
+      <c r="K36" s="43" t="s">
+        <v>212</v>
+      </c>
+      <c r="L36" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="M36" s="43"/>
+      <c r="N36" s="43"/>
+      <c r="O36" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="P36" s="43"/>
+      <c r="Q36" s="44" t="s">
+        <v>353</v>
+      </c>
+      <c r="R36" s="45" t="s">
+        <v>354</v>
+      </c>
+      <c r="S36" s="45" t="s">
+        <v>111</v>
       </c>
       <c r="T36" s="23">
         <v>32</v>
@@ -4701,47 +4778,43 @@
         <v>3</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D37" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="E37" s="51" t="s">
-        <v>253</v>
-      </c>
+      <c r="E37" s="25"/>
       <c r="F37" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G37" s="27">
-        <v>85000</v>
+        <v>0</v>
       </c>
       <c r="H37" s="27">
         <v>0</v>
       </c>
       <c r="I37" s="27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J37" s="27"/>
       <c r="K37" s="28" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="L37" s="28" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M37" s="28"/>
       <c r="N37" s="28"/>
-      <c r="O37" s="28" t="s">
-        <v>157</v>
-      </c>
+      <c r="O37" s="28"/>
       <c r="P37" s="28"/>
-      <c r="Q37" s="59" t="s">
-        <v>144</v>
-      </c>
-      <c r="R37" s="59" t="s">
-        <v>145</v>
-      </c>
-      <c r="S37" s="59" t="s">
-        <v>153</v>
+      <c r="Q37" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="R37" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="S37" s="30" t="s">
+        <v>152</v>
       </c>
       <c r="T37" s="23">
         <v>33</v>
@@ -4752,16 +4825,16 @@
         <v>3</v>
       </c>
       <c r="C38" s="23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D38" s="23" t="s">
         <v>141</v>
       </c>
       <c r="E38" s="51" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F38" s="26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G38" s="27">
         <v>85000</v>
@@ -4770,29 +4843,29 @@
         <v>0</v>
       </c>
       <c r="I38" s="27">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J38" s="27"/>
       <c r="K38" s="28" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="L38" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M38" s="28"/>
       <c r="N38" s="28"/>
       <c r="O38" s="28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P38" s="28"/>
       <c r="Q38" s="59" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="R38" s="59" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="S38" s="59" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="T38" s="23">
         <v>34</v>
@@ -4803,16 +4876,16 @@
         <v>3</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D39" s="23" t="s">
         <v>141</v>
       </c>
       <c r="E39" s="51" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="F39" s="26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G39" s="27">
         <v>85000</v>
@@ -4821,178 +4894,178 @@
         <v>0</v>
       </c>
       <c r="I39" s="27">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J39" s="27"/>
       <c r="K39" s="28" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L39" s="28" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M39" s="28"/>
       <c r="N39" s="28"/>
       <c r="O39" s="28" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="P39" s="28"/>
       <c r="Q39" s="59" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="R39" s="59" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="S39" s="59" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="T39" s="23">
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B40" s="24" t="s">
         <v>3</v>
       </c>
       <c r="C40" s="23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D40" s="23" t="s">
         <v>141</v>
       </c>
       <c r="E40" s="51" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="F40" s="26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G40" s="27">
-        <v>0</v>
+        <v>85000</v>
       </c>
       <c r="H40" s="27">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="I40" s="27">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="J40" s="27"/>
       <c r="K40" s="28" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L40" s="28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M40" s="28"/>
       <c r="N40" s="28"/>
       <c r="O40" s="28" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="P40" s="28"/>
-      <c r="Q40" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="R40" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="S40" s="30" t="s">
-        <v>156</v>
+      <c r="Q40" s="59" t="s">
+        <v>148</v>
+      </c>
+      <c r="R40" s="59" t="s">
+        <v>149</v>
+      </c>
+      <c r="S40" s="59" t="s">
+        <v>155</v>
       </c>
       <c r="T40" s="23">
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B41" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="D41" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E41" s="16"/>
-      <c r="F41" s="17">
-        <v>0</v>
-      </c>
-      <c r="G41" s="18">
-        <v>0</v>
-      </c>
-      <c r="H41" s="18">
-        <v>0</v>
-      </c>
-      <c r="I41" s="18">
-        <v>0</v>
-      </c>
-      <c r="J41" s="18"/>
-      <c r="K41" s="19" t="s">
-        <v>218</v>
-      </c>
-      <c r="L41" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="M41" s="19"/>
-      <c r="N41" s="19"/>
-      <c r="O41" s="20"/>
-      <c r="P41" s="20"/>
-      <c r="Q41" s="21" t="s">
-        <v>356</v>
-      </c>
-      <c r="R41" s="22" t="s">
-        <v>357</v>
-      </c>
-      <c r="S41" s="22" t="s">
-        <v>113</v>
+    <row r="41" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="D41" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="E41" s="51" t="s">
+        <v>261</v>
+      </c>
+      <c r="F41" s="26">
+        <v>4</v>
+      </c>
+      <c r="G41" s="27">
+        <v>0</v>
+      </c>
+      <c r="H41" s="27">
+        <v>45</v>
+      </c>
+      <c r="I41" s="27">
+        <v>10</v>
+      </c>
+      <c r="J41" s="27"/>
+      <c r="K41" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="L41" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="M41" s="28"/>
+      <c r="N41" s="28"/>
+      <c r="O41" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="P41" s="28"/>
+      <c r="Q41" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="R41" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="S41" s="30" t="s">
+        <v>156</v>
       </c>
       <c r="T41" s="23">
         <v>37</v>
       </c>
     </row>
     <row r="42" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B42" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="C42" s="32" t="s">
-        <v>114</v>
-      </c>
-      <c r="D42" s="32" t="s">
+      <c r="B42" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="D42" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E42" s="52" t="s">
-        <v>237</v>
-      </c>
-      <c r="F42" s="34">
-        <v>1</v>
-      </c>
-      <c r="G42" s="35">
-        <v>95000</v>
-      </c>
-      <c r="H42" s="35">
-        <v>0</v>
-      </c>
-      <c r="I42" s="35">
-        <v>1</v>
-      </c>
-      <c r="J42" s="35"/>
-      <c r="K42" s="36" t="s">
-        <v>219</v>
-      </c>
-      <c r="L42" s="36" t="s">
-        <v>114</v>
-      </c>
-      <c r="M42" s="36"/>
-      <c r="N42" s="36"/>
-      <c r="O42" s="28" t="s">
-        <v>161</v>
-      </c>
-      <c r="P42" s="28"/>
-      <c r="Q42" s="37" t="s">
-        <v>358</v>
-      </c>
-      <c r="R42" s="38" t="s">
-        <v>359</v>
-      </c>
-      <c r="S42" s="38" t="s">
-        <v>115</v>
+      <c r="E42" s="16"/>
+      <c r="F42" s="17">
+        <v>0</v>
+      </c>
+      <c r="G42" s="18">
+        <v>0</v>
+      </c>
+      <c r="H42" s="18">
+        <v>0</v>
+      </c>
+      <c r="I42" s="18">
+        <v>0</v>
+      </c>
+      <c r="J42" s="18"/>
+      <c r="K42" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="L42" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="M42" s="19"/>
+      <c r="N42" s="19"/>
+      <c r="O42" s="20"/>
+      <c r="P42" s="20"/>
+      <c r="Q42" s="21" t="s">
+        <v>355</v>
+      </c>
+      <c r="R42" s="22" t="s">
+        <v>356</v>
+      </c>
+      <c r="S42" s="22" t="s">
+        <v>113</v>
       </c>
       <c r="T42" s="23">
         <v>38</v>
@@ -5003,16 +5076,16 @@
         <v>3</v>
       </c>
       <c r="C43" s="32" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D43" s="32" t="s">
         <v>13</v>
       </c>
       <c r="E43" s="52" t="s">
-        <v>257</v>
+        <v>237</v>
       </c>
       <c r="F43" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G43" s="35">
         <v>95000</v>
@@ -5021,29 +5094,29 @@
         <v>0</v>
       </c>
       <c r="I43" s="35">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J43" s="35"/>
       <c r="K43" s="36" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="L43" s="36" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M43" s="36"/>
       <c r="N43" s="36"/>
       <c r="O43" s="28" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P43" s="28"/>
       <c r="Q43" s="37" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="R43" s="38" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="S43" s="38" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="T43" s="23">
         <v>39</v>
@@ -5054,16 +5127,16 @@
         <v>3</v>
       </c>
       <c r="C44" s="32" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D44" s="32" t="s">
         <v>13</v>
       </c>
       <c r="E44" s="52" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F44" s="34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G44" s="35">
         <v>95000</v>
@@ -5072,31 +5145,29 @@
         <v>0</v>
       </c>
       <c r="I44" s="35">
-        <v>7</v>
-      </c>
-      <c r="J44" s="27"/>
-      <c r="K44" s="28" t="s">
-        <v>221</v>
-      </c>
-      <c r="L44" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="M44" s="28"/>
-      <c r="N44" s="28"/>
+        <v>4</v>
+      </c>
+      <c r="J44" s="35"/>
+      <c r="K44" s="36" t="s">
+        <v>220</v>
+      </c>
+      <c r="L44" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="M44" s="36"/>
+      <c r="N44" s="36"/>
       <c r="O44" s="28" t="s">
-        <v>163</v>
-      </c>
-      <c r="P44" s="28" t="s">
-        <v>165</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="P44" s="28"/>
       <c r="Q44" s="37" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="R44" s="38" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="S44" s="38" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="T44" s="23">
         <v>40</v>
@@ -5107,194 +5178,196 @@
         <v>3</v>
       </c>
       <c r="C45" s="32" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D45" s="32" t="s">
         <v>13</v>
       </c>
       <c r="E45" s="52" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F45" s="34">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G45" s="35">
-        <v>0</v>
+        <v>95000</v>
       </c>
       <c r="H45" s="35">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="I45" s="35">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="J45" s="27"/>
       <c r="K45" s="28" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="L45" s="28" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="M45" s="28"/>
       <c r="N45" s="28"/>
-      <c r="O45" s="28"/>
-      <c r="P45" s="28"/>
+      <c r="O45" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="P45" s="28" t="s">
+        <v>165</v>
+      </c>
       <c r="Q45" s="37" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="R45" s="38" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="S45" s="38" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="T45" s="23">
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="2:20" s="46" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="C46" s="40" t="s">
-        <v>283</v>
-      </c>
-      <c r="D46" s="40" t="s">
+    <row r="46" spans="2:20" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D46" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="E46" s="55" t="s">
-        <v>277</v>
-      </c>
-      <c r="F46" s="41">
-        <v>5</v>
-      </c>
-      <c r="G46" s="42">
-        <v>0</v>
-      </c>
-      <c r="H46" s="42">
-        <v>55</v>
-      </c>
-      <c r="I46" s="42"/>
-      <c r="J46" s="42" t="s">
-        <v>181</v>
-      </c>
-      <c r="K46" s="43" t="s">
-        <v>284</v>
-      </c>
-      <c r="L46" s="43" t="s">
-        <v>283</v>
-      </c>
-      <c r="M46" s="43"/>
-      <c r="N46" s="43"/>
-      <c r="O46" s="43" t="s">
-        <v>291</v>
-      </c>
-      <c r="P46" s="43"/>
-      <c r="Q46" s="29" t="s">
-        <v>293</v>
-      </c>
-      <c r="R46" s="45" t="s">
-        <v>366</v>
-      </c>
-      <c r="S46" s="45" t="s">
-        <v>285</v>
+      <c r="E46" s="52" t="s">
+        <v>262</v>
+      </c>
+      <c r="F46" s="34">
+        <v>4</v>
+      </c>
+      <c r="G46" s="35">
+        <v>0</v>
+      </c>
+      <c r="H46" s="35">
+        <v>45</v>
+      </c>
+      <c r="I46" s="35">
+        <v>10</v>
+      </c>
+      <c r="J46" s="27"/>
+      <c r="K46" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="L46" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="M46" s="28"/>
+      <c r="N46" s="28"/>
+      <c r="O46" s="28"/>
+      <c r="P46" s="28"/>
+      <c r="Q46" s="37" t="s">
+        <v>363</v>
+      </c>
+      <c r="R46" s="38" t="s">
+        <v>364</v>
+      </c>
+      <c r="S46" s="38" t="s">
+        <v>121</v>
       </c>
       <c r="T46" s="23">
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B47" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C47" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="D47" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="E47" s="16"/>
-      <c r="F47" s="17">
-        <v>0</v>
-      </c>
-      <c r="G47" s="18">
-        <v>0</v>
-      </c>
-      <c r="H47" s="18">
-        <v>0</v>
-      </c>
-      <c r="I47" s="18">
-        <v>0</v>
-      </c>
-      <c r="J47" s="18"/>
-      <c r="K47" s="19" t="s">
-        <v>223</v>
-      </c>
-      <c r="L47" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="M47" s="19"/>
-      <c r="N47" s="19"/>
-      <c r="O47" s="20"/>
-      <c r="P47" s="20"/>
-      <c r="Q47" s="21" t="s">
-        <v>367</v>
-      </c>
-      <c r="R47" s="22" t="s">
-        <v>368</v>
-      </c>
-      <c r="S47" s="22" t="s">
-        <v>123</v>
+    <row r="47" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" s="40" t="s">
+        <v>282</v>
+      </c>
+      <c r="D47" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E47" s="55" t="s">
+        <v>276</v>
+      </c>
+      <c r="F47" s="41">
+        <v>5</v>
+      </c>
+      <c r="G47" s="42">
+        <v>0</v>
+      </c>
+      <c r="H47" s="42">
+        <v>55</v>
+      </c>
+      <c r="I47" s="42"/>
+      <c r="J47" s="42" t="s">
+        <v>181</v>
+      </c>
+      <c r="K47" s="43" t="s">
+        <v>283</v>
+      </c>
+      <c r="L47" s="43" t="s">
+        <v>282</v>
+      </c>
+      <c r="M47" s="43"/>
+      <c r="N47" s="43"/>
+      <c r="O47" s="43" t="s">
+        <v>290</v>
+      </c>
+      <c r="P47" s="43"/>
+      <c r="Q47" s="29" t="s">
+        <v>292</v>
+      </c>
+      <c r="R47" s="45" t="s">
+        <v>365</v>
+      </c>
+      <c r="S47" s="45" t="s">
+        <v>284</v>
       </c>
       <c r="T47" s="23">
         <v>43</v>
       </c>
     </row>
     <row r="48" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B48" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="C48" s="32" t="s">
-        <v>124</v>
-      </c>
-      <c r="D48" s="32" t="s">
+      <c r="B48" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="D48" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E48" s="52" t="s">
-        <v>257</v>
-      </c>
-      <c r="F48" s="34">
-        <v>1</v>
-      </c>
-      <c r="G48" s="35">
-        <v>135000</v>
-      </c>
-      <c r="H48" s="35">
-        <v>0</v>
-      </c>
-      <c r="I48" s="35">
-        <v>1</v>
-      </c>
-      <c r="J48" s="35"/>
-      <c r="K48" s="36" t="s">
-        <v>224</v>
-      </c>
-      <c r="L48" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="M48" s="36"/>
-      <c r="N48" s="36"/>
-      <c r="O48" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="P48" s="28"/>
-      <c r="Q48" s="37" t="s">
-        <v>369</v>
-      </c>
-      <c r="R48" s="38" t="s">
-        <v>370</v>
-      </c>
-      <c r="S48" s="38" t="s">
-        <v>127</v>
+      <c r="E48" s="16"/>
+      <c r="F48" s="17">
+        <v>0</v>
+      </c>
+      <c r="G48" s="18">
+        <v>0</v>
+      </c>
+      <c r="H48" s="18">
+        <v>0</v>
+      </c>
+      <c r="I48" s="18">
+        <v>0</v>
+      </c>
+      <c r="J48" s="18"/>
+      <c r="K48" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="L48" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="M48" s="19"/>
+      <c r="N48" s="19"/>
+      <c r="O48" s="20"/>
+      <c r="P48" s="20"/>
+      <c r="Q48" s="21" t="s">
+        <v>366</v>
+      </c>
+      <c r="R48" s="22" t="s">
+        <v>367</v>
+      </c>
+      <c r="S48" s="22" t="s">
+        <v>123</v>
       </c>
       <c r="T48" s="23">
         <v>44</v>
@@ -5305,16 +5378,16 @@
         <v>3</v>
       </c>
       <c r="C49" s="32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D49" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="E49" s="51" t="s">
-        <v>259</v>
+      <c r="E49" s="52" t="s">
+        <v>257</v>
       </c>
       <c r="F49" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G49" s="35">
         <v>135000</v>
@@ -5323,29 +5396,29 @@
         <v>0</v>
       </c>
       <c r="I49" s="35">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J49" s="35"/>
       <c r="K49" s="36" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L49" s="36" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="M49" s="36"/>
       <c r="N49" s="36"/>
       <c r="O49" s="28" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="P49" s="28"/>
       <c r="Q49" s="37" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="R49" s="38" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="S49" s="38" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="T49" s="23">
         <v>45</v>
@@ -5356,16 +5429,16 @@
         <v>3</v>
       </c>
       <c r="C50" s="32" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D50" s="32" t="s">
         <v>14</v>
       </c>
       <c r="E50" s="51" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="F50" s="34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G50" s="35">
         <v>135000</v>
@@ -5374,29 +5447,29 @@
         <v>0</v>
       </c>
       <c r="I50" s="35">
-        <v>7</v>
-      </c>
-      <c r="J50" s="27"/>
-      <c r="K50" s="28" t="s">
-        <v>226</v>
-      </c>
-      <c r="L50" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="M50" s="28"/>
-      <c r="N50" s="28"/>
+        <v>4</v>
+      </c>
+      <c r="J50" s="35"/>
+      <c r="K50" s="36" t="s">
+        <v>225</v>
+      </c>
+      <c r="L50" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="M50" s="36"/>
+      <c r="N50" s="36"/>
       <c r="O50" s="28" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="P50" s="28"/>
       <c r="Q50" s="37" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="R50" s="38" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="S50" s="38" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="T50" s="23">
         <v>46</v>
@@ -5407,196 +5480,196 @@
         <v>3</v>
       </c>
       <c r="C51" s="32" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D51" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="E51" s="52" t="s">
-        <v>263</v>
+      <c r="E51" s="51" t="s">
+        <v>254</v>
       </c>
       <c r="F51" s="34">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G51" s="35">
-        <v>0</v>
+        <v>135000</v>
       </c>
       <c r="H51" s="35">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="I51" s="35">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="J51" s="27"/>
       <c r="K51" s="28" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L51" s="28" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M51" s="28"/>
       <c r="N51" s="28"/>
       <c r="O51" s="28" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P51" s="28"/>
       <c r="Q51" s="37" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="R51" s="38" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="S51" s="38" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="T51" s="23">
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="2:20" s="46" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:20" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="31" t="s">
         <v>3</v>
       </c>
       <c r="C52" s="32" t="s">
-        <v>286</v>
+        <v>133</v>
       </c>
       <c r="D52" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="E52" s="51" t="s">
-        <v>278</v>
+      <c r="E52" s="52" t="s">
+        <v>263</v>
       </c>
       <c r="F52" s="34">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G52" s="35">
         <v>0</v>
       </c>
       <c r="H52" s="35">
-        <v>55</v>
-      </c>
-      <c r="I52" s="35"/>
-      <c r="J52" s="27" t="s">
-        <v>181</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="I52" s="35">
+        <v>10</v>
+      </c>
+      <c r="J52" s="27"/>
       <c r="K52" s="28" t="s">
-        <v>287</v>
+        <v>227</v>
       </c>
       <c r="L52" s="28" t="s">
-        <v>286</v>
+        <v>133</v>
       </c>
       <c r="M52" s="28"/>
       <c r="N52" s="28"/>
       <c r="O52" s="28" t="s">
-        <v>289</v>
+        <v>134</v>
       </c>
       <c r="P52" s="28"/>
       <c r="Q52" s="37" t="s">
-        <v>294</v>
+        <v>374</v>
       </c>
       <c r="R52" s="38" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="S52" s="38" t="s">
-        <v>288</v>
+        <v>135</v>
       </c>
       <c r="T52" s="23">
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B53" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C53" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="D53" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="E53" s="16"/>
-      <c r="F53" s="17">
-        <v>0</v>
-      </c>
-      <c r="G53" s="18">
-        <v>0</v>
-      </c>
-      <c r="H53" s="18">
-        <v>0</v>
-      </c>
-      <c r="I53" s="18">
-        <v>0</v>
-      </c>
-      <c r="J53" s="18"/>
-      <c r="K53" s="19" t="s">
-        <v>228</v>
-      </c>
-      <c r="L53" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="M53" s="19"/>
-      <c r="N53" s="19"/>
-      <c r="O53" s="20"/>
-      <c r="P53" s="20"/>
-      <c r="Q53" s="21" t="s">
-        <v>378</v>
-      </c>
-      <c r="R53" s="22" t="s">
-        <v>379</v>
-      </c>
-      <c r="S53" s="22" t="s">
-        <v>176</v>
+    <row r="53" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53" s="32" t="s">
+        <v>285</v>
+      </c>
+      <c r="D53" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="E53" s="51" t="s">
+        <v>277</v>
+      </c>
+      <c r="F53" s="34">
+        <v>5</v>
+      </c>
+      <c r="G53" s="35">
+        <v>0</v>
+      </c>
+      <c r="H53" s="35">
+        <v>55</v>
+      </c>
+      <c r="I53" s="35"/>
+      <c r="J53" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="K53" s="28" t="s">
+        <v>286</v>
+      </c>
+      <c r="L53" s="28" t="s">
+        <v>285</v>
+      </c>
+      <c r="M53" s="28"/>
+      <c r="N53" s="28"/>
+      <c r="O53" s="28" t="s">
+        <v>288</v>
+      </c>
+      <c r="P53" s="28"/>
+      <c r="Q53" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="R53" s="38" t="s">
+        <v>376</v>
+      </c>
+      <c r="S53" s="38" t="s">
+        <v>287</v>
       </c>
       <c r="T53" s="23">
         <v>49</v>
       </c>
     </row>
     <row r="54" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B54" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="C54" s="32" t="s">
-        <v>169</v>
-      </c>
-      <c r="D54" s="32" t="s">
+      <c r="B54" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C54" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="D54" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="E54" s="52" t="s">
-        <v>248</v>
-      </c>
-      <c r="F54" s="34">
-        <v>1</v>
-      </c>
-      <c r="G54" s="35">
-        <v>155000</v>
-      </c>
-      <c r="H54" s="35">
-        <v>0</v>
-      </c>
-      <c r="I54" s="35">
-        <v>1</v>
-      </c>
-      <c r="J54" s="35"/>
-      <c r="K54" s="36" t="s">
-        <v>229</v>
-      </c>
-      <c r="L54" s="36" t="s">
-        <v>169</v>
-      </c>
-      <c r="M54" s="36"/>
-      <c r="N54" s="36"/>
-      <c r="O54" s="28" t="s">
-        <v>182</v>
-      </c>
-      <c r="P54" s="28"/>
-      <c r="Q54" s="37" t="s">
-        <v>380</v>
-      </c>
-      <c r="R54" s="38" t="s">
-        <v>381</v>
-      </c>
-      <c r="S54" s="38" t="s">
-        <v>177</v>
+      <c r="E54" s="16"/>
+      <c r="F54" s="17">
+        <v>0</v>
+      </c>
+      <c r="G54" s="18">
+        <v>0</v>
+      </c>
+      <c r="H54" s="18">
+        <v>0</v>
+      </c>
+      <c r="I54" s="18">
+        <v>0</v>
+      </c>
+      <c r="J54" s="18"/>
+      <c r="K54" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="L54" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="M54" s="19"/>
+      <c r="N54" s="19"/>
+      <c r="O54" s="20"/>
+      <c r="P54" s="20"/>
+      <c r="Q54" s="21" t="s">
+        <v>377</v>
+      </c>
+      <c r="R54" s="22" t="s">
+        <v>378</v>
+      </c>
+      <c r="S54" s="22" t="s">
+        <v>176</v>
       </c>
       <c r="T54" s="23">
         <v>50</v>
@@ -5607,16 +5680,16 @@
         <v>3</v>
       </c>
       <c r="C55" s="32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D55" s="32" t="s">
         <v>167</v>
       </c>
-      <c r="E55" s="51" t="s">
-        <v>254</v>
+      <c r="E55" s="52" t="s">
+        <v>248</v>
       </c>
       <c r="F55" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G55" s="35">
         <v>155000</v>
@@ -5625,29 +5698,29 @@
         <v>0</v>
       </c>
       <c r="I55" s="35">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J55" s="35"/>
       <c r="K55" s="36" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L55" s="36" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M55" s="36"/>
       <c r="N55" s="36"/>
       <c r="O55" s="28" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="P55" s="28"/>
       <c r="Q55" s="37" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="R55" s="38" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="S55" s="38" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="T55" s="23">
         <v>51</v>
@@ -5658,16 +5731,16 @@
         <v>3</v>
       </c>
       <c r="C56" s="32" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D56" s="32" t="s">
         <v>167</v>
       </c>
       <c r="E56" s="51" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
       <c r="F56" s="34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G56" s="35">
         <v>155000</v>
@@ -5675,181 +5748,181 @@
       <c r="H56" s="35">
         <v>0</v>
       </c>
-      <c r="I56" s="27">
-        <v>7</v>
-      </c>
-      <c r="J56" s="27"/>
-      <c r="K56" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="L56" s="28" t="s">
-        <v>171</v>
-      </c>
-      <c r="M56" s="28"/>
-      <c r="N56" s="28"/>
+      <c r="I56" s="35">
+        <v>4</v>
+      </c>
+      <c r="J56" s="35"/>
+      <c r="K56" s="36" t="s">
+        <v>230</v>
+      </c>
+      <c r="L56" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="M56" s="36"/>
+      <c r="N56" s="36"/>
       <c r="O56" s="28" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="P56" s="28"/>
       <c r="Q56" s="37" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="R56" s="38" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="S56" s="38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="T56" s="23">
         <v>52</v>
       </c>
     </row>
-    <row r="57" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B57" s="31" t="s">
         <v>3</v>
       </c>
       <c r="C57" s="32" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D57" s="32" t="s">
         <v>167</v>
       </c>
-      <c r="E57" s="55" t="s">
-        <v>264</v>
+      <c r="E57" s="51" t="s">
+        <v>240</v>
       </c>
       <c r="F57" s="34">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G57" s="35">
-        <v>0</v>
+        <v>155000</v>
       </c>
       <c r="H57" s="35">
-        <v>45</v>
-      </c>
-      <c r="I57" s="42">
-        <v>10</v>
-      </c>
-      <c r="J57" s="42"/>
-      <c r="K57" s="43" t="s">
-        <v>232</v>
+        <v>0</v>
+      </c>
+      <c r="I57" s="27">
+        <v>7</v>
+      </c>
+      <c r="J57" s="27"/>
+      <c r="K57" s="28" t="s">
+        <v>231</v>
       </c>
       <c r="L57" s="28" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M57" s="28"/>
       <c r="N57" s="28"/>
       <c r="O57" s="28" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="P57" s="28"/>
       <c r="Q57" s="37" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="R57" s="38" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="S57" s="38" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="T57" s="23">
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B58" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C58" s="15" t="s">
-        <v>233</v>
-      </c>
-      <c r="D58" s="15" t="s">
-        <v>234</v>
-      </c>
-      <c r="E58" s="47"/>
-      <c r="F58" s="17">
-        <v>0</v>
-      </c>
-      <c r="G58" s="18">
-        <v>0</v>
-      </c>
-      <c r="H58" s="18">
-        <v>0</v>
-      </c>
-      <c r="I58" s="48">
-        <v>0</v>
-      </c>
-      <c r="J58" s="48"/>
-      <c r="K58" s="19" t="s">
-        <v>235</v>
-      </c>
-      <c r="L58" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="M58" s="19"/>
-      <c r="N58" s="19"/>
-      <c r="O58" s="20" t="s">
-        <v>271</v>
-      </c>
-      <c r="P58" s="20"/>
-      <c r="Q58" s="21" t="s">
-        <v>388</v>
-      </c>
-      <c r="R58" s="22" t="s">
-        <v>389</v>
-      </c>
-      <c r="S58" s="22" t="s">
-        <v>266</v>
+    <row r="58" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C58" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="D58" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="E58" s="55" t="s">
+        <v>264</v>
+      </c>
+      <c r="F58" s="34">
+        <v>4</v>
+      </c>
+      <c r="G58" s="35">
+        <v>0</v>
+      </c>
+      <c r="H58" s="35">
+        <v>45</v>
+      </c>
+      <c r="I58" s="42">
+        <v>10</v>
+      </c>
+      <c r="J58" s="42"/>
+      <c r="K58" s="43" t="s">
+        <v>232</v>
+      </c>
+      <c r="L58" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="M58" s="28"/>
+      <c r="N58" s="28"/>
+      <c r="O58" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="P58" s="28"/>
+      <c r="Q58" s="37" t="s">
+        <v>385</v>
+      </c>
+      <c r="R58" s="38" t="s">
+        <v>386</v>
+      </c>
+      <c r="S58" s="38" t="s">
+        <v>180</v>
       </c>
       <c r="T58" s="23">
         <v>54</v>
       </c>
     </row>
     <row r="59" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B59" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="C59" s="32" t="s">
-        <v>236</v>
-      </c>
-      <c r="D59" s="32" t="s">
+      <c r="B59" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C59" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="D59" s="15" t="s">
         <v>234</v>
       </c>
-      <c r="E59" s="49" t="s">
-        <v>265</v>
-      </c>
-      <c r="F59" s="34">
-        <v>1</v>
-      </c>
-      <c r="G59" s="35">
-        <v>300000</v>
-      </c>
-      <c r="H59" s="35">
-        <v>0</v>
-      </c>
-      <c r="I59" s="50">
-        <v>1</v>
-      </c>
-      <c r="J59" s="35"/>
-      <c r="K59" s="36" t="s">
-        <v>238</v>
-      </c>
-      <c r="L59" s="36" t="s">
-        <v>236</v>
-      </c>
-      <c r="M59" s="36"/>
-      <c r="N59" s="36"/>
-      <c r="O59" s="28" t="s">
-        <v>272</v>
-      </c>
-      <c r="P59" s="28"/>
-      <c r="Q59" s="37" t="s">
-        <v>390</v>
-      </c>
-      <c r="R59" s="38" t="s">
-        <v>391</v>
-      </c>
-      <c r="S59" s="38" t="s">
-        <v>267</v>
+      <c r="E59" s="47"/>
+      <c r="F59" s="17">
+        <v>0</v>
+      </c>
+      <c r="G59" s="18">
+        <v>0</v>
+      </c>
+      <c r="H59" s="18">
+        <v>0</v>
+      </c>
+      <c r="I59" s="48">
+        <v>0</v>
+      </c>
+      <c r="J59" s="48"/>
+      <c r="K59" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="L59" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="M59" s="19"/>
+      <c r="N59" s="19"/>
+      <c r="O59" s="20" t="s">
+        <v>270</v>
+      </c>
+      <c r="P59" s="20"/>
+      <c r="Q59" s="21" t="s">
+        <v>387</v>
+      </c>
+      <c r="R59" s="22" t="s">
+        <v>388</v>
+      </c>
+      <c r="S59" s="22" t="s">
+        <v>266</v>
       </c>
       <c r="T59" s="23">
         <v>55</v>
@@ -5860,16 +5933,16 @@
         <v>3</v>
       </c>
       <c r="C60" s="32" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D60" s="32" t="s">
         <v>234</v>
       </c>
-      <c r="E60" s="51" t="s">
-        <v>240</v>
+      <c r="E60" s="49" t="s">
+        <v>265</v>
       </c>
       <c r="F60" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G60" s="35">
         <v>300000</v>
@@ -5877,30 +5950,30 @@
       <c r="H60" s="35">
         <v>0</v>
       </c>
-      <c r="I60" s="35">
-        <v>4</v>
+      <c r="I60" s="50">
+        <v>1</v>
       </c>
       <c r="J60" s="35"/>
       <c r="K60" s="36" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="L60" s="36" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="M60" s="36"/>
       <c r="N60" s="36"/>
       <c r="O60" s="28" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="P60" s="28"/>
       <c r="Q60" s="37" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="R60" s="38" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="S60" s="38" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="T60" s="23">
         <v>56</v>
@@ -5911,16 +5984,16 @@
         <v>3</v>
       </c>
       <c r="C61" s="32" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D61" s="32" t="s">
         <v>234</v>
       </c>
       <c r="E61" s="51" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F61" s="34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G61" s="35">
         <v>300000</v>
@@ -5928,230 +6001,228 @@
       <c r="H61" s="35">
         <v>0</v>
       </c>
-      <c r="I61" s="27">
-        <v>7</v>
-      </c>
-      <c r="J61" s="27"/>
-      <c r="K61" s="28" t="s">
-        <v>244</v>
-      </c>
-      <c r="L61" s="28" t="s">
-        <v>242</v>
-      </c>
-      <c r="M61" s="28"/>
-      <c r="N61" s="28"/>
+      <c r="I61" s="35">
+        <v>4</v>
+      </c>
+      <c r="J61" s="35"/>
+      <c r="K61" s="36" t="s">
+        <v>241</v>
+      </c>
+      <c r="L61" s="36" t="s">
+        <v>239</v>
+      </c>
+      <c r="M61" s="36"/>
+      <c r="N61" s="36"/>
       <c r="O61" s="28" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="P61" s="28"/>
       <c r="Q61" s="37" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="R61" s="38" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="S61" s="38" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="T61" s="23">
         <v>57</v>
       </c>
     </row>
-    <row r="62" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B62" s="31" t="s">
         <v>3</v>
       </c>
       <c r="C62" s="32" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D62" s="32" t="s">
         <v>234</v>
       </c>
-      <c r="E62" s="55" t="s">
-        <v>246</v>
+      <c r="E62" s="51" t="s">
+        <v>243</v>
       </c>
       <c r="F62" s="34">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G62" s="35">
-        <v>0</v>
+        <v>300000</v>
       </c>
       <c r="H62" s="35">
-        <v>45</v>
-      </c>
-      <c r="I62" s="42">
-        <v>10</v>
-      </c>
-      <c r="J62" s="42"/>
+        <v>0</v>
+      </c>
+      <c r="I62" s="27">
+        <v>7</v>
+      </c>
+      <c r="J62" s="27"/>
       <c r="K62" s="28" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="L62" s="28" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="M62" s="28"/>
       <c r="N62" s="28"/>
       <c r="O62" s="28" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="P62" s="28"/>
       <c r="Q62" s="37" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="R62" s="38" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="S62" s="38" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="T62" s="23">
         <v>58</v>
       </c>
     </row>
     <row r="63" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B63" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C63" s="15" t="s">
-        <v>398</v>
-      </c>
-      <c r="D63" s="15" t="s">
-        <v>403</v>
-      </c>
-      <c r="E63" s="47"/>
-      <c r="F63" s="17">
-        <v>0</v>
-      </c>
-      <c r="G63" s="18">
-        <v>0</v>
-      </c>
-      <c r="H63" s="18">
-        <v>0</v>
-      </c>
-      <c r="I63" s="48">
-        <v>0</v>
-      </c>
-      <c r="J63" s="48"/>
-      <c r="K63" s="19" t="s">
-        <v>404</v>
-      </c>
-      <c r="L63" s="19" t="s">
-        <v>398</v>
-      </c>
-      <c r="M63" s="19"/>
-      <c r="N63" s="19"/>
-      <c r="O63" s="20"/>
-      <c r="P63" s="20"/>
-      <c r="Q63" s="21" t="s">
-        <v>409</v>
-      </c>
-      <c r="R63" s="22" t="s">
-        <v>414</v>
-      </c>
-      <c r="S63" s="22" t="s">
-        <v>419</v>
+      <c r="B63" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C63" s="32" t="s">
+        <v>245</v>
+      </c>
+      <c r="D63" s="32" t="s">
+        <v>234</v>
+      </c>
+      <c r="E63" s="51" t="s">
+        <v>246</v>
+      </c>
+      <c r="F63" s="34">
+        <v>4</v>
+      </c>
+      <c r="G63" s="35">
+        <v>0</v>
+      </c>
+      <c r="H63" s="35">
+        <v>45</v>
+      </c>
+      <c r="I63" s="27">
+        <v>10</v>
+      </c>
+      <c r="J63" s="27"/>
+      <c r="K63" s="28" t="s">
+        <v>247</v>
+      </c>
+      <c r="L63" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="M63" s="28"/>
+      <c r="N63" s="28"/>
+      <c r="O63" s="28" t="s">
+        <v>274</v>
+      </c>
+      <c r="P63" s="28"/>
+      <c r="Q63" s="37" t="s">
+        <v>395</v>
+      </c>
+      <c r="R63" s="38" t="s">
+        <v>396</v>
+      </c>
+      <c r="S63" s="38" t="s">
+        <v>269</v>
       </c>
       <c r="T63" s="23">
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="31" t="s">
         <v>3</v>
       </c>
       <c r="C64" s="32" t="s">
-        <v>399</v>
+        <v>437</v>
       </c>
       <c r="D64" s="32" t="s">
-        <v>403</v>
-      </c>
-      <c r="E64" s="49" t="s">
-        <v>243</v>
+        <v>234</v>
+      </c>
+      <c r="E64" s="62" t="s">
+        <v>438</v>
       </c>
       <c r="F64" s="34">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G64" s="35">
-        <v>400000</v>
+        <v>0</v>
       </c>
       <c r="H64" s="35">
-        <v>0</v>
-      </c>
-      <c r="I64" s="50">
-        <v>1</v>
-      </c>
-      <c r="J64" s="35"/>
-      <c r="K64" s="36" t="s">
-        <v>405</v>
-      </c>
-      <c r="L64" s="36" t="s">
-        <v>399</v>
-      </c>
-      <c r="M64" s="36"/>
-      <c r="N64" s="36"/>
-      <c r="O64" s="28" t="s">
-        <v>427</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="I64" s="60"/>
+      <c r="J64" s="60" t="s">
+        <v>433</v>
+      </c>
+      <c r="K64" s="28" t="s">
+        <v>439</v>
+      </c>
+      <c r="L64" s="28" t="s">
+        <v>437</v>
+      </c>
+      <c r="M64" s="28"/>
+      <c r="N64" s="28"/>
+      <c r="O64" s="28"/>
       <c r="P64" s="28"/>
       <c r="Q64" s="37" t="s">
-        <v>410</v>
+        <v>440</v>
       </c>
       <c r="R64" s="38" t="s">
-        <v>415</v>
+        <v>441</v>
       </c>
       <c r="S64" s="38" t="s">
-        <v>420</v>
+        <v>442</v>
       </c>
       <c r="T64" s="23">
         <v>60</v>
       </c>
     </row>
     <row r="65" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B65" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="C65" s="32" t="s">
-        <v>400</v>
-      </c>
-      <c r="D65" s="32" t="s">
+      <c r="B65" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C65" s="15" t="s">
+        <v>397</v>
+      </c>
+      <c r="D65" s="15" t="s">
+        <v>402</v>
+      </c>
+      <c r="E65" s="47"/>
+      <c r="F65" s="17">
+        <v>0</v>
+      </c>
+      <c r="G65" s="18">
+        <v>0</v>
+      </c>
+      <c r="H65" s="18">
+        <v>0</v>
+      </c>
+      <c r="I65" s="48">
+        <v>0</v>
+      </c>
+      <c r="J65" s="48"/>
+      <c r="K65" s="19" t="s">
         <v>403</v>
       </c>
-      <c r="E65" s="51" t="s">
-        <v>426</v>
-      </c>
-      <c r="F65" s="34">
-        <v>2</v>
-      </c>
-      <c r="G65" s="35">
-        <v>400000</v>
-      </c>
-      <c r="H65" s="35">
-        <v>0</v>
-      </c>
-      <c r="I65" s="35">
-        <v>4</v>
-      </c>
-      <c r="J65" s="35"/>
-      <c r="K65" s="36" t="s">
-        <v>406</v>
-      </c>
-      <c r="L65" s="36" t="s">
-        <v>400</v>
-      </c>
-      <c r="M65" s="36"/>
-      <c r="N65" s="36"/>
-      <c r="O65" s="28" t="s">
-        <v>428</v>
-      </c>
-      <c r="P65" s="28"/>
-      <c r="Q65" s="37" t="s">
-        <v>411</v>
-      </c>
-      <c r="R65" s="38" t="s">
-        <v>416</v>
-      </c>
-      <c r="S65" s="38" t="s">
-        <v>421</v>
+      <c r="L65" s="19" t="s">
+        <v>397</v>
+      </c>
+      <c r="M65" s="19"/>
+      <c r="N65" s="19"/>
+      <c r="O65" s="20"/>
+      <c r="P65" s="20"/>
+      <c r="Q65" s="21" t="s">
+        <v>408</v>
+      </c>
+      <c r="R65" s="22" t="s">
+        <v>413</v>
+      </c>
+      <c r="S65" s="22" t="s">
+        <v>418</v>
       </c>
       <c r="T65" s="23">
         <v>61</v>
@@ -6162,47 +6233,47 @@
         <v>3</v>
       </c>
       <c r="C66" s="32" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="D66" s="32" t="s">
-        <v>403</v>
-      </c>
-      <c r="E66" s="51" t="s">
-        <v>425</v>
+        <v>402</v>
+      </c>
+      <c r="E66" s="49" t="s">
+        <v>243</v>
       </c>
       <c r="F66" s="34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G66" s="35">
-        <v>0</v>
+        <v>400000</v>
       </c>
       <c r="H66" s="35">
-        <v>55</v>
-      </c>
-      <c r="I66" s="27">
-        <v>7</v>
-      </c>
-      <c r="J66" s="27"/>
-      <c r="K66" s="28" t="s">
-        <v>407</v>
-      </c>
-      <c r="L66" s="28" t="s">
-        <v>401</v>
-      </c>
-      <c r="M66" s="28"/>
-      <c r="N66" s="28"/>
+        <v>0</v>
+      </c>
+      <c r="I66" s="50">
+        <v>1</v>
+      </c>
+      <c r="J66" s="35"/>
+      <c r="K66" s="36" t="s">
+        <v>404</v>
+      </c>
+      <c r="L66" s="36" t="s">
+        <v>398</v>
+      </c>
+      <c r="M66" s="36"/>
+      <c r="N66" s="36"/>
       <c r="O66" s="28" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="P66" s="28"/>
       <c r="Q66" s="37" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="R66" s="38" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="S66" s="38" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="T66" s="23">
         <v>62</v>
@@ -6213,52 +6284,154 @@
         <v>3</v>
       </c>
       <c r="C67" s="32" t="s">
+        <v>399</v>
+      </c>
+      <c r="D67" s="32" t="s">
         <v>402</v>
       </c>
-      <c r="D67" s="32" t="s">
-        <v>403</v>
-      </c>
       <c r="E67" s="51" t="s">
-        <v>246</v>
+        <v>425</v>
       </c>
       <c r="F67" s="34">
+        <v>2</v>
+      </c>
+      <c r="G67" s="35">
+        <v>400000</v>
+      </c>
+      <c r="H67" s="35">
+        <v>0</v>
+      </c>
+      <c r="I67" s="35">
         <v>4</v>
       </c>
-      <c r="G67" s="35">
-        <v>0</v>
-      </c>
-      <c r="H67" s="35">
-        <v>65</v>
-      </c>
-      <c r="I67" s="48">
-        <v>0</v>
-      </c>
-      <c r="J67" s="27" t="s">
-        <v>424</v>
-      </c>
-      <c r="K67" s="28" t="s">
-        <v>408</v>
-      </c>
-      <c r="L67" s="28" t="s">
-        <v>402</v>
-      </c>
-      <c r="M67" s="28"/>
-      <c r="N67" s="28"/>
+      <c r="J67" s="35"/>
+      <c r="K67" s="36" t="s">
+        <v>405</v>
+      </c>
+      <c r="L67" s="36" t="s">
+        <v>399</v>
+      </c>
+      <c r="M67" s="36"/>
+      <c r="N67" s="36"/>
       <c r="O67" s="28" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="P67" s="28"/>
       <c r="Q67" s="37" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="R67" s="38" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="S67" s="38" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="T67" s="23">
         <v>63</v>
+      </c>
+    </row>
+    <row r="68" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B68" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C68" s="32" t="s">
+        <v>400</v>
+      </c>
+      <c r="D68" s="32" t="s">
+        <v>402</v>
+      </c>
+      <c r="E68" s="51" t="s">
+        <v>424</v>
+      </c>
+      <c r="F68" s="34">
+        <v>3</v>
+      </c>
+      <c r="G68" s="35">
+        <v>0</v>
+      </c>
+      <c r="H68" s="35">
+        <v>55</v>
+      </c>
+      <c r="I68" s="27">
+        <v>7</v>
+      </c>
+      <c r="J68" s="27"/>
+      <c r="K68" s="28" t="s">
+        <v>406</v>
+      </c>
+      <c r="L68" s="28" t="s">
+        <v>400</v>
+      </c>
+      <c r="M68" s="28"/>
+      <c r="N68" s="28"/>
+      <c r="O68" s="28" t="s">
+        <v>429</v>
+      </c>
+      <c r="P68" s="28"/>
+      <c r="Q68" s="37" t="s">
+        <v>411</v>
+      </c>
+      <c r="R68" s="38" t="s">
+        <v>416</v>
+      </c>
+      <c r="S68" s="38" t="s">
+        <v>421</v>
+      </c>
+      <c r="T68" s="23">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="69" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B69" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C69" s="32" t="s">
+        <v>401</v>
+      </c>
+      <c r="D69" s="32" t="s">
+        <v>402</v>
+      </c>
+      <c r="E69" s="51" t="s">
+        <v>246</v>
+      </c>
+      <c r="F69" s="34">
+        <v>4</v>
+      </c>
+      <c r="G69" s="35">
+        <v>0</v>
+      </c>
+      <c r="H69" s="35">
+        <v>65</v>
+      </c>
+      <c r="I69" s="48">
+        <v>0</v>
+      </c>
+      <c r="J69" s="27" t="s">
+        <v>423</v>
+      </c>
+      <c r="K69" s="28" t="s">
+        <v>407</v>
+      </c>
+      <c r="L69" s="28" t="s">
+        <v>401</v>
+      </c>
+      <c r="M69" s="28"/>
+      <c r="N69" s="28"/>
+      <c r="O69" s="28" t="s">
+        <v>428</v>
+      </c>
+      <c r="P69" s="28"/>
+      <c r="Q69" s="37" t="s">
+        <v>412</v>
+      </c>
+      <c r="R69" s="38" t="s">
+        <v>417</v>
+      </c>
+      <c r="S69" s="38" t="s">
+        <v>422</v>
+      </c>
+      <c r="T69" s="23">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding body parts for CNY umbra disguise
Former-commit-id: dcf1d82f6255b41d13cb4906f9650a84785179df
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="444">
   <si>
     <t>[sku]</t>
   </si>
@@ -1353,6 +1353,9 @@
   </si>
   <si>
     <t>darkdragon_skin_chineseNewYear</t>
+  </si>
+  <si>
+    <t>PF_Dark_LNY_Chin;PF_Dark_LNY_Helmet;PF_Dark_LNY_Shoulder_LF;PF_Dark_LNY_Shoulder_RT;PF_Dark_LNY_Side_LF;PF_Dark_LNY_Side_RT;PF_Dark_LNY_Skirt;PF_Dark_LNY_Wing_LF;PF_Dark_LNY_Wing_RT</t>
   </si>
 </sst>
 </file>
@@ -1492,7 +1495,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -1759,26 +1762,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
@@ -1955,13 +1943,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3050,8 +3032,8 @@
   </sheetPr>
   <dimension ref="B1:T69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="O64" sqref="O64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4481,7 +4463,7 @@
       <c r="D31" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E31" s="61" t="s">
+      <c r="E31" s="60" t="s">
         <v>431</v>
       </c>
       <c r="F31" s="26">
@@ -6142,7 +6124,7 @@
       <c r="D64" s="32" t="s">
         <v>234</v>
       </c>
-      <c r="E64" s="62" t="s">
+      <c r="E64" s="55" t="s">
         <v>438</v>
       </c>
       <c r="F64" s="34">
@@ -6154,8 +6136,8 @@
       <c r="H64" s="35">
         <v>65</v>
       </c>
-      <c r="I64" s="60"/>
-      <c r="J64" s="60" t="s">
+      <c r="I64" s="42"/>
+      <c r="J64" s="42" t="s">
         <v>433</v>
       </c>
       <c r="K64" s="28" t="s">
@@ -6166,7 +6148,9 @@
       </c>
       <c r="M64" s="28"/>
       <c r="N64" s="28"/>
-      <c r="O64" s="28"/>
+      <c r="O64" s="28" t="s">
+        <v>443</v>
+      </c>
       <c r="P64" s="28"/>
       <c r="Q64" s="37" t="s">
         <v>440</v>

</xml_diff>

<commit_message>
Added FX_PF_ChineseDragonBoost for Dark Dragon LNY Skin.
Former-commit-id: a877d48b64c97a1e4984fa86c6c1aae66afbb17c
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="445">
   <si>
     <t>[sku]</t>
   </si>
@@ -1356,6 +1356,9 @@
   </si>
   <si>
     <t>PF_Dark_LNY_Chin;PF_Dark_LNY_Helmet;PF_Dark_LNY_Shoulder_LF;PF_Dark_LNY_Shoulder_RT;PF_Dark_LNY_Side_LF;PF_Dark_LNY_Side_RT;PF_Dark_LNY_Skirt;PF_Dark_LNY_Wing_LF;PF_Dark_LNY_Wing_RT</t>
+  </si>
+  <si>
+    <t>FX_PF_ChineseDragonBoost</t>
   </si>
 </sst>
 </file>
@@ -3032,8 +3035,8 @@
   </sheetPr>
   <dimension ref="B1:T69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="O64" sqref="O64"/>
+    <sheetView tabSelected="1" topLeftCell="G34" workbookViewId="0">
+      <selection activeCell="O70" sqref="O70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6151,7 +6154,9 @@
       <c r="O64" s="28" t="s">
         <v>443</v>
       </c>
-      <c r="P64" s="28"/>
+      <c r="P64" s="28" t="s">
+        <v>444</v>
+      </c>
       <c r="Q64" s="37" t="s">
         <v>440</v>
       </c>

</xml_diff>

<commit_message>
Dragon Classic LNY disguise parts
Former-commit-id: 3ab7ca2ac8a14a78b17fcb4aa5018d25bf9c3849
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="446">
   <si>
     <t>[sku]</t>
   </si>
@@ -1359,6 +1359,9 @@
   </si>
   <si>
     <t>FX_PF_ChineseDragonBoost</t>
+  </si>
+  <si>
+    <t>PF_Classic_LNY_Helmet;PF_Classic_LNY_Belt;PF_Classic_LNY_Chin;PF_Classic_LNY_Shoulder_LF;PF_Classic_LNY_Shoulder_RT;PF_ClassicLNY_Wing_LF;PF_ClassicLNY_Wing_RT</t>
   </si>
 </sst>
 </file>
@@ -1498,7 +1501,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -1750,26 +1753,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
@@ -1946,8 +1934,11 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3035,8 +3026,8 @@
   </sheetPr>
   <dimension ref="B1:T69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G34" workbookViewId="0">
-      <selection activeCell="O70" sqref="O70"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4412,13 +4403,13 @@
       <c r="C30" s="23" t="s">
         <v>279</v>
       </c>
-      <c r="D30" s="23" t="s">
+      <c r="D30" s="60" t="s">
         <v>11</v>
       </c>
       <c r="E30" s="51" t="s">
         <v>275</v>
       </c>
-      <c r="F30" s="26">
+      <c r="F30" s="61">
         <v>5</v>
       </c>
       <c r="G30" s="27">
@@ -4466,7 +4457,7 @@
       <c r="D31" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E31" s="60" t="s">
+      <c r="E31" s="54" t="s">
         <v>431</v>
       </c>
       <c r="F31" s="26">
@@ -4490,7 +4481,9 @@
       </c>
       <c r="M31" s="28"/>
       <c r="N31" s="28"/>
-      <c r="O31" s="28"/>
+      <c r="O31" s="28" t="s">
+        <v>445</v>
+      </c>
       <c r="P31" s="28"/>
       <c r="Q31" s="29" t="s">
         <v>435</v>

</xml_diff>

<commit_message>
Skeleton texts (just english) and some values
Former-commit-id: 9d0afc3c8c761f252bb33cb3051b279c3f8c8048
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="disguises" sheetId="5" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3162,8 +3162,8 @@
   </sheetPr>
   <dimension ref="B1:T74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L40" workbookViewId="0">
-      <selection activeCell="F80" sqref="F80"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="I77" sqref="I77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6769,7 +6769,7 @@
         <v>70</v>
       </c>
       <c r="I74" s="63">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J74" s="63"/>
       <c r="K74" s="28" t="s">

</xml_diff>

<commit_message>
Added the prefabs for the skeleton skins in content!
Former-commit-id: d42979665c33cc0ad80ce38a9e1c5b500fbee084
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="479">
   <si>
     <t>[sku]</t>
   </si>
@@ -1451,13 +1451,16 @@
     <t>PF_skeleton_body_fire;PF_skeleton_mouth_fire;PF_skeleton_tail_fire</t>
   </si>
   <si>
-    <t>PF_skeleton_termi_wing_LF;PF_skeleton_termi_wing_LF</t>
-  </si>
-  <si>
-    <t>PF_skeleton_mex_guitar;PF_skeleton_mex_hat;PF_skeleton_mex_jacket;PF_skeleton_mex_sleeve_RT;PF_skeleton_mex_sleeve_LF</t>
-  </si>
-  <si>
-    <t>PF_skeleton_viking_necklace;PF_skeleton_viking_axe;PF_skeleton_viking_belt;PF_skeleton_viking_helmet;PF_skeleton_viking_shield;PF_skeleton_viking_shoulder_LF;PF_skeleton_viking_shoulder_RT</t>
+    <t>PF_skeleton_motu_axe;PF_skeleton_motu_chest;PF_skeleton_motu_hood;PF_skeleton_motu_shin_LF;PF_skeleton_motu_shin_RT;PF_skeleton_motu_shoulder_LF;PF_skeleton_motu_shoulder_RT;PF_skeleton_mouth_fire_blue;PF_skeleton_tail_fire_blue</t>
+  </si>
+  <si>
+    <t>PF_skeleton_termi_wing_LF;PF_skeleton_termi_wing_RT;PF_skeleton_body_fire;PF_skeleton_mouth_fire;PF_skeleton_tail_fire</t>
+  </si>
+  <si>
+    <t>PF_skeleton_mex_guitar;PF_skeleton_mex_hat;PF_skeleton_mex_jacket;PF_skeleton_mex_sleeve_RT;PF_skeleton_mex_sleeve_LF;PF_skeleton_mouth_fire</t>
+  </si>
+  <si>
+    <t>PF_skeleton_viking_necklace;PF_skeleton_viking_axe;PF_skeleton_viking_belt;PF_skeleton_viking_helmet;PF_skeleton_viking_shield;PF_skeleton_viking_shoulder_LF;PF_skeleton_viking_shoulder_RT;PF_skeleton_body_fire_blue;PF_skeleton_mouth_fire_blue;PF_skeleton_tail_fire_blue</t>
   </si>
 </sst>
 </file>
@@ -3246,7 +3249,7 @@
   <dimension ref="B1:T74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+      <selection activeCell="J81" sqref="J81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6681,7 +6684,7 @@
         <v>469</v>
       </c>
       <c r="T70" s="71">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="2:20" x14ac:dyDescent="0.25">
@@ -6732,7 +6735,7 @@
         <v>470</v>
       </c>
       <c r="T71" s="63">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="72" spans="2:20" x14ac:dyDescent="0.25">
@@ -6769,7 +6772,9 @@
       </c>
       <c r="M72" s="62"/>
       <c r="N72" s="62"/>
-      <c r="O72" s="62"/>
+      <c r="O72" s="62" t="s">
+        <v>476</v>
+      </c>
       <c r="P72" s="62"/>
       <c r="Q72" s="68" t="s">
         <v>461</v>
@@ -6781,7 +6786,7 @@
         <v>471</v>
       </c>
       <c r="T72" s="63">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="73" spans="2:20" x14ac:dyDescent="0.25">
@@ -6819,7 +6824,7 @@
       <c r="M73" s="62"/>
       <c r="N73" s="62"/>
       <c r="O73" s="62" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="P73" s="62"/>
       <c r="Q73" s="68" t="s">
@@ -6832,7 +6837,7 @@
         <v>472</v>
       </c>
       <c r="T73" s="63">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="74" spans="2:20" x14ac:dyDescent="0.25">
@@ -6870,7 +6875,7 @@
       <c r="M74" s="85"/>
       <c r="N74" s="85"/>
       <c r="O74" s="85" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="P74" s="85"/>
       <c r="Q74" s="69" t="s">
@@ -6883,7 +6888,7 @@
         <v>473</v>
       </c>
       <c r="T74" s="80">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding texts and setting values in the excel
Former-commit-id: cffe49487194a54f99b4200dba71d67b89244f79
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="483">
   <si>
     <t>[sku]</t>
   </si>
@@ -191,18 +191,12 @@
     <t>dragon_fat_2</t>
   </si>
   <si>
-    <t>PF_Mobster_Gun;PF_Mobster_Hat;PF_Mobster_Rose;PF_Mobster_Tie</t>
-  </si>
-  <si>
     <t>fat_mobster</t>
   </si>
   <si>
     <t>dragon_fat_3</t>
   </si>
   <si>
-    <t>PF_Scientist_Hat;PF_Scientist_Potion;PF_Scientist_Bowtie</t>
-  </si>
-  <si>
     <t>fat_scientist</t>
   </si>
   <si>
@@ -524,9 +518,6 @@
     <t>PS_RanbowTrail</t>
   </si>
   <si>
-    <t>PF_Rapper_Hat;PF_Rapper_Clock</t>
-  </si>
-  <si>
     <t>dragon_goldheist</t>
   </si>
   <si>
@@ -599,18 +590,6 @@
     <t>icon_reptile_2</t>
   </si>
   <si>
-    <t>icon_fat_0</t>
-  </si>
-  <si>
-    <t>icon_fat_1</t>
-  </si>
-  <si>
-    <t>icon_fat_2</t>
-  </si>
-  <si>
-    <t>icon_fat_3</t>
-  </si>
-  <si>
     <t>icon_bug_0</t>
   </si>
   <si>
@@ -1461,6 +1440,39 @@
   </si>
   <si>
     <t>PF_skeleton_viking_necklace;PF_skeleton_viking_axe;PF_skeleton_viking_belt;PF_skeleton_viking_helmet;PF_skeleton_viking_shield;PF_skeleton_viking_shoulder_LF;PF_skeleton_viking_shoulder_RT;PF_skeleton_body_fire_blue;PF_skeleton_mouth_fire_blue;PF_skeleton_tail_fire_blue</t>
+  </si>
+  <si>
+    <t>icon_tony_0</t>
+  </si>
+  <si>
+    <t>icon_tony_1</t>
+  </si>
+  <si>
+    <t>icon_tony_2</t>
+  </si>
+  <si>
+    <t>icon_tony_3</t>
+  </si>
+  <si>
+    <t>dragon_tony_0</t>
+  </si>
+  <si>
+    <t>dragon_tony_1</t>
+  </si>
+  <si>
+    <t>dragon_tony_2</t>
+  </si>
+  <si>
+    <t>dragon_tony_3</t>
+  </si>
+  <si>
+    <t>PF_tony_rap_chain;PF_tony_rap_head;PF_tony_rap_hoodie;PF_tony_rap_micro</t>
+  </si>
+  <si>
+    <t>PF_tony_mafia_belt;PF_tony_mafia_bowtie;PF_tony_mafia_gun;PF_tony_mafia_hat</t>
+  </si>
+  <si>
+    <t>PF_tony_scientist_beard;PF_tony_scientist_belt;PF_tony_scientist_hat</t>
   </si>
 </sst>
 </file>
@@ -3248,8 +3260,8 @@
   </sheetPr>
   <dimension ref="B1:T74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="J81" sqref="J81"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3338,7 +3350,7 @@
         <v>22</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="K4" s="11" t="s">
         <v>1</v>
@@ -3356,7 +3368,7 @@
         <v>26</v>
       </c>
       <c r="P4" s="11" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="Q4" s="12" t="s">
         <v>4</v>
@@ -3396,7 +3408,7 @@
       </c>
       <c r="J5" s="18"/>
       <c r="K5" s="19" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="L5" s="19" t="s">
         <v>29</v>
@@ -3406,10 +3418,10 @@
       <c r="O5" s="20"/>
       <c r="P5" s="20"/>
       <c r="Q5" s="21" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="R5" s="22" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="S5" s="22" t="s">
         <v>30</v>
@@ -3429,7 +3441,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="50" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F6" s="26">
         <v>1</v>
@@ -3445,7 +3457,7 @@
       </c>
       <c r="J6" s="27"/>
       <c r="K6" s="28" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="L6" s="28" t="s">
         <v>31</v>
@@ -3457,10 +3469,10 @@
       </c>
       <c r="P6" s="28"/>
       <c r="Q6" s="29" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="R6" s="30" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="S6" s="30" t="s">
         <v>33</v>
@@ -3494,7 +3506,7 @@
       </c>
       <c r="J7" s="18"/>
       <c r="K7" s="19" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="L7" s="19" t="s">
         <v>34</v>
@@ -3504,10 +3516,10 @@
       <c r="O7" s="20"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="21" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="R7" s="22" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="S7" s="22" t="s">
         <v>35</v>
@@ -3527,7 +3539,7 @@
         <v>6</v>
       </c>
       <c r="E8" s="51" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="F8" s="34">
         <v>1</v>
@@ -3543,7 +3555,7 @@
       </c>
       <c r="J8" s="35"/>
       <c r="K8" s="36" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="L8" s="36" t="s">
         <v>36</v>
@@ -3555,10 +3567,10 @@
       </c>
       <c r="P8" s="57"/>
       <c r="Q8" s="37" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="R8" s="38" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="S8" s="38" t="s">
         <v>38</v>
@@ -3578,7 +3590,7 @@
         <v>6</v>
       </c>
       <c r="E9" s="51" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="F9" s="26">
         <v>2</v>
@@ -3594,7 +3606,7 @@
       </c>
       <c r="J9" s="27"/>
       <c r="K9" s="28" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="L9" s="28" t="s">
         <v>39</v>
@@ -3606,10 +3618,10 @@
       </c>
       <c r="P9" s="43"/>
       <c r="Q9" s="29" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="R9" s="30" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="S9" s="30" t="s">
         <v>41</v>
@@ -3643,7 +3655,7 @@
       </c>
       <c r="J10" s="18"/>
       <c r="K10" s="19" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="L10" s="19" t="s">
         <v>42</v>
@@ -3653,10 +3665,10 @@
       <c r="O10" s="28"/>
       <c r="P10" s="28"/>
       <c r="Q10" s="21" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="R10" s="22" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="S10" s="22" t="s">
         <v>43</v>
@@ -3676,7 +3688,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="53" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F11" s="34">
         <v>1</v>
@@ -3692,7 +3704,7 @@
       </c>
       <c r="J11" s="35"/>
       <c r="K11" s="36" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L11" s="36" t="s">
         <v>44</v>
@@ -3704,10 +3716,10 @@
       </c>
       <c r="P11" s="28"/>
       <c r="Q11" s="37" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="R11" s="38" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="S11" s="38" t="s">
         <v>46</v>
@@ -3727,7 +3739,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="54" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="F12" s="41">
         <v>2</v>
@@ -3741,7 +3753,7 @@
       </c>
       <c r="J12" s="42"/>
       <c r="K12" s="43" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="L12" s="43" t="s">
         <v>47</v>
@@ -3753,10 +3765,10 @@
       </c>
       <c r="P12" s="43"/>
       <c r="Q12" s="44" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="R12" s="45" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="S12" s="45" t="s">
         <v>49</v>
@@ -3790,20 +3802,20 @@
       </c>
       <c r="J13" s="35"/>
       <c r="K13" s="36" t="s">
-        <v>191</v>
+        <v>472</v>
       </c>
       <c r="L13" s="36" t="s">
-        <v>50</v>
+        <v>476</v>
       </c>
       <c r="M13" s="36"/>
       <c r="N13" s="36"/>
       <c r="O13" s="28"/>
       <c r="P13" s="28"/>
       <c r="Q13" s="37" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="R13" s="38" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="S13" s="38" t="s">
         <v>51</v>
@@ -3823,7 +3835,7 @@
         <v>8</v>
       </c>
       <c r="E14" s="50" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F14" s="34">
         <v>1</v>
@@ -3839,22 +3851,22 @@
       </c>
       <c r="J14" s="35"/>
       <c r="K14" s="36" t="s">
-        <v>192</v>
+        <v>473</v>
       </c>
       <c r="L14" s="36" t="s">
-        <v>52</v>
+        <v>477</v>
       </c>
       <c r="M14" s="36"/>
       <c r="N14" s="36"/>
       <c r="O14" s="28" t="s">
-        <v>166</v>
+        <v>480</v>
       </c>
       <c r="P14" s="28"/>
       <c r="Q14" s="37" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="R14" s="38" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="S14" s="38" t="s">
         <v>53</v>
@@ -3874,7 +3886,7 @@
         <v>8</v>
       </c>
       <c r="E15" s="50" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="F15" s="26">
         <v>2</v>
@@ -3890,25 +3902,25 @@
       </c>
       <c r="J15" s="27"/>
       <c r="K15" s="28" t="s">
-        <v>193</v>
+        <v>474</v>
       </c>
       <c r="L15" s="28" t="s">
-        <v>54</v>
+        <v>478</v>
       </c>
       <c r="M15" s="28"/>
       <c r="N15" s="28"/>
       <c r="O15" s="28" t="s">
-        <v>55</v>
+        <v>481</v>
       </c>
       <c r="P15" s="28"/>
       <c r="Q15" s="58" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="R15" s="58" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="S15" s="58" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="T15" s="23">
         <v>11</v>
@@ -3919,13 +3931,13 @@
         <v>3</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D16" s="23" t="s">
         <v>8</v>
       </c>
       <c r="E16" s="50" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="F16" s="26">
         <v>3</v>
@@ -3941,25 +3953,25 @@
       </c>
       <c r="J16" s="27"/>
       <c r="K16" s="28" t="s">
-        <v>194</v>
+        <v>475</v>
       </c>
       <c r="L16" s="28" t="s">
-        <v>57</v>
+        <v>479</v>
       </c>
       <c r="M16" s="28"/>
       <c r="N16" s="28"/>
       <c r="O16" s="28" t="s">
-        <v>58</v>
+        <v>482</v>
       </c>
       <c r="P16" s="28"/>
       <c r="Q16" s="29" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="R16" s="30" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="S16" s="30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="T16" s="23">
         <v>12</v>
@@ -3970,7 +3982,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>9</v>
@@ -3990,23 +4002,23 @@
       </c>
       <c r="J17" s="18"/>
       <c r="K17" s="19" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="L17" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="M17" s="19"/>
       <c r="N17" s="19"/>
       <c r="O17" s="20"/>
       <c r="P17" s="20"/>
       <c r="Q17" s="21" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="R17" s="22" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="S17" s="22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="T17" s="23">
         <v>13</v>
@@ -4017,13 +4029,13 @@
         <v>3</v>
       </c>
       <c r="C18" s="32" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D18" s="32" t="s">
         <v>9</v>
       </c>
       <c r="E18" s="51" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="F18" s="34">
         <v>1</v>
@@ -4039,25 +4051,25 @@
       </c>
       <c r="J18" s="35"/>
       <c r="K18" s="36" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="L18" s="36" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="M18" s="36"/>
       <c r="N18" s="36"/>
       <c r="O18" s="28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="P18" s="28"/>
       <c r="Q18" s="37" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="R18" s="38" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="S18" s="38" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="T18" s="23">
         <v>14</v>
@@ -4068,13 +4080,13 @@
         <v>3</v>
       </c>
       <c r="C19" s="32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D19" s="32" t="s">
         <v>9</v>
       </c>
       <c r="E19" s="55" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="F19" s="34">
         <v>2</v>
@@ -4090,25 +4102,25 @@
       </c>
       <c r="J19" s="35"/>
       <c r="K19" s="36" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="L19" s="36" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M19" s="36"/>
       <c r="N19" s="36"/>
       <c r="O19" s="28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="P19" s="28"/>
       <c r="Q19" s="37" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="R19" s="38" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="S19" s="38" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T19" s="23">
         <v>15</v>
@@ -4119,13 +4131,13 @@
         <v>3</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D20" s="23" t="s">
         <v>9</v>
       </c>
       <c r="E20" s="53" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="F20" s="26">
         <v>3</v>
@@ -4141,25 +4153,25 @@
       </c>
       <c r="J20" s="27"/>
       <c r="K20" s="28" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="L20" s="28" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M20" s="28"/>
       <c r="N20" s="28"/>
       <c r="O20" s="28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P20" s="28"/>
       <c r="Q20" s="29" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="R20" s="30" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="S20" s="30" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="T20" s="23">
         <v>16</v>
@@ -4170,7 +4182,7 @@
         <v>3</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>10</v>
@@ -4190,25 +4202,25 @@
       </c>
       <c r="J21" s="18"/>
       <c r="K21" s="19" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="L21" s="19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M21" s="19"/>
       <c r="N21" s="19"/>
       <c r="O21" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="P21" s="20"/>
       <c r="Q21" s="21" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="R21" s="22" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="S21" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="T21" s="23">
         <v>17</v>
@@ -4219,13 +4231,13 @@
         <v>3</v>
       </c>
       <c r="C22" s="32" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D22" s="32" t="s">
         <v>10</v>
       </c>
       <c r="E22" s="51" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F22" s="34">
         <v>1</v>
@@ -4241,25 +4253,25 @@
       </c>
       <c r="J22" s="35"/>
       <c r="K22" s="36" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="L22" s="36" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="M22" s="36"/>
       <c r="N22" s="36"/>
       <c r="O22" s="28" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P22" s="28"/>
       <c r="Q22" s="37" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="R22" s="38" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="S22" s="38" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="T22" s="23">
         <v>18</v>
@@ -4270,13 +4282,13 @@
         <v>3</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D23" s="32" t="s">
         <v>10</v>
       </c>
       <c r="E23" s="51" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="F23" s="34">
         <v>2</v>
@@ -4292,25 +4304,25 @@
       </c>
       <c r="J23" s="35"/>
       <c r="K23" s="36" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="L23" s="36" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="M23" s="36"/>
       <c r="N23" s="36"/>
       <c r="O23" s="28" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="P23" s="28"/>
       <c r="Q23" s="37" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="R23" s="38" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="S23" s="38" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="T23" s="23">
         <v>19</v>
@@ -4321,13 +4333,13 @@
         <v>3</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D24" s="23" t="s">
         <v>10</v>
       </c>
       <c r="E24" s="50" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="F24" s="26">
         <v>3</v>
@@ -4343,25 +4355,25 @@
       </c>
       <c r="J24" s="27"/>
       <c r="K24" s="28" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="L24" s="28" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M24" s="28"/>
       <c r="N24" s="28"/>
       <c r="O24" s="28" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="P24" s="28"/>
       <c r="Q24" s="29" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="R24" s="30" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="S24" s="30" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="T24" s="23">
         <v>20</v>
@@ -4372,7 +4384,7 @@
         <v>3</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D25" s="15" t="s">
         <v>11</v>
@@ -4392,23 +4404,23 @@
       </c>
       <c r="J25" s="18"/>
       <c r="K25" s="19" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="L25" s="19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="M25" s="19"/>
       <c r="N25" s="19"/>
       <c r="O25" s="20"/>
       <c r="P25" s="20"/>
       <c r="Q25" s="21" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="R25" s="22" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="S25" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="T25" s="23">
         <v>21</v>
@@ -4419,13 +4431,13 @@
         <v>3</v>
       </c>
       <c r="C26" s="32" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D26" s="32" t="s">
         <v>11</v>
       </c>
       <c r="E26" s="51" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="F26" s="34">
         <v>1</v>
@@ -4441,25 +4453,25 @@
       </c>
       <c r="J26" s="35"/>
       <c r="K26" s="36" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="L26" s="36" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M26" s="36"/>
       <c r="N26" s="36"/>
       <c r="O26" s="28" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="P26" s="28"/>
       <c r="Q26" s="37" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="R26" s="38" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="S26" s="38" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="T26" s="23">
         <v>22</v>
@@ -4470,13 +4482,13 @@
         <v>3</v>
       </c>
       <c r="C27" s="32" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D27" s="32" t="s">
         <v>11</v>
       </c>
       <c r="E27" s="51" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="F27" s="34">
         <v>2</v>
@@ -4492,25 +4504,25 @@
       </c>
       <c r="J27" s="35"/>
       <c r="K27" s="36" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="L27" s="36" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="M27" s="36"/>
       <c r="N27" s="36"/>
       <c r="O27" s="28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="P27" s="28"/>
       <c r="Q27" s="37" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="R27" s="38" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="S27" s="38" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="T27" s="23">
         <v>23</v>
@@ -4521,13 +4533,13 @@
         <v>3</v>
       </c>
       <c r="C28" s="32" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D28" s="32" t="s">
         <v>11</v>
       </c>
       <c r="E28" s="51" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="F28" s="34">
         <v>3</v>
@@ -4543,25 +4555,25 @@
       </c>
       <c r="J28" s="27"/>
       <c r="K28" s="28" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="L28" s="28" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="M28" s="28"/>
       <c r="N28" s="28"/>
       <c r="O28" s="28" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="P28" s="28"/>
       <c r="Q28" s="37" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="R28" s="38" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="S28" s="38" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="T28" s="23">
         <v>24</v>
@@ -4572,13 +4584,13 @@
         <v>3</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D29" s="23" t="s">
         <v>11</v>
       </c>
       <c r="E29" s="50" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="F29" s="26">
         <v>4</v>
@@ -4594,25 +4606,25 @@
       </c>
       <c r="J29" s="27"/>
       <c r="K29" s="28" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="L29" s="28" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="M29" s="28"/>
       <c r="N29" s="28"/>
       <c r="O29" s="28" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="P29" s="28"/>
       <c r="Q29" s="58" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="R29" s="58" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="S29" s="58" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="T29" s="23">
         <v>25</v>
@@ -4623,13 +4635,13 @@
         <v>3</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="D30" s="59" t="s">
         <v>11</v>
       </c>
       <c r="E30" s="50" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F30" s="60">
         <v>5</v>
@@ -4642,28 +4654,28 @@
       </c>
       <c r="I30" s="27"/>
       <c r="J30" s="27" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="K30" s="28" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="L30" s="28" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="M30" s="28"/>
       <c r="N30" s="28"/>
       <c r="O30" s="28" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="P30" s="28"/>
       <c r="Q30" s="29" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="R30" s="30" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="S30" s="30" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="T30" s="23">
         <v>26</v>
@@ -4674,13 +4686,13 @@
         <v>3</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="D31" s="23" t="s">
         <v>11</v>
       </c>
       <c r="E31" s="53" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="F31" s="26">
         <v>6</v>
@@ -4693,28 +4705,28 @@
       </c>
       <c r="I31" s="27"/>
       <c r="J31" s="27" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="K31" s="28" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="L31" s="28" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="M31" s="28"/>
       <c r="N31" s="28"/>
       <c r="O31" s="28" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="P31" s="28"/>
       <c r="Q31" s="29" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="R31" s="30" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="S31" s="30" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="T31" s="23">
         <v>27</v>
@@ -4725,7 +4737,7 @@
         <v>3</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D32" s="15" t="s">
         <v>12</v>
@@ -4745,25 +4757,25 @@
       </c>
       <c r="J32" s="18"/>
       <c r="K32" s="19" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="L32" s="19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="M32" s="19"/>
       <c r="N32" s="19"/>
       <c r="O32" s="20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="P32" s="20"/>
       <c r="Q32" s="21" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="R32" s="22" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="S32" s="22" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="T32" s="23">
         <v>28</v>
@@ -4774,13 +4786,13 @@
         <v>3</v>
       </c>
       <c r="C33" s="32" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D33" s="32" t="s">
         <v>12</v>
       </c>
       <c r="E33" s="51" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="F33" s="34">
         <v>1</v>
@@ -4796,25 +4808,25 @@
       </c>
       <c r="J33" s="35"/>
       <c r="K33" s="36" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="L33" s="36" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="M33" s="36"/>
       <c r="N33" s="36"/>
       <c r="O33" s="28" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="P33" s="28"/>
       <c r="Q33" s="37" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="R33" s="38" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="S33" s="38" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="T33" s="23">
         <v>29</v>
@@ -4825,13 +4837,13 @@
         <v>3</v>
       </c>
       <c r="C34" s="32" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D34" s="32" t="s">
         <v>12</v>
       </c>
       <c r="E34" s="51" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="F34" s="34">
         <v>2</v>
@@ -4847,25 +4859,25 @@
       </c>
       <c r="J34" s="35"/>
       <c r="K34" s="36" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="L34" s="36" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M34" s="36"/>
       <c r="N34" s="36"/>
       <c r="O34" s="28" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="P34" s="28"/>
       <c r="Q34" s="37" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="R34" s="38" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="S34" s="38" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="T34" s="23">
         <v>30</v>
@@ -4876,13 +4888,13 @@
         <v>3</v>
       </c>
       <c r="C35" s="32" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D35" s="32" t="s">
         <v>12</v>
       </c>
       <c r="E35" s="50" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="F35" s="34">
         <v>3</v>
@@ -4898,25 +4910,25 @@
       </c>
       <c r="J35" s="27"/>
       <c r="K35" s="28" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="L35" s="28" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="M35" s="28"/>
       <c r="N35" s="28"/>
       <c r="O35" s="28" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="P35" s="28"/>
       <c r="Q35" s="37" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="R35" s="38" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="S35" s="38" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="T35" s="23">
         <v>31</v>
@@ -4927,13 +4939,13 @@
         <v>3</v>
       </c>
       <c r="C36" s="40" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D36" s="40" t="s">
         <v>12</v>
       </c>
       <c r="E36" s="54" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="F36" s="41">
         <v>4</v>
@@ -4949,25 +4961,25 @@
       </c>
       <c r="J36" s="42"/>
       <c r="K36" s="43" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="L36" s="43" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="M36" s="43"/>
       <c r="N36" s="43"/>
       <c r="O36" s="43" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="P36" s="43"/>
       <c r="Q36" s="44" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="R36" s="45" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="S36" s="45" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="T36" s="23">
         <v>32</v>
@@ -4978,10 +4990,10 @@
         <v>3</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E37" s="25"/>
       <c r="F37" s="26">
@@ -4998,23 +5010,23 @@
       </c>
       <c r="J37" s="27"/>
       <c r="K37" s="28" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="L37" s="28" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="M37" s="28"/>
       <c r="N37" s="28"/>
       <c r="O37" s="28"/>
       <c r="P37" s="28"/>
       <c r="Q37" s="29" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="R37" s="30" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="S37" s="30" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="T37" s="23">
         <v>33</v>
@@ -5025,13 +5037,13 @@
         <v>3</v>
       </c>
       <c r="C38" s="23" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E38" s="50" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="F38" s="26">
         <v>1</v>
@@ -5047,25 +5059,25 @@
       </c>
       <c r="J38" s="27"/>
       <c r="K38" s="28" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="L38" s="28" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="M38" s="28"/>
       <c r="N38" s="28"/>
       <c r="O38" s="28" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="P38" s="28"/>
       <c r="Q38" s="58" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="R38" s="58" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="S38" s="58" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="T38" s="23">
         <v>34</v>
@@ -5076,13 +5088,13 @@
         <v>3</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E39" s="50" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="F39" s="26">
         <v>2</v>
@@ -5098,25 +5110,25 @@
       </c>
       <c r="J39" s="27"/>
       <c r="K39" s="28" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="L39" s="28" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M39" s="28"/>
       <c r="N39" s="28"/>
       <c r="O39" s="28" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="P39" s="28"/>
       <c r="Q39" s="58" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="R39" s="58" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="S39" s="58" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="T39" s="23">
         <v>35</v>
@@ -5127,13 +5139,13 @@
         <v>3</v>
       </c>
       <c r="C40" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="D40" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="D40" s="23" t="s">
-        <v>141</v>
-      </c>
       <c r="E40" s="50" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="F40" s="26">
         <v>3</v>
@@ -5149,25 +5161,25 @@
       </c>
       <c r="J40" s="27"/>
       <c r="K40" s="28" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="L40" s="28" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M40" s="28"/>
       <c r="N40" s="28"/>
       <c r="O40" s="28" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="P40" s="28"/>
       <c r="Q40" s="58" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="R40" s="58" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="S40" s="58" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="T40" s="23">
         <v>36</v>
@@ -5178,13 +5190,13 @@
         <v>3</v>
       </c>
       <c r="C41" s="23" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E41" s="50" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="F41" s="26">
         <v>4</v>
@@ -5200,25 +5212,25 @@
       </c>
       <c r="J41" s="27"/>
       <c r="K41" s="28" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="L41" s="28" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="M41" s="28"/>
       <c r="N41" s="28"/>
       <c r="O41" s="28" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="P41" s="28"/>
       <c r="Q41" s="29" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="R41" s="30" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="S41" s="30" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="T41" s="23">
         <v>37</v>
@@ -5229,7 +5241,7 @@
         <v>3</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D42" s="15" t="s">
         <v>13</v>
@@ -5249,23 +5261,23 @@
       </c>
       <c r="J42" s="18"/>
       <c r="K42" s="19" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="L42" s="19" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M42" s="19"/>
       <c r="N42" s="19"/>
       <c r="O42" s="20"/>
       <c r="P42" s="20"/>
       <c r="Q42" s="21" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="R42" s="22" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="S42" s="22" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="T42" s="23">
         <v>38</v>
@@ -5276,13 +5288,13 @@
         <v>3</v>
       </c>
       <c r="C43" s="32" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D43" s="32" t="s">
         <v>13</v>
       </c>
       <c r="E43" s="51" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F43" s="34">
         <v>1</v>
@@ -5298,25 +5310,25 @@
       </c>
       <c r="J43" s="35"/>
       <c r="K43" s="36" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="L43" s="36" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M43" s="36"/>
       <c r="N43" s="36"/>
       <c r="O43" s="28" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="P43" s="28"/>
       <c r="Q43" s="37" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="R43" s="38" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="S43" s="38" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="T43" s="23">
         <v>39</v>
@@ -5327,13 +5339,13 @@
         <v>3</v>
       </c>
       <c r="C44" s="32" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D44" s="32" t="s">
         <v>13</v>
       </c>
       <c r="E44" s="51" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="F44" s="34">
         <v>2</v>
@@ -5349,25 +5361,25 @@
       </c>
       <c r="J44" s="35"/>
       <c r="K44" s="36" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="L44" s="36" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M44" s="36"/>
       <c r="N44" s="36"/>
       <c r="O44" s="28" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="P44" s="28"/>
       <c r="Q44" s="37" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="R44" s="38" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="S44" s="38" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="T44" s="23">
         <v>40</v>
@@ -5378,13 +5390,13 @@
         <v>3</v>
       </c>
       <c r="C45" s="32" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D45" s="32" t="s">
         <v>13</v>
       </c>
       <c r="E45" s="51" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="F45" s="34">
         <v>3</v>
@@ -5400,27 +5412,27 @@
       </c>
       <c r="J45" s="27"/>
       <c r="K45" s="28" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="L45" s="28" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M45" s="28"/>
       <c r="N45" s="28"/>
       <c r="O45" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="P45" s="28" t="s">
         <v>163</v>
       </c>
-      <c r="P45" s="28" t="s">
-        <v>165</v>
-      </c>
       <c r="Q45" s="37" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="R45" s="38" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="S45" s="38" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="T45" s="23">
         <v>41</v>
@@ -5431,13 +5443,13 @@
         <v>3</v>
       </c>
       <c r="C46" s="32" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D46" s="32" t="s">
         <v>13</v>
       </c>
       <c r="E46" s="51" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="F46" s="34">
         <v>4</v>
@@ -5453,23 +5465,23 @@
       </c>
       <c r="J46" s="27"/>
       <c r="K46" s="28" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="L46" s="28" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="M46" s="28"/>
       <c r="N46" s="28"/>
       <c r="O46" s="28"/>
       <c r="P46" s="28"/>
       <c r="Q46" s="37" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="R46" s="38" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="S46" s="38" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="T46" s="23">
         <v>42</v>
@@ -5480,13 +5492,13 @@
         <v>3</v>
       </c>
       <c r="C47" s="40" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="D47" s="40" t="s">
         <v>13</v>
       </c>
       <c r="E47" s="54" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="F47" s="41">
         <v>5</v>
@@ -5499,28 +5511,28 @@
       </c>
       <c r="I47" s="42"/>
       <c r="J47" s="42" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="K47" s="43" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="L47" s="43" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="M47" s="43"/>
       <c r="N47" s="43"/>
       <c r="O47" s="43" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="P47" s="43"/>
       <c r="Q47" s="29" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="R47" s="45" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="S47" s="45" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="T47" s="23">
         <v>43</v>
@@ -5531,7 +5543,7 @@
         <v>3</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D48" s="15" t="s">
         <v>14</v>
@@ -5551,23 +5563,23 @@
       </c>
       <c r="J48" s="18"/>
       <c r="K48" s="19" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="L48" s="19" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="M48" s="19"/>
       <c r="N48" s="19"/>
       <c r="O48" s="20"/>
       <c r="P48" s="20"/>
       <c r="Q48" s="21" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="R48" s="22" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="S48" s="22" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="T48" s="23">
         <v>44</v>
@@ -5578,13 +5590,13 @@
         <v>3</v>
       </c>
       <c r="C49" s="32" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D49" s="32" t="s">
         <v>14</v>
       </c>
       <c r="E49" s="51" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="F49" s="34">
         <v>1</v>
@@ -5600,25 +5612,25 @@
       </c>
       <c r="J49" s="35"/>
       <c r="K49" s="36" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="L49" s="36" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="M49" s="36"/>
       <c r="N49" s="36"/>
       <c r="O49" s="28" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="P49" s="28"/>
       <c r="Q49" s="37" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="R49" s="38" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="S49" s="38" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="T49" s="23">
         <v>45</v>
@@ -5629,13 +5641,13 @@
         <v>3</v>
       </c>
       <c r="C50" s="32" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D50" s="32" t="s">
         <v>14</v>
       </c>
       <c r="E50" s="50" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="F50" s="34">
         <v>2</v>
@@ -5651,25 +5663,25 @@
       </c>
       <c r="J50" s="35"/>
       <c r="K50" s="36" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="L50" s="36" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M50" s="36"/>
       <c r="N50" s="36"/>
       <c r="O50" s="28" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="P50" s="28"/>
       <c r="Q50" s="37" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="R50" s="38" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="S50" s="38" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="T50" s="23">
         <v>46</v>
@@ -5680,13 +5692,13 @@
         <v>3</v>
       </c>
       <c r="C51" s="32" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D51" s="32" t="s">
         <v>14</v>
       </c>
       <c r="E51" s="50" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="F51" s="34">
         <v>3</v>
@@ -5702,25 +5714,25 @@
       </c>
       <c r="J51" s="27"/>
       <c r="K51" s="28" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="L51" s="28" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="M51" s="28"/>
       <c r="N51" s="28"/>
       <c r="O51" s="28" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="P51" s="28"/>
       <c r="Q51" s="37" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="R51" s="38" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="S51" s="38" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="T51" s="23">
         <v>47</v>
@@ -5731,13 +5743,13 @@
         <v>3</v>
       </c>
       <c r="C52" s="32" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D52" s="32" t="s">
         <v>14</v>
       </c>
       <c r="E52" s="51" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="F52" s="34">
         <v>4</v>
@@ -5753,25 +5765,25 @@
       </c>
       <c r="J52" s="27"/>
       <c r="K52" s="28" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="L52" s="28" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="M52" s="28"/>
       <c r="N52" s="28"/>
       <c r="O52" s="28" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="P52" s="28"/>
       <c r="Q52" s="37" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="R52" s="38" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="S52" s="38" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="T52" s="23">
         <v>48</v>
@@ -5782,13 +5794,13 @@
         <v>3</v>
       </c>
       <c r="C53" s="32" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="D53" s="32" t="s">
         <v>14</v>
       </c>
       <c r="E53" s="50" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F53" s="34">
         <v>5</v>
@@ -5801,28 +5813,28 @@
       </c>
       <c r="I53" s="35"/>
       <c r="J53" s="27" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="K53" s="28" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="L53" s="28" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="M53" s="28"/>
       <c r="N53" s="28"/>
       <c r="O53" s="28" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="P53" s="28"/>
       <c r="Q53" s="37" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="R53" s="38" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="S53" s="38" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="T53" s="23">
         <v>49</v>
@@ -5833,10 +5845,10 @@
         <v>3</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E54" s="16"/>
       <c r="F54" s="17">
@@ -5853,23 +5865,23 @@
       </c>
       <c r="J54" s="18"/>
       <c r="K54" s="19" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="L54" s="19" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="M54" s="19"/>
       <c r="N54" s="19"/>
       <c r="O54" s="20"/>
       <c r="P54" s="20"/>
       <c r="Q54" s="21" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="R54" s="22" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="S54" s="22" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="T54" s="23">
         <v>50</v>
@@ -5880,13 +5892,13 @@
         <v>3</v>
       </c>
       <c r="C55" s="32" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D55" s="32" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E55" s="51" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="F55" s="34">
         <v>1</v>
@@ -5902,25 +5914,25 @@
       </c>
       <c r="J55" s="35"/>
       <c r="K55" s="36" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="L55" s="36" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="M55" s="36"/>
       <c r="N55" s="36"/>
       <c r="O55" s="28" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="P55" s="28"/>
       <c r="Q55" s="37" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="R55" s="38" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="S55" s="38" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="T55" s="23">
         <v>51</v>
@@ -5931,13 +5943,13 @@
         <v>3</v>
       </c>
       <c r="C56" s="32" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D56" s="32" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E56" s="50" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="F56" s="34">
         <v>2</v>
@@ -5953,25 +5965,25 @@
       </c>
       <c r="J56" s="35"/>
       <c r="K56" s="36" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="L56" s="36" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="M56" s="36"/>
       <c r="N56" s="36"/>
       <c r="O56" s="28" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="P56" s="28"/>
       <c r="Q56" s="37" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="R56" s="38" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="S56" s="38" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="T56" s="23">
         <v>52</v>
@@ -5982,13 +5994,13 @@
         <v>3</v>
       </c>
       <c r="C57" s="32" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D57" s="32" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E57" s="50" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="F57" s="34">
         <v>3</v>
@@ -6004,25 +6016,25 @@
       </c>
       <c r="J57" s="27"/>
       <c r="K57" s="28" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="L57" s="28" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="M57" s="28"/>
       <c r="N57" s="28"/>
       <c r="O57" s="28" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="P57" s="28"/>
       <c r="Q57" s="37" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="R57" s="38" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="S57" s="38" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="T57" s="23">
         <v>53</v>
@@ -6033,13 +6045,13 @@
         <v>3</v>
       </c>
       <c r="C58" s="32" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D58" s="32" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E58" s="54" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="F58" s="34">
         <v>4</v>
@@ -6055,25 +6067,25 @@
       </c>
       <c r="J58" s="42"/>
       <c r="K58" s="43" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="L58" s="28" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="M58" s="28"/>
       <c r="N58" s="28"/>
       <c r="O58" s="28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="P58" s="28"/>
       <c r="Q58" s="37" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="R58" s="38" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="S58" s="38" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="T58" s="23">
         <v>54</v>
@@ -6084,10 +6096,10 @@
         <v>3</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="D59" s="15" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="E59" s="50"/>
       <c r="F59" s="17">
@@ -6104,25 +6116,25 @@
       </c>
       <c r="J59" s="47"/>
       <c r="K59" s="19" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="L59" s="19" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="M59" s="19"/>
       <c r="N59" s="19"/>
       <c r="O59" s="20" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="P59" s="20"/>
       <c r="Q59" s="21" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="R59" s="22" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="S59" s="22" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="T59" s="23">
         <v>55</v>
@@ -6133,13 +6145,13 @@
         <v>3</v>
       </c>
       <c r="C60" s="32" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="D60" s="32" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="E60" s="48" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="F60" s="34">
         <v>1</v>
@@ -6155,25 +6167,25 @@
       </c>
       <c r="J60" s="35"/>
       <c r="K60" s="36" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="L60" s="36" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="M60" s="36"/>
       <c r="N60" s="36"/>
       <c r="O60" s="28" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="P60" s="28"/>
       <c r="Q60" s="37" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="R60" s="38" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="S60" s="38" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="T60" s="23">
         <v>56</v>
@@ -6184,13 +6196,13 @@
         <v>3</v>
       </c>
       <c r="C61" s="32" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="D61" s="32" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="E61" s="50" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="F61" s="34">
         <v>2</v>
@@ -6206,25 +6218,25 @@
       </c>
       <c r="J61" s="35"/>
       <c r="K61" s="36" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="L61" s="36" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="M61" s="36"/>
       <c r="N61" s="36"/>
       <c r="O61" s="28" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="P61" s="28"/>
       <c r="Q61" s="37" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="R61" s="38" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="S61" s="38" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="T61" s="23">
         <v>57</v>
@@ -6235,13 +6247,13 @@
         <v>3</v>
       </c>
       <c r="C62" s="32" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D62" s="32" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="E62" s="50" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="F62" s="34">
         <v>3</v>
@@ -6257,25 +6269,25 @@
       </c>
       <c r="J62" s="27"/>
       <c r="K62" s="28" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="L62" s="28" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="M62" s="28"/>
       <c r="N62" s="28"/>
       <c r="O62" s="28" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="P62" s="28"/>
       <c r="Q62" s="37" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="R62" s="38" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="S62" s="38" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="T62" s="23">
         <v>58</v>
@@ -6286,13 +6298,13 @@
         <v>3</v>
       </c>
       <c r="C63" s="32" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="D63" s="32" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="E63" s="50" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="F63" s="34">
         <v>4</v>
@@ -6308,25 +6320,25 @@
       </c>
       <c r="J63" s="27"/>
       <c r="K63" s="28" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="L63" s="28" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="M63" s="28"/>
       <c r="N63" s="28"/>
       <c r="O63" s="28" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="P63" s="28"/>
       <c r="Q63" s="37" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="R63" s="38" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="S63" s="38" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="T63" s="23">
         <v>59</v>
@@ -6337,13 +6349,13 @@
         <v>3</v>
       </c>
       <c r="C64" s="32" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="D64" s="32" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="E64" s="54" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="F64" s="34">
         <v>5</v>
@@ -6356,30 +6368,30 @@
       </c>
       <c r="I64" s="42"/>
       <c r="J64" s="42" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="K64" s="28" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="L64" s="28" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="M64" s="28"/>
       <c r="N64" s="28"/>
       <c r="O64" s="28" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="P64" s="28" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="Q64" s="37" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="R64" s="38" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="S64" s="38" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
       <c r="T64" s="23">
         <v>60</v>
@@ -6390,10 +6402,10 @@
         <v>3</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="D65" s="15" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="E65" s="50"/>
       <c r="F65" s="17">
@@ -6410,23 +6422,23 @@
       </c>
       <c r="J65" s="47"/>
       <c r="K65" s="19" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="L65" s="19" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="M65" s="19"/>
       <c r="N65" s="19"/>
       <c r="O65" s="20"/>
       <c r="P65" s="20"/>
       <c r="Q65" s="21" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="R65" s="22" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="S65" s="22" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="T65" s="23">
         <v>61</v>
@@ -6437,13 +6449,13 @@
         <v>3</v>
       </c>
       <c r="C66" s="32" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="D66" s="32" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="E66" s="48" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="F66" s="34">
         <v>1</v>
@@ -6459,25 +6471,25 @@
       </c>
       <c r="J66" s="35"/>
       <c r="K66" s="36" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="L66" s="36" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="M66" s="36"/>
       <c r="N66" s="36"/>
       <c r="O66" s="28" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="P66" s="28"/>
       <c r="Q66" s="37" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="R66" s="38" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="S66" s="38" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="T66" s="23">
         <v>62</v>
@@ -6488,13 +6500,13 @@
         <v>3</v>
       </c>
       <c r="C67" s="32" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="D67" s="32" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="E67" s="50" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="F67" s="34">
         <v>2</v>
@@ -6510,25 +6522,25 @@
       </c>
       <c r="J67" s="35"/>
       <c r="K67" s="36" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="L67" s="36" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="M67" s="36"/>
       <c r="N67" s="36"/>
       <c r="O67" s="28" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="P67" s="28"/>
       <c r="Q67" s="37" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="R67" s="38" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="S67" s="38" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="T67" s="23">
         <v>63</v>
@@ -6539,13 +6551,13 @@
         <v>3</v>
       </c>
       <c r="C68" s="32" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="D68" s="32" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="E68" s="50" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="F68" s="34">
         <v>3</v>
@@ -6561,25 +6573,25 @@
       </c>
       <c r="J68" s="27"/>
       <c r="K68" s="28" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="L68" s="28" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="M68" s="28"/>
       <c r="N68" s="28"/>
       <c r="O68" s="28" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="P68" s="28"/>
       <c r="Q68" s="37" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="R68" s="38" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="S68" s="38" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="T68" s="23">
         <v>64</v>
@@ -6590,13 +6602,13 @@
         <v>3</v>
       </c>
       <c r="C69" s="23" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="D69" s="23" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="E69" s="50" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="F69" s="26">
         <v>4</v>
@@ -6611,28 +6623,28 @@
         <v>0</v>
       </c>
       <c r="J69" s="27" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="K69" s="28" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="L69" s="28" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="M69" s="28"/>
       <c r="N69" s="28"/>
       <c r="O69" s="28" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="P69" s="28"/>
       <c r="Q69" s="29" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="R69" s="30" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="S69" s="30" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="T69" s="23">
         <v>65</v>
@@ -6643,10 +6655,10 @@
         <v>3</v>
       </c>
       <c r="C70" s="71" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="D70" s="71" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="E70" s="72"/>
       <c r="F70" s="73">
@@ -6663,25 +6675,25 @@
       </c>
       <c r="J70" s="74"/>
       <c r="K70" s="75" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="L70" s="75" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="M70" s="76"/>
       <c r="N70" s="76"/>
       <c r="O70" s="76" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="P70" s="76"/>
       <c r="Q70" s="77" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
       <c r="R70" s="78" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="S70" s="78" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="T70" s="71">
         <v>66</v>
@@ -6692,13 +6704,13 @@
         <v>3</v>
       </c>
       <c r="C71" s="66" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="D71" s="66" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="E71" s="67" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="F71" s="64">
         <v>1</v>
@@ -6714,25 +6726,25 @@
       </c>
       <c r="J71" s="61"/>
       <c r="K71" s="28" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="L71" s="28" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="M71" s="62"/>
       <c r="N71" s="62"/>
       <c r="O71" s="62" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="P71" s="62"/>
       <c r="Q71" s="68" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="R71" s="58" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="S71" s="58" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="T71" s="63">
         <v>67</v>
@@ -6743,13 +6755,13 @@
         <v>3</v>
       </c>
       <c r="C72" s="66" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="D72" s="66" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="E72" s="67" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="F72" s="64">
         <v>2</v>
@@ -6765,25 +6777,25 @@
       </c>
       <c r="J72" s="61"/>
       <c r="K72" s="28" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="L72" s="28" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="M72" s="62"/>
       <c r="N72" s="62"/>
       <c r="O72" s="62" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="P72" s="62"/>
       <c r="Q72" s="68" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="R72" s="58" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="S72" s="58" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="T72" s="63">
         <v>68</v>
@@ -6794,13 +6806,13 @@
         <v>3</v>
       </c>
       <c r="C73" s="66" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="D73" s="66" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="E73" s="67" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="F73" s="64">
         <v>3</v>
@@ -6816,25 +6828,25 @@
       </c>
       <c r="J73" s="61"/>
       <c r="K73" s="28" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="L73" s="28" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="M73" s="62"/>
       <c r="N73" s="62"/>
       <c r="O73" s="62" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
       <c r="P73" s="62"/>
       <c r="Q73" s="68" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="R73" s="58" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="S73" s="58" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="T73" s="63">
         <v>69</v>
@@ -6845,13 +6857,13 @@
         <v>3</v>
       </c>
       <c r="C74" s="80" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="D74" s="80" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="E74" s="81" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="F74" s="82">
         <v>4</v>
@@ -6867,25 +6879,25 @@
       </c>
       <c r="J74" s="83"/>
       <c r="K74" s="84" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="L74" s="84" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="M74" s="85"/>
       <c r="N74" s="85"/>
       <c r="O74" s="85" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
       <c r="P74" s="85"/>
       <c r="Q74" s="69" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="R74" s="38" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="S74" s="38" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="T74" s="80">
         <v>70</v>

</xml_diff>

<commit_message>
Fixing disguise 0 name
Former-commit-id: 8f1178957fd313907a65219e25e27e6fd26fb537
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -935,9 +935,6 @@
     <t>TID_DRAGON_REPTILE_2_DESC</t>
   </si>
   <si>
-    <t>TID_SKIN_FAT_0_NAME</t>
-  </si>
-  <si>
     <t>TID_DRAGON_FAT_0_DESC</t>
   </si>
   <si>
@@ -1473,6 +1470,9 @@
   </si>
   <si>
     <t>PF_tony_scientist_beard;PF_tony_scientist_belt;PF_tony_scientist_hat</t>
+  </si>
+  <si>
+    <t>TID_SKIN_TONY_0_NAME</t>
   </si>
 </sst>
 </file>
@@ -3260,8 +3260,8 @@
   </sheetPr>
   <dimension ref="B1:T74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" topLeftCell="H4" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3802,20 +3802,20 @@
       </c>
       <c r="J13" s="35"/>
       <c r="K13" s="36" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="L13" s="36" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="M13" s="36"/>
       <c r="N13" s="36"/>
       <c r="O13" s="28"/>
       <c r="P13" s="28"/>
       <c r="Q13" s="37" t="s">
+        <v>482</v>
+      </c>
+      <c r="R13" s="38" t="s">
         <v>303</v>
-      </c>
-      <c r="R13" s="38" t="s">
-        <v>304</v>
       </c>
       <c r="S13" s="38" t="s">
         <v>51</v>
@@ -3851,22 +3851,22 @@
       </c>
       <c r="J14" s="35"/>
       <c r="K14" s="36" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="L14" s="36" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="M14" s="36"/>
       <c r="N14" s="36"/>
       <c r="O14" s="28" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="P14" s="28"/>
       <c r="Q14" s="37" t="s">
+        <v>304</v>
+      </c>
+      <c r="R14" s="38" t="s">
         <v>305</v>
-      </c>
-      <c r="R14" s="38" t="s">
-        <v>306</v>
       </c>
       <c r="S14" s="38" t="s">
         <v>53</v>
@@ -3902,22 +3902,22 @@
       </c>
       <c r="J15" s="27"/>
       <c r="K15" s="28" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="L15" s="28" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="M15" s="28"/>
       <c r="N15" s="28"/>
       <c r="O15" s="28" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="P15" s="28"/>
       <c r="Q15" s="58" t="s">
+        <v>306</v>
+      </c>
+      <c r="R15" s="58" t="s">
         <v>307</v>
-      </c>
-      <c r="R15" s="58" t="s">
-        <v>308</v>
       </c>
       <c r="S15" s="58" t="s">
         <v>55</v>
@@ -3953,22 +3953,22 @@
       </c>
       <c r="J16" s="27"/>
       <c r="K16" s="28" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="L16" s="28" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="M16" s="28"/>
       <c r="N16" s="28"/>
       <c r="O16" s="28" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="P16" s="28"/>
       <c r="Q16" s="29" t="s">
+        <v>308</v>
+      </c>
+      <c r="R16" s="30" t="s">
         <v>309</v>
-      </c>
-      <c r="R16" s="30" t="s">
-        <v>310</v>
       </c>
       <c r="S16" s="30" t="s">
         <v>57</v>
@@ -4012,10 +4012,10 @@
       <c r="O17" s="20"/>
       <c r="P17" s="20"/>
       <c r="Q17" s="21" t="s">
+        <v>310</v>
+      </c>
+      <c r="R17" s="22" t="s">
         <v>311</v>
-      </c>
-      <c r="R17" s="22" t="s">
-        <v>312</v>
       </c>
       <c r="S17" s="22" t="s">
         <v>59</v>
@@ -4063,10 +4063,10 @@
       </c>
       <c r="P18" s="28"/>
       <c r="Q18" s="37" t="s">
+        <v>312</v>
+      </c>
+      <c r="R18" s="38" t="s">
         <v>313</v>
-      </c>
-      <c r="R18" s="38" t="s">
-        <v>314</v>
       </c>
       <c r="S18" s="38" t="s">
         <v>63</v>
@@ -4114,10 +4114,10 @@
       </c>
       <c r="P19" s="28"/>
       <c r="Q19" s="37" t="s">
+        <v>314</v>
+      </c>
+      <c r="R19" s="38" t="s">
         <v>315</v>
-      </c>
-      <c r="R19" s="38" t="s">
-        <v>316</v>
       </c>
       <c r="S19" s="38" t="s">
         <v>65</v>
@@ -4165,10 +4165,10 @@
       </c>
       <c r="P20" s="28"/>
       <c r="Q20" s="29" t="s">
+        <v>316</v>
+      </c>
+      <c r="R20" s="30" t="s">
         <v>317</v>
-      </c>
-      <c r="R20" s="30" t="s">
-        <v>318</v>
       </c>
       <c r="S20" s="30" t="s">
         <v>68</v>
@@ -4214,10 +4214,10 @@
       </c>
       <c r="P21" s="20"/>
       <c r="Q21" s="21" t="s">
+        <v>318</v>
+      </c>
+      <c r="R21" s="22" t="s">
         <v>319</v>
-      </c>
-      <c r="R21" s="22" t="s">
-        <v>320</v>
       </c>
       <c r="S21" s="22" t="s">
         <v>71</v>
@@ -4265,10 +4265,10 @@
       </c>
       <c r="P22" s="28"/>
       <c r="Q22" s="37" t="s">
+        <v>320</v>
+      </c>
+      <c r="R22" s="38" t="s">
         <v>321</v>
-      </c>
-      <c r="R22" s="38" t="s">
-        <v>322</v>
       </c>
       <c r="S22" s="38" t="s">
         <v>74</v>
@@ -4316,10 +4316,10 @@
       </c>
       <c r="P23" s="28"/>
       <c r="Q23" s="37" t="s">
+        <v>322</v>
+      </c>
+      <c r="R23" s="38" t="s">
         <v>323</v>
-      </c>
-      <c r="R23" s="38" t="s">
-        <v>324</v>
       </c>
       <c r="S23" s="38" t="s">
         <v>77</v>
@@ -4367,10 +4367,10 @@
       </c>
       <c r="P24" s="28"/>
       <c r="Q24" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="R24" s="30" t="s">
         <v>325</v>
-      </c>
-      <c r="R24" s="30" t="s">
-        <v>326</v>
       </c>
       <c r="S24" s="30" t="s">
         <v>80</v>
@@ -4414,10 +4414,10 @@
       <c r="O25" s="20"/>
       <c r="P25" s="20"/>
       <c r="Q25" s="21" t="s">
+        <v>326</v>
+      </c>
+      <c r="R25" s="22" t="s">
         <v>327</v>
-      </c>
-      <c r="R25" s="22" t="s">
-        <v>328</v>
       </c>
       <c r="S25" s="22" t="s">
         <v>82</v>
@@ -4465,10 +4465,10 @@
       </c>
       <c r="P26" s="28"/>
       <c r="Q26" s="37" t="s">
+        <v>328</v>
+      </c>
+      <c r="R26" s="38" t="s">
         <v>329</v>
-      </c>
-      <c r="R26" s="38" t="s">
-        <v>330</v>
       </c>
       <c r="S26" s="38" t="s">
         <v>85</v>
@@ -4516,10 +4516,10 @@
       </c>
       <c r="P27" s="28"/>
       <c r="Q27" s="37" t="s">
+        <v>330</v>
+      </c>
+      <c r="R27" s="38" t="s">
         <v>331</v>
-      </c>
-      <c r="R27" s="38" t="s">
-        <v>332</v>
       </c>
       <c r="S27" s="38" t="s">
         <v>88</v>
@@ -4567,10 +4567,10 @@
       </c>
       <c r="P28" s="28"/>
       <c r="Q28" s="37" t="s">
+        <v>332</v>
+      </c>
+      <c r="R28" s="38" t="s">
         <v>333</v>
-      </c>
-      <c r="R28" s="38" t="s">
-        <v>334</v>
       </c>
       <c r="S28" s="38" t="s">
         <v>91</v>
@@ -4618,10 +4618,10 @@
       </c>
       <c r="P29" s="28"/>
       <c r="Q29" s="58" t="s">
+        <v>334</v>
+      </c>
+      <c r="R29" s="58" t="s">
         <v>335</v>
-      </c>
-      <c r="R29" s="58" t="s">
-        <v>336</v>
       </c>
       <c r="S29" s="58" t="s">
         <v>94</v>
@@ -4672,7 +4672,7 @@
         <v>284</v>
       </c>
       <c r="R30" s="30" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="S30" s="30" t="s">
         <v>274</v>
@@ -4686,13 +4686,13 @@
         <v>3</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D31" s="23" t="s">
         <v>11</v>
       </c>
       <c r="E31" s="53" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F31" s="26">
         <v>6</v>
@@ -4705,28 +4705,28 @@
       </c>
       <c r="I31" s="27"/>
       <c r="J31" s="27" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="K31" s="28" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="L31" s="28" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="M31" s="28"/>
       <c r="N31" s="28"/>
       <c r="O31" s="28" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="P31" s="28"/>
       <c r="Q31" s="29" t="s">
+        <v>427</v>
+      </c>
+      <c r="R31" s="30" t="s">
         <v>428</v>
       </c>
-      <c r="R31" s="30" t="s">
-        <v>429</v>
-      </c>
       <c r="S31" s="30" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="T31" s="23">
         <v>27</v>
@@ -4769,10 +4769,10 @@
       </c>
       <c r="P32" s="20"/>
       <c r="Q32" s="21" t="s">
+        <v>337</v>
+      </c>
+      <c r="R32" s="22" t="s">
         <v>338</v>
-      </c>
-      <c r="R32" s="22" t="s">
-        <v>339</v>
       </c>
       <c r="S32" s="22" t="s">
         <v>97</v>
@@ -4820,10 +4820,10 @@
       </c>
       <c r="P33" s="28"/>
       <c r="Q33" s="37" t="s">
+        <v>339</v>
+      </c>
+      <c r="R33" s="38" t="s">
         <v>340</v>
-      </c>
-      <c r="R33" s="38" t="s">
-        <v>341</v>
       </c>
       <c r="S33" s="38" t="s">
         <v>100</v>
@@ -4871,10 +4871,10 @@
       </c>
       <c r="P34" s="28"/>
       <c r="Q34" s="37" t="s">
+        <v>341</v>
+      </c>
+      <c r="R34" s="38" t="s">
         <v>342</v>
-      </c>
-      <c r="R34" s="38" t="s">
-        <v>343</v>
       </c>
       <c r="S34" s="38" t="s">
         <v>104</v>
@@ -4922,10 +4922,10 @@
       </c>
       <c r="P35" s="28"/>
       <c r="Q35" s="37" t="s">
+        <v>343</v>
+      </c>
+      <c r="R35" s="38" t="s">
         <v>344</v>
-      </c>
-      <c r="R35" s="38" t="s">
-        <v>345</v>
       </c>
       <c r="S35" s="38" t="s">
         <v>106</v>
@@ -4973,10 +4973,10 @@
       </c>
       <c r="P36" s="43"/>
       <c r="Q36" s="44" t="s">
+        <v>345</v>
+      </c>
+      <c r="R36" s="45" t="s">
         <v>346</v>
-      </c>
-      <c r="R36" s="45" t="s">
-        <v>347</v>
       </c>
       <c r="S36" s="45" t="s">
         <v>109</v>
@@ -5271,10 +5271,10 @@
       <c r="O42" s="20"/>
       <c r="P42" s="20"/>
       <c r="Q42" s="21" t="s">
+        <v>347</v>
+      </c>
+      <c r="R42" s="22" t="s">
         <v>348</v>
-      </c>
-      <c r="R42" s="22" t="s">
-        <v>349</v>
       </c>
       <c r="S42" s="22" t="s">
         <v>111</v>
@@ -5322,10 +5322,10 @@
       </c>
       <c r="P43" s="28"/>
       <c r="Q43" s="37" t="s">
+        <v>349</v>
+      </c>
+      <c r="R43" s="38" t="s">
         <v>350</v>
-      </c>
-      <c r="R43" s="38" t="s">
-        <v>351</v>
       </c>
       <c r="S43" s="38" t="s">
         <v>113</v>
@@ -5373,10 +5373,10 @@
       </c>
       <c r="P44" s="28"/>
       <c r="Q44" s="37" t="s">
+        <v>351</v>
+      </c>
+      <c r="R44" s="38" t="s">
         <v>352</v>
-      </c>
-      <c r="R44" s="38" t="s">
-        <v>353</v>
       </c>
       <c r="S44" s="38" t="s">
         <v>115</v>
@@ -5426,10 +5426,10 @@
         <v>163</v>
       </c>
       <c r="Q45" s="37" t="s">
+        <v>353</v>
+      </c>
+      <c r="R45" s="38" t="s">
         <v>354</v>
-      </c>
-      <c r="R45" s="38" t="s">
-        <v>355</v>
       </c>
       <c r="S45" s="38" t="s">
         <v>117</v>
@@ -5475,10 +5475,10 @@
       <c r="O46" s="28"/>
       <c r="P46" s="28"/>
       <c r="Q46" s="37" t="s">
+        <v>355</v>
+      </c>
+      <c r="R46" s="38" t="s">
         <v>356</v>
-      </c>
-      <c r="R46" s="38" t="s">
-        <v>357</v>
       </c>
       <c r="S46" s="38" t="s">
         <v>119</v>
@@ -5529,7 +5529,7 @@
         <v>285</v>
       </c>
       <c r="R47" s="45" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="S47" s="45" t="s">
         <v>277</v>
@@ -5573,10 +5573,10 @@
       <c r="O48" s="20"/>
       <c r="P48" s="20"/>
       <c r="Q48" s="21" t="s">
+        <v>358</v>
+      </c>
+      <c r="R48" s="22" t="s">
         <v>359</v>
-      </c>
-      <c r="R48" s="22" t="s">
-        <v>360</v>
       </c>
       <c r="S48" s="22" t="s">
         <v>121</v>
@@ -5624,10 +5624,10 @@
       </c>
       <c r="P49" s="28"/>
       <c r="Q49" s="37" t="s">
+        <v>360</v>
+      </c>
+      <c r="R49" s="38" t="s">
         <v>361</v>
-      </c>
-      <c r="R49" s="38" t="s">
-        <v>362</v>
       </c>
       <c r="S49" s="38" t="s">
         <v>125</v>
@@ -5675,10 +5675,10 @@
       </c>
       <c r="P50" s="28"/>
       <c r="Q50" s="37" t="s">
+        <v>362</v>
+      </c>
+      <c r="R50" s="38" t="s">
         <v>363</v>
-      </c>
-      <c r="R50" s="38" t="s">
-        <v>364</v>
       </c>
       <c r="S50" s="38" t="s">
         <v>127</v>
@@ -5726,10 +5726,10 @@
       </c>
       <c r="P51" s="28"/>
       <c r="Q51" s="37" t="s">
+        <v>364</v>
+      </c>
+      <c r="R51" s="38" t="s">
         <v>365</v>
-      </c>
-      <c r="R51" s="38" t="s">
-        <v>366</v>
       </c>
       <c r="S51" s="38" t="s">
         <v>130</v>
@@ -5777,10 +5777,10 @@
       </c>
       <c r="P52" s="28"/>
       <c r="Q52" s="37" t="s">
+        <v>366</v>
+      </c>
+      <c r="R52" s="38" t="s">
         <v>367</v>
-      </c>
-      <c r="R52" s="38" t="s">
-        <v>368</v>
       </c>
       <c r="S52" s="38" t="s">
         <v>133</v>
@@ -5831,7 +5831,7 @@
         <v>286</v>
       </c>
       <c r="R53" s="38" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="S53" s="38" t="s">
         <v>280</v>
@@ -5875,10 +5875,10 @@
       <c r="O54" s="20"/>
       <c r="P54" s="20"/>
       <c r="Q54" s="21" t="s">
+        <v>369</v>
+      </c>
+      <c r="R54" s="22" t="s">
         <v>370</v>
-      </c>
-      <c r="R54" s="22" t="s">
-        <v>371</v>
       </c>
       <c r="S54" s="22" t="s">
         <v>173</v>
@@ -5926,10 +5926,10 @@
       </c>
       <c r="P55" s="28"/>
       <c r="Q55" s="37" t="s">
+        <v>371</v>
+      </c>
+      <c r="R55" s="38" t="s">
         <v>372</v>
-      </c>
-      <c r="R55" s="38" t="s">
-        <v>373</v>
       </c>
       <c r="S55" s="38" t="s">
         <v>174</v>
@@ -5977,10 +5977,10 @@
       </c>
       <c r="P56" s="28"/>
       <c r="Q56" s="37" t="s">
+        <v>373</v>
+      </c>
+      <c r="R56" s="38" t="s">
         <v>374</v>
-      </c>
-      <c r="R56" s="38" t="s">
-        <v>375</v>
       </c>
       <c r="S56" s="38" t="s">
         <v>175</v>
@@ -6028,10 +6028,10 @@
       </c>
       <c r="P57" s="28"/>
       <c r="Q57" s="37" t="s">
+        <v>375</v>
+      </c>
+      <c r="R57" s="38" t="s">
         <v>376</v>
-      </c>
-      <c r="R57" s="38" t="s">
-        <v>377</v>
       </c>
       <c r="S57" s="38" t="s">
         <v>176</v>
@@ -6079,10 +6079,10 @@
       </c>
       <c r="P58" s="28"/>
       <c r="Q58" s="37" t="s">
+        <v>377</v>
+      </c>
+      <c r="R58" s="38" t="s">
         <v>378</v>
-      </c>
-      <c r="R58" s="38" t="s">
-        <v>379</v>
       </c>
       <c r="S58" s="38" t="s">
         <v>177</v>
@@ -6128,10 +6128,10 @@
       </c>
       <c r="P59" s="20"/>
       <c r="Q59" s="21" t="s">
+        <v>379</v>
+      </c>
+      <c r="R59" s="22" t="s">
         <v>380</v>
-      </c>
-      <c r="R59" s="22" t="s">
-        <v>381</v>
       </c>
       <c r="S59" s="22" t="s">
         <v>259</v>
@@ -6179,10 +6179,10 @@
       </c>
       <c r="P60" s="28"/>
       <c r="Q60" s="37" t="s">
+        <v>381</v>
+      </c>
+      <c r="R60" s="38" t="s">
         <v>382</v>
-      </c>
-      <c r="R60" s="38" t="s">
-        <v>383</v>
       </c>
       <c r="S60" s="38" t="s">
         <v>260</v>
@@ -6230,10 +6230,10 @@
       </c>
       <c r="P61" s="28"/>
       <c r="Q61" s="37" t="s">
+        <v>383</v>
+      </c>
+      <c r="R61" s="38" t="s">
         <v>384</v>
-      </c>
-      <c r="R61" s="38" t="s">
-        <v>385</v>
       </c>
       <c r="S61" s="38" t="s">
         <v>261</v>
@@ -6281,10 +6281,10 @@
       </c>
       <c r="P62" s="28"/>
       <c r="Q62" s="37" t="s">
+        <v>385</v>
+      </c>
+      <c r="R62" s="38" t="s">
         <v>386</v>
-      </c>
-      <c r="R62" s="38" t="s">
-        <v>387</v>
       </c>
       <c r="S62" s="38" t="s">
         <v>262</v>
@@ -6332,10 +6332,10 @@
       </c>
       <c r="P63" s="28"/>
       <c r="Q63" s="37" t="s">
+        <v>387</v>
+      </c>
+      <c r="R63" s="38" t="s">
         <v>388</v>
-      </c>
-      <c r="R63" s="38" t="s">
-        <v>389</v>
       </c>
       <c r="S63" s="38" t="s">
         <v>262</v>
@@ -6349,13 +6349,13 @@
         <v>3</v>
       </c>
       <c r="C64" s="32" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D64" s="32" t="s">
         <v>227</v>
       </c>
       <c r="E64" s="54" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F64" s="34">
         <v>5</v>
@@ -6368,30 +6368,30 @@
       </c>
       <c r="I64" s="42"/>
       <c r="J64" s="42" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="K64" s="28" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="L64" s="28" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="M64" s="28"/>
       <c r="N64" s="28"/>
       <c r="O64" s="28" t="s">
+        <v>435</v>
+      </c>
+      <c r="P64" s="28" t="s">
         <v>436</v>
       </c>
-      <c r="P64" s="28" t="s">
-        <v>437</v>
-      </c>
       <c r="Q64" s="37" t="s">
+        <v>432</v>
+      </c>
+      <c r="R64" s="38" t="s">
         <v>433</v>
       </c>
-      <c r="R64" s="38" t="s">
+      <c r="S64" s="38" t="s">
         <v>434</v>
-      </c>
-      <c r="S64" s="38" t="s">
-        <v>435</v>
       </c>
       <c r="T64" s="23">
         <v>60</v>
@@ -6402,10 +6402,10 @@
         <v>3</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D65" s="15" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E65" s="50"/>
       <c r="F65" s="17">
@@ -6422,23 +6422,23 @@
       </c>
       <c r="J65" s="47"/>
       <c r="K65" s="19" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L65" s="19" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="M65" s="19"/>
       <c r="N65" s="19"/>
       <c r="O65" s="20"/>
       <c r="P65" s="20"/>
       <c r="Q65" s="21" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="R65" s="22" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="S65" s="22" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="T65" s="23">
         <v>61</v>
@@ -6449,10 +6449,10 @@
         <v>3</v>
       </c>
       <c r="C66" s="32" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D66" s="32" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E66" s="48" t="s">
         <v>236</v>
@@ -6471,25 +6471,25 @@
       </c>
       <c r="J66" s="35"/>
       <c r="K66" s="36" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="L66" s="36" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="M66" s="36"/>
       <c r="N66" s="36"/>
       <c r="O66" s="28" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="P66" s="28"/>
       <c r="Q66" s="37" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="R66" s="38" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="S66" s="38" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="T66" s="23">
         <v>62</v>
@@ -6500,13 +6500,13 @@
         <v>3</v>
       </c>
       <c r="C67" s="32" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D67" s="32" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E67" s="50" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F67" s="34">
         <v>2</v>
@@ -6522,25 +6522,25 @@
       </c>
       <c r="J67" s="35"/>
       <c r="K67" s="36" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="L67" s="36" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="M67" s="36"/>
       <c r="N67" s="36"/>
       <c r="O67" s="28" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="P67" s="28"/>
       <c r="Q67" s="37" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="R67" s="38" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="S67" s="38" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="T67" s="23">
         <v>63</v>
@@ -6551,13 +6551,13 @@
         <v>3</v>
       </c>
       <c r="C68" s="32" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D68" s="32" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E68" s="50" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F68" s="34">
         <v>3</v>
@@ -6573,25 +6573,25 @@
       </c>
       <c r="J68" s="27"/>
       <c r="K68" s="28" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="L68" s="28" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="M68" s="28"/>
       <c r="N68" s="28"/>
       <c r="O68" s="28" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="P68" s="28"/>
       <c r="Q68" s="37" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="R68" s="38" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="S68" s="38" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="T68" s="23">
         <v>64</v>
@@ -6602,10 +6602,10 @@
         <v>3</v>
       </c>
       <c r="C69" s="23" t="s">
+        <v>393</v>
+      </c>
+      <c r="D69" s="23" t="s">
         <v>394</v>
-      </c>
-      <c r="D69" s="23" t="s">
-        <v>395</v>
       </c>
       <c r="E69" s="50" t="s">
         <v>239</v>
@@ -6623,28 +6623,28 @@
         <v>0</v>
       </c>
       <c r="J69" s="27" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="K69" s="28" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="L69" s="28" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="M69" s="28"/>
       <c r="N69" s="28"/>
       <c r="O69" s="28" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="P69" s="28"/>
       <c r="Q69" s="29" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="R69" s="30" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="S69" s="30" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="T69" s="23">
         <v>65</v>
@@ -6655,10 +6655,10 @@
         <v>3</v>
       </c>
       <c r="C70" s="71" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D70" s="71" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E70" s="72"/>
       <c r="F70" s="73">
@@ -6675,25 +6675,25 @@
       </c>
       <c r="J70" s="74"/>
       <c r="K70" s="75" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="L70" s="75" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="M70" s="76"/>
       <c r="N70" s="76"/>
       <c r="O70" s="76" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="P70" s="76"/>
       <c r="Q70" s="77" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="R70" s="78" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="S70" s="78" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="T70" s="71">
         <v>66</v>
@@ -6704,13 +6704,13 @@
         <v>3</v>
       </c>
       <c r="C71" s="66" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D71" s="66" t="s">
+        <v>443</v>
+      </c>
+      <c r="E71" s="67" t="s">
         <v>444</v>
-      </c>
-      <c r="E71" s="67" t="s">
-        <v>445</v>
       </c>
       <c r="F71" s="64">
         <v>1</v>
@@ -6726,25 +6726,25 @@
       </c>
       <c r="J71" s="61"/>
       <c r="K71" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="L71" s="28" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="M71" s="62"/>
       <c r="N71" s="62"/>
       <c r="O71" s="62" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="P71" s="62"/>
       <c r="Q71" s="68" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="R71" s="58" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="S71" s="58" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="T71" s="63">
         <v>67</v>
@@ -6755,10 +6755,10 @@
         <v>3</v>
       </c>
       <c r="C72" s="66" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D72" s="66" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E72" s="67" t="s">
         <v>247</v>
@@ -6777,25 +6777,25 @@
       </c>
       <c r="J72" s="61"/>
       <c r="K72" s="28" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="L72" s="28" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="M72" s="62"/>
       <c r="N72" s="62"/>
       <c r="O72" s="62" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="P72" s="62"/>
       <c r="Q72" s="68" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="R72" s="58" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="S72" s="58" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="T72" s="63">
         <v>68</v>
@@ -6806,13 +6806,13 @@
         <v>3</v>
       </c>
       <c r="C73" s="66" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D73" s="66" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E73" s="67" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F73" s="64">
         <v>3</v>
@@ -6828,25 +6828,25 @@
       </c>
       <c r="J73" s="61"/>
       <c r="K73" s="28" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="L73" s="28" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="M73" s="62"/>
       <c r="N73" s="62"/>
       <c r="O73" s="62" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="P73" s="62"/>
       <c r="Q73" s="68" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="R73" s="58" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="S73" s="58" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="T73" s="63">
         <v>69</v>
@@ -6857,13 +6857,13 @@
         <v>3</v>
       </c>
       <c r="C74" s="80" t="s">
+        <v>442</v>
+      </c>
+      <c r="D74" s="80" t="s">
         <v>443</v>
       </c>
-      <c r="D74" s="80" t="s">
-        <v>444</v>
-      </c>
       <c r="E74" s="81" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F74" s="82">
         <v>4</v>
@@ -6879,25 +6879,25 @@
       </c>
       <c r="J74" s="83"/>
       <c r="K74" s="84" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="L74" s="84" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="M74" s="85"/>
       <c r="N74" s="85"/>
       <c r="O74" s="85" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="P74" s="85"/>
       <c r="Q74" s="69" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="R74" s="38" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="S74" s="38" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="T74" s="80">
         <v>70</v>

</xml_diff>

<commit_message>
WIP adding dragon light to content (not final values)
Former-commit-id: 99c0ec347ad7156df4f2afadc045f85ebfc7192a
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="509">
   <si>
     <t>[sku]</t>
   </si>
@@ -1476,13 +1476,88 @@
   </si>
   <si>
     <t>dragon_light_0</t>
+  </si>
+  <si>
+    <t>dragon_light_1</t>
+  </si>
+  <si>
+    <t>dragon_light_2</t>
+  </si>
+  <si>
+    <t>dragon_light_3</t>
+  </si>
+  <si>
+    <t>dragon_light_4</t>
+  </si>
+  <si>
+    <t>dragon_light</t>
+  </si>
+  <si>
+    <t>icon_light_0</t>
+  </si>
+  <si>
+    <t>icon_light_1</t>
+  </si>
+  <si>
+    <t>icon_light_2</t>
+  </si>
+  <si>
+    <t>icon_light_3</t>
+  </si>
+  <si>
+    <t>icon_light_4</t>
+  </si>
+  <si>
+    <t>TID_SKIN_LIGHT_0_NAME</t>
+  </si>
+  <si>
+    <t>TID_SKIN_LIGHT_1_NAME</t>
+  </si>
+  <si>
+    <t>TID_SKIN_LIGHT_2_NAME</t>
+  </si>
+  <si>
+    <t>TID_SKIN_LIGHT_3_NAME</t>
+  </si>
+  <si>
+    <t>TID_SKIN_LIGHT_4_NAME</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_LIGHT_0_DESC</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_LIGHT_1_DESC</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_LIGHT_2_DESC</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_LIGHT_3_DESC</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_LIGHT_4_DESC</t>
+  </si>
+  <si>
+    <t>lightdragon_default</t>
+  </si>
+  <si>
+    <t>lightdragon_skin_1</t>
+  </si>
+  <si>
+    <t>lightdragon_skin_2</t>
+  </si>
+  <si>
+    <t>lightdragon_skin_3</t>
+  </si>
+  <si>
+    <t>lightdragon_skin_4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1537,6 +1612,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1620,7 +1703,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1876,28 +1959,6 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -1922,7 +1983,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
@@ -2129,42 +2190,15 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2175,6 +2209,51 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2965,8 +3044,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="disguisesDefinitions6" displayName="disguisesDefinitions6" ref="B4:T74" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19">
-  <autoFilter ref="B4:T74"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="disguisesDefinitions6" displayName="disguisesDefinitions6" ref="B4:T79" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19">
+  <autoFilter ref="B4:T79"/>
   <sortState ref="B5:T46">
     <sortCondition ref="T4:T46"/>
   </sortState>
@@ -3261,10 +3340,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="B1:T74"/>
+  <dimension ref="B1:T79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="L71" sqref="L71"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6600,53 +6679,53 @@
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B69" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C69" s="23" t="s">
+    <row r="69" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C69" s="40" t="s">
         <v>393</v>
       </c>
-      <c r="D69" s="23" t="s">
+      <c r="D69" s="40" t="s">
         <v>394</v>
       </c>
-      <c r="E69" s="50" t="s">
+      <c r="E69" s="54" t="s">
         <v>239</v>
       </c>
-      <c r="F69" s="26">
+      <c r="F69" s="41">
         <v>4</v>
       </c>
-      <c r="G69" s="27">
-        <v>0</v>
-      </c>
-      <c r="H69" s="27">
+      <c r="G69" s="42">
+        <v>0</v>
+      </c>
+      <c r="H69" s="42">
         <v>65</v>
       </c>
-      <c r="I69" s="47">
-        <v>0</v>
-      </c>
-      <c r="J69" s="27" t="s">
+      <c r="I69" s="85">
+        <v>0</v>
+      </c>
+      <c r="J69" s="42" t="s">
         <v>415</v>
       </c>
-      <c r="K69" s="28" t="s">
+      <c r="K69" s="43" t="s">
         <v>399</v>
       </c>
-      <c r="L69" s="28" t="s">
+      <c r="L69" s="43" t="s">
         <v>393</v>
       </c>
-      <c r="M69" s="28"/>
-      <c r="N69" s="28"/>
-      <c r="O69" s="28" t="s">
+      <c r="M69" s="43"/>
+      <c r="N69" s="43"/>
+      <c r="O69" s="43" t="s">
         <v>420</v>
       </c>
-      <c r="P69" s="28"/>
-      <c r="Q69" s="29" t="s">
+      <c r="P69" s="43"/>
+      <c r="Q69" s="44" t="s">
         <v>404</v>
       </c>
-      <c r="R69" s="30" t="s">
+      <c r="R69" s="45" t="s">
         <v>409</v>
       </c>
-      <c r="S69" s="30" t="s">
+      <c r="S69" s="44" t="s">
         <v>414</v>
       </c>
       <c r="T69" s="23">
@@ -6654,51 +6733,51 @@
       </c>
     </row>
     <row r="70" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B70" s="70" t="s">
-        <v>3</v>
-      </c>
-      <c r="C70" s="71" t="s">
+      <c r="B70" s="83" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70" s="78" t="s">
         <v>438</v>
       </c>
-      <c r="D70" s="71" t="s">
+      <c r="D70" s="78" t="s">
         <v>443</v>
       </c>
-      <c r="E70" s="72"/>
-      <c r="F70" s="73">
-        <v>0</v>
-      </c>
-      <c r="G70" s="74">
-        <v>0</v>
-      </c>
-      <c r="H70" s="74">
-        <v>0</v>
-      </c>
-      <c r="I70" s="74">
-        <v>0</v>
-      </c>
-      <c r="J70" s="74"/>
-      <c r="K70" s="75" t="s">
+      <c r="E70" s="77"/>
+      <c r="F70" s="64">
+        <v>0</v>
+      </c>
+      <c r="G70" s="61">
+        <v>0</v>
+      </c>
+      <c r="H70" s="61">
+        <v>0</v>
+      </c>
+      <c r="I70" s="61">
+        <v>0</v>
+      </c>
+      <c r="J70" s="61"/>
+      <c r="K70" s="28" t="s">
         <v>446</v>
       </c>
-      <c r="L70" s="75" t="s">
+      <c r="L70" s="28" t="s">
         <v>483</v>
       </c>
-      <c r="M70" s="76"/>
-      <c r="N70" s="76"/>
-      <c r="O70" s="76" t="s">
+      <c r="M70" s="62"/>
+      <c r="N70" s="62"/>
+      <c r="O70" s="62" t="s">
         <v>466</v>
       </c>
-      <c r="P70" s="76"/>
-      <c r="Q70" s="77" t="s">
+      <c r="P70" s="62"/>
+      <c r="Q70" s="84" t="s">
         <v>451</v>
       </c>
-      <c r="R70" s="78" t="s">
+      <c r="R70" s="30" t="s">
         <v>456</v>
       </c>
-      <c r="S70" s="78" t="s">
+      <c r="S70" s="30" t="s">
         <v>461</v>
       </c>
-      <c r="T70" s="71">
+      <c r="T70" s="70">
         <v>66</v>
       </c>
     </row>
@@ -6855,55 +6934,298 @@
         <v>69</v>
       </c>
     </row>
-    <row r="74" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B74" s="79" t="s">
-        <v>3</v>
-      </c>
-      <c r="C74" s="80" t="s">
+    <row r="74" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="86" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74" s="87" t="s">
         <v>442</v>
       </c>
-      <c r="D74" s="80" t="s">
+      <c r="D74" s="87" t="s">
         <v>443</v>
       </c>
-      <c r="E74" s="81" t="s">
+      <c r="E74" s="54" t="s">
         <v>445</v>
       </c>
-      <c r="F74" s="82">
+      <c r="F74" s="88">
         <v>4</v>
       </c>
-      <c r="G74" s="83">
-        <v>0</v>
-      </c>
-      <c r="H74" s="83">
+      <c r="G74" s="89">
+        <v>0</v>
+      </c>
+      <c r="H74" s="89">
         <v>70</v>
       </c>
-      <c r="I74" s="83">
+      <c r="I74" s="89">
         <v>10</v>
       </c>
-      <c r="J74" s="83"/>
-      <c r="K74" s="84" t="s">
+      <c r="J74" s="89"/>
+      <c r="K74" s="43" t="s">
         <v>450</v>
       </c>
-      <c r="L74" s="84" t="s">
+      <c r="L74" s="43" t="s">
         <v>442</v>
       </c>
-      <c r="M74" s="85"/>
-      <c r="N74" s="85"/>
-      <c r="O74" s="85" t="s">
+      <c r="M74" s="90"/>
+      <c r="N74" s="90"/>
+      <c r="O74" s="90" t="s">
         <v>470</v>
       </c>
-      <c r="P74" s="85"/>
-      <c r="Q74" s="69" t="s">
+      <c r="P74" s="90"/>
+      <c r="Q74" s="91" t="s">
         <v>455</v>
       </c>
-      <c r="R74" s="38" t="s">
+      <c r="R74" s="45" t="s">
         <v>460</v>
       </c>
-      <c r="S74" s="38" t="s">
+      <c r="S74" s="44" t="s">
         <v>465</v>
       </c>
-      <c r="T74" s="80">
+      <c r="T74" s="72">
         <v>70</v>
+      </c>
+    </row>
+    <row r="75" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B75" s="83" t="s">
+        <v>3</v>
+      </c>
+      <c r="C75" s="78" t="s">
+        <v>483</v>
+      </c>
+      <c r="D75" s="78" t="s">
+        <v>488</v>
+      </c>
+      <c r="E75" s="77"/>
+      <c r="F75" s="64">
+        <v>0</v>
+      </c>
+      <c r="G75" s="61">
+        <v>0</v>
+      </c>
+      <c r="H75" s="61">
+        <v>0</v>
+      </c>
+      <c r="I75" s="61">
+        <v>0</v>
+      </c>
+      <c r="J75" s="61"/>
+      <c r="K75" s="28" t="s">
+        <v>489</v>
+      </c>
+      <c r="L75" s="28" t="s">
+        <v>483</v>
+      </c>
+      <c r="M75" s="62"/>
+      <c r="N75" s="62"/>
+      <c r="O75" s="62"/>
+      <c r="P75" s="62"/>
+      <c r="Q75" s="84" t="s">
+        <v>494</v>
+      </c>
+      <c r="R75" s="30" t="s">
+        <v>499</v>
+      </c>
+      <c r="S75" s="30" t="s">
+        <v>504</v>
+      </c>
+      <c r="T75" s="70">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="76" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B76" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="C76" s="66" t="s">
+        <v>484</v>
+      </c>
+      <c r="D76" s="66" t="s">
+        <v>488</v>
+      </c>
+      <c r="E76" s="79" t="s">
+        <v>444</v>
+      </c>
+      <c r="F76" s="64">
+        <v>1</v>
+      </c>
+      <c r="G76" s="81">
+        <v>500000</v>
+      </c>
+      <c r="H76" s="81">
+        <v>0</v>
+      </c>
+      <c r="I76" s="81">
+        <v>1</v>
+      </c>
+      <c r="J76" s="61"/>
+      <c r="K76" s="28" t="s">
+        <v>490</v>
+      </c>
+      <c r="L76" s="28" t="s">
+        <v>484</v>
+      </c>
+      <c r="M76" s="62"/>
+      <c r="N76" s="62"/>
+      <c r="O76" s="62"/>
+      <c r="P76" s="62"/>
+      <c r="Q76" s="68" t="s">
+        <v>495</v>
+      </c>
+      <c r="R76" s="58" t="s">
+        <v>500</v>
+      </c>
+      <c r="S76" s="58" t="s">
+        <v>505</v>
+      </c>
+      <c r="T76" s="63">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="77" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B77" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="C77" s="66" t="s">
+        <v>485</v>
+      </c>
+      <c r="D77" s="66" t="s">
+        <v>488</v>
+      </c>
+      <c r="E77" s="79" t="s">
+        <v>247</v>
+      </c>
+      <c r="F77" s="64">
+        <v>2</v>
+      </c>
+      <c r="G77" s="81">
+        <v>500000</v>
+      </c>
+      <c r="H77" s="81">
+        <v>0</v>
+      </c>
+      <c r="I77" s="81">
+        <v>4</v>
+      </c>
+      <c r="J77" s="61"/>
+      <c r="K77" s="28" t="s">
+        <v>491</v>
+      </c>
+      <c r="L77" s="28" t="s">
+        <v>485</v>
+      </c>
+      <c r="M77" s="62"/>
+      <c r="N77" s="62"/>
+      <c r="O77" s="62"/>
+      <c r="P77" s="62"/>
+      <c r="Q77" s="68" t="s">
+        <v>496</v>
+      </c>
+      <c r="R77" s="58" t="s">
+        <v>501</v>
+      </c>
+      <c r="S77" s="58" t="s">
+        <v>506</v>
+      </c>
+      <c r="T77" s="63">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="78" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B78" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="C78" s="66" t="s">
+        <v>486</v>
+      </c>
+      <c r="D78" s="66" t="s">
+        <v>488</v>
+      </c>
+      <c r="E78" s="79" t="s">
+        <v>423</v>
+      </c>
+      <c r="F78" s="64">
+        <v>3</v>
+      </c>
+      <c r="G78" s="81">
+        <v>0</v>
+      </c>
+      <c r="H78" s="81">
+        <v>55</v>
+      </c>
+      <c r="I78" s="81">
+        <v>7</v>
+      </c>
+      <c r="J78" s="61"/>
+      <c r="K78" s="28" t="s">
+        <v>492</v>
+      </c>
+      <c r="L78" s="28" t="s">
+        <v>486</v>
+      </c>
+      <c r="M78" s="62"/>
+      <c r="N78" s="62"/>
+      <c r="O78" s="62"/>
+      <c r="P78" s="62"/>
+      <c r="Q78" s="68" t="s">
+        <v>497</v>
+      </c>
+      <c r="R78" s="58" t="s">
+        <v>502</v>
+      </c>
+      <c r="S78" s="58" t="s">
+        <v>507</v>
+      </c>
+      <c r="T78" s="63">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="79" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B79" s="71" t="s">
+        <v>3</v>
+      </c>
+      <c r="C79" s="72" t="s">
+        <v>487</v>
+      </c>
+      <c r="D79" s="72" t="s">
+        <v>488</v>
+      </c>
+      <c r="E79" s="80" t="s">
+        <v>445</v>
+      </c>
+      <c r="F79" s="73">
+        <v>4</v>
+      </c>
+      <c r="G79" s="82">
+        <v>0</v>
+      </c>
+      <c r="H79" s="82">
+        <v>70</v>
+      </c>
+      <c r="I79" s="82">
+        <v>10</v>
+      </c>
+      <c r="J79" s="74"/>
+      <c r="K79" s="75" t="s">
+        <v>493</v>
+      </c>
+      <c r="L79" s="75" t="s">
+        <v>487</v>
+      </c>
+      <c r="M79" s="76"/>
+      <c r="N79" s="76"/>
+      <c r="O79" s="76"/>
+      <c r="P79" s="76"/>
+      <c r="Q79" s="69" t="s">
+        <v>498</v>
+      </c>
+      <c r="R79" s="38" t="s">
+        <v>503</v>
+      </c>
+      <c r="S79" s="38" t="s">
+        <v>508</v>
+      </c>
+      <c r="T79" s="72">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WIP Adding dragon light to menu
Former-commit-id: f5b8f43244581c69f501593ffbf57a9dc331ebac
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -3343,7 +3343,7 @@
   <dimension ref="B1:T79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E82" sqref="E82"/>
+      <selection activeCell="L70" sqref="L70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6760,7 +6760,7 @@
         <v>446</v>
       </c>
       <c r="L70" s="28" t="s">
-        <v>483</v>
+        <v>438</v>
       </c>
       <c r="M70" s="62"/>
       <c r="N70" s="62"/>

</xml_diff>

<commit_message>
Light dragon statsm Skins powerups and new Powerup disguise_furyDuration_hp_transform_gold
Former-commit-id: 055e88aa594ac50159994ffb7f754902591c9416
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="510">
   <si>
     <t>[sku]</t>
   </si>
@@ -1551,6 +1551,9 @@
   </si>
   <si>
     <t>lightdragon_skin_4</t>
+  </si>
+  <si>
+    <t>disguise_furyDuration_hp_transform_gold</t>
   </si>
 </sst>
 </file>
@@ -1703,7 +1706,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -1979,11 +1982,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
@@ -2217,12 +2235,6 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2254,6 +2266,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3342,8 +3363,8 @@
   </sheetPr>
   <dimension ref="B1:T79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="L70" sqref="L70"/>
+    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
+      <selection activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6701,7 +6722,7 @@
       <c r="H69" s="42">
         <v>65</v>
       </c>
-      <c r="I69" s="85">
+      <c r="I69" s="83">
         <v>0</v>
       </c>
       <c r="J69" s="42" t="s">
@@ -6733,7 +6754,7 @@
       </c>
     </row>
     <row r="70" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B70" s="83" t="s">
+      <c r="B70" s="81" t="s">
         <v>3</v>
       </c>
       <c r="C70" s="78" t="s">
@@ -6768,7 +6789,7 @@
         <v>466</v>
       </c>
       <c r="P70" s="62"/>
-      <c r="Q70" s="84" t="s">
+      <c r="Q70" s="82" t="s">
         <v>451</v>
       </c>
       <c r="R70" s="30" t="s">
@@ -6935,44 +6956,44 @@
       </c>
     </row>
     <row r="74" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="86" t="s">
-        <v>3</v>
-      </c>
-      <c r="C74" s="87" t="s">
+      <c r="B74" s="84" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74" s="85" t="s">
         <v>442</v>
       </c>
-      <c r="D74" s="87" t="s">
+      <c r="D74" s="85" t="s">
         <v>443</v>
       </c>
       <c r="E74" s="54" t="s">
         <v>445</v>
       </c>
-      <c r="F74" s="88">
+      <c r="F74" s="86">
         <v>4</v>
       </c>
-      <c r="G74" s="89">
-        <v>0</v>
-      </c>
-      <c r="H74" s="89">
+      <c r="G74" s="87">
+        <v>0</v>
+      </c>
+      <c r="H74" s="87">
         <v>70</v>
       </c>
-      <c r="I74" s="89">
+      <c r="I74" s="87">
         <v>10</v>
       </c>
-      <c r="J74" s="89"/>
+      <c r="J74" s="87"/>
       <c r="K74" s="43" t="s">
         <v>450</v>
       </c>
       <c r="L74" s="43" t="s">
         <v>442</v>
       </c>
-      <c r="M74" s="90"/>
-      <c r="N74" s="90"/>
-      <c r="O74" s="90" t="s">
+      <c r="M74" s="88"/>
+      <c r="N74" s="88"/>
+      <c r="O74" s="88" t="s">
         <v>470</v>
       </c>
-      <c r="P74" s="90"/>
-      <c r="Q74" s="91" t="s">
+      <c r="P74" s="88"/>
+      <c r="Q74" s="89" t="s">
         <v>455</v>
       </c>
       <c r="R74" s="45" t="s">
@@ -6986,7 +7007,7 @@
       </c>
     </row>
     <row r="75" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B75" s="83" t="s">
+      <c r="B75" s="81" t="s">
         <v>3</v>
       </c>
       <c r="C75" s="78" t="s">
@@ -7019,7 +7040,7 @@
       <c r="N75" s="62"/>
       <c r="O75" s="62"/>
       <c r="P75" s="62"/>
-      <c r="Q75" s="84" t="s">
+      <c r="Q75" s="82" t="s">
         <v>494</v>
       </c>
       <c r="R75" s="30" t="s">
@@ -7042,19 +7063,19 @@
       <c r="D76" s="66" t="s">
         <v>488</v>
       </c>
-      <c r="E76" s="79" t="s">
-        <v>444</v>
+      <c r="E76" s="90" t="s">
+        <v>247</v>
       </c>
       <c r="F76" s="64">
         <v>1</v>
       </c>
-      <c r="G76" s="81">
+      <c r="G76" s="79">
         <v>500000</v>
       </c>
-      <c r="H76" s="81">
-        <v>0</v>
-      </c>
-      <c r="I76" s="81">
+      <c r="H76" s="79">
+        <v>0</v>
+      </c>
+      <c r="I76" s="79">
         <v>1</v>
       </c>
       <c r="J76" s="61"/>
@@ -7091,19 +7112,19 @@
       <c r="D77" s="66" t="s">
         <v>488</v>
       </c>
-      <c r="E77" s="79" t="s">
-        <v>247</v>
+      <c r="E77" s="91" t="s">
+        <v>248</v>
       </c>
       <c r="F77" s="64">
         <v>2</v>
       </c>
-      <c r="G77" s="81">
+      <c r="G77" s="79">
         <v>500000</v>
       </c>
-      <c r="H77" s="81">
-        <v>0</v>
-      </c>
-      <c r="I77" s="81">
+      <c r="H77" s="79">
+        <v>0</v>
+      </c>
+      <c r="I77" s="79">
         <v>4</v>
       </c>
       <c r="J77" s="61"/>
@@ -7140,19 +7161,19 @@
       <c r="D78" s="66" t="s">
         <v>488</v>
       </c>
-      <c r="E78" s="79" t="s">
-        <v>423</v>
+      <c r="E78" s="91" t="s">
+        <v>430</v>
       </c>
       <c r="F78" s="64">
         <v>3</v>
       </c>
-      <c r="G78" s="81">
-        <v>0</v>
-      </c>
-      <c r="H78" s="81">
-        <v>55</v>
-      </c>
-      <c r="I78" s="81">
+      <c r="G78" s="79">
+        <v>0</v>
+      </c>
+      <c r="H78" s="79">
+        <v>60</v>
+      </c>
+      <c r="I78" s="79">
         <v>7</v>
       </c>
       <c r="J78" s="61"/>
@@ -7189,19 +7210,19 @@
       <c r="D79" s="72" t="s">
         <v>488</v>
       </c>
-      <c r="E79" s="80" t="s">
-        <v>445</v>
+      <c r="E79" s="92" t="s">
+        <v>509</v>
       </c>
       <c r="F79" s="73">
         <v>4</v>
       </c>
-      <c r="G79" s="82">
-        <v>0</v>
-      </c>
-      <c r="H79" s="82">
-        <v>70</v>
-      </c>
-      <c r="I79" s="82">
+      <c r="G79" s="80">
+        <v>0</v>
+      </c>
+      <c r="H79" s="80">
+        <v>75</v>
+      </c>
+      <c r="I79" s="80">
         <v>10</v>
       </c>
       <c r="J79" s="74"/>

</xml_diff>

<commit_message>
Light dragon stats Skins powerups and new Powerup disguise_furyDuration_hp_transform_gold_LOW
Former-commit-id: add7c61515c5a16165682bbf2fdda031d693d17b
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="511">
   <si>
     <t>[sku]</t>
   </si>
@@ -1553,7 +1553,10 @@
     <t>lightdragon_skin_4</t>
   </si>
   <si>
-    <t>disguise_furyDuration_hp_transform_gold</t>
+    <t>transform_gold_LOW</t>
+  </si>
+  <si>
+    <t>disguise_furyDuration_hp_transform_gold_LOW</t>
   </si>
 </sst>
 </file>
@@ -3363,8 +3366,8 @@
   </sheetPr>
   <dimension ref="B1:T79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
-      <selection activeCell="E81" sqref="E81"/>
+    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
+      <selection activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7070,7 +7073,7 @@
         <v>1</v>
       </c>
       <c r="G76" s="79">
-        <v>500000</v>
+        <v>600000</v>
       </c>
       <c r="H76" s="79">
         <v>0</v>
@@ -7119,10 +7122,10 @@
         <v>2</v>
       </c>
       <c r="G77" s="79">
-        <v>500000</v>
+        <v>0</v>
       </c>
       <c r="H77" s="79">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="I77" s="79">
         <v>4</v>
@@ -7162,7 +7165,7 @@
         <v>488</v>
       </c>
       <c r="E78" s="91" t="s">
-        <v>430</v>
+        <v>509</v>
       </c>
       <c r="F78" s="64">
         <v>3</v>
@@ -7211,7 +7214,7 @@
         <v>488</v>
       </c>
       <c r="E79" s="92" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="F79" s="73">
         <v>4</v>

</xml_diff>

<commit_message>
Adding components for the 4th disguise
Former-commit-id: c0d87918ceb1cfc3927633b2b19a9c42cada248d
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="512">
   <si>
     <t>[sku]</t>
   </si>
@@ -1557,6 +1557,9 @@
   </si>
   <si>
     <t>disguise_furyDuration_hp_transform_gold_LOW</t>
+  </si>
+  <si>
+    <t>PF_light_archangel_back;PF_light_archangel_head;PF_light_archangel_lower_jaw;PF_light_archangel_shoulder_left;PF_light_archangel_shoulder_right;PF_light_archangel_staff;PF_light_archangel_waist</t>
   </si>
 </sst>
 </file>
@@ -2277,7 +2280,7 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3367,7 +3370,7 @@
   <dimension ref="B1:T79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
-      <selection activeCell="E79" sqref="E79"/>
+      <selection activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7237,7 +7240,9 @@
       </c>
       <c r="M79" s="76"/>
       <c r="N79" s="76"/>
-      <c r="O79" s="76"/>
+      <c r="O79" s="76" t="s">
+        <v>511</v>
+      </c>
       <c r="P79" s="76"/>
       <c r="Q79" s="69" t="s">
         <v>498</v>

</xml_diff>

<commit_message>
TEXTS not localized yet
Former-commit-id: 3910797ceaf7328bef356289f261d5826d7c9f96
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -1572,7 +1572,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1627,14 +1627,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -2013,7 +2005,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
@@ -2278,9 +2270,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3375,8 +3364,8 @@
   </sheetPr>
   <dimension ref="B1:T79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
-      <selection activeCell="O78" sqref="O78"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="I78" sqref="I78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3387,7 +3376,8 @@
     <col min="5" max="5" width="47.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
     <col min="10" max="10" width="17.140625" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
     <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
@@ -7075,20 +7065,20 @@
       <c r="D76" s="66" t="s">
         <v>488</v>
       </c>
-      <c r="E76" s="92" t="s">
-        <v>247</v>
+      <c r="E76" s="91" t="s">
+        <v>509</v>
       </c>
       <c r="F76" s="64">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G76" s="79">
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="H76" s="79">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="I76" s="79">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J76" s="61"/>
       <c r="K76" s="28" t="s">
@@ -7104,10 +7094,10 @@
       </c>
       <c r="P76" s="62"/>
       <c r="Q76" s="68" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="R76" s="58" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="S76" s="58" t="s">
         <v>505</v>
@@ -7127,19 +7117,19 @@
         <v>488</v>
       </c>
       <c r="E77" s="50" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F77" s="64">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G77" s="79">
-        <v>0</v>
+        <v>900000</v>
       </c>
       <c r="H77" s="79">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="I77" s="79">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J77" s="61"/>
       <c r="K77" s="28" t="s">
@@ -7155,10 +7145,10 @@
       </c>
       <c r="P77" s="62"/>
       <c r="Q77" s="68" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="R77" s="58" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="S77" s="58" t="s">
         <v>506</v>
@@ -7177,20 +7167,20 @@
       <c r="D78" s="66" t="s">
         <v>488</v>
       </c>
-      <c r="E78" s="90" t="s">
-        <v>509</v>
+      <c r="E78" s="50" t="s">
+        <v>248</v>
       </c>
       <c r="F78" s="64">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G78" s="79">
         <v>0</v>
       </c>
       <c r="H78" s="79">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="I78" s="79">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J78" s="61"/>
       <c r="K78" s="28" t="s">
@@ -7204,10 +7194,10 @@
       <c r="O78" s="62"/>
       <c r="P78" s="62"/>
       <c r="Q78" s="68" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="R78" s="58" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="S78" s="58" t="s">
         <v>507</v>
@@ -7226,7 +7216,7 @@
       <c r="D79" s="72" t="s">
         <v>488</v>
       </c>
-      <c r="E79" s="91" t="s">
+      <c r="E79" s="90" t="s">
         <v>510</v>
       </c>
       <c r="F79" s="73">

</xml_diff>

<commit_message>
Adding vfx to content for dragon light
Former-commit-id: eca638891f744aa5794743a3af18e2115ded340a
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="516">
   <si>
     <t>[sku]</t>
   </si>
@@ -1559,13 +1559,19 @@
     <t>disguise_furyDuration_hp_transform_gold_LOW</t>
   </si>
   <si>
-    <t>PF_light_archangel_back;PF_light_archangel_head;PF_light_archangel_lower_jaw;PF_light_archangel_shoulder_left;PF_light_archangel_shoulder_right;PF_light_archangel_staff;PF_light_archangel_waist</t>
-  </si>
-  <si>
-    <t>PF_light_phoenix_horn_1;PF_light_phoenix_horn_2</t>
-  </si>
-  <si>
-    <t>PF_light_nature_horn</t>
+    <t>FX_PF_LightDragon_Skin00_Wings_Right;FX_PF_LightDragon_Skin00_Wings_Left</t>
+  </si>
+  <si>
+    <t>PF_light_phoenix_horn_1;PF_light_phoenix_horn_2;FX_PF_LightDragon_Skin01_Wings_Right;FX_PF_LightDragon_Skin01_Wings_Left;FX_PF_LightDragon_Skin01_Wings_Right_Trail;FX_PF_LightDragon_Skin01_Wings_Left_Trail</t>
+  </si>
+  <si>
+    <t>PF_light_nature_horn;FX_PF_LightDragon_Skin02_Wings_Right;FX_PF_LightDragon_Skin02_Wings_Left;FX_PF_LightDragon_Skin02_Tail</t>
+  </si>
+  <si>
+    <t>FX_PF_LightDragon_Skin03_Wings_Right;FX_PF_LightDragon_Skin03_Wings_Left;FX_PF_LightDragon_Skin03_Wand</t>
+  </si>
+  <si>
+    <t>PF_light_archangel_back;PF_light_archangel_head;PF_light_archangel_lower_jaw;PF_light_archangel_shoulder_left;PF_light_archangel_shoulder_right;PF_light_archangel_staff;PF_light_archangel_waist;FX_PF_LightDragon_Skin04_Wings_Right;FX_PF_LightDragon_Skin04_Wings_Left;FX_PF_LightDragon_Skin04_Head</t>
   </si>
 </sst>
 </file>
@@ -3364,8 +3370,8 @@
   </sheetPr>
   <dimension ref="B1:T79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="I78" sqref="I78"/>
+    <sheetView tabSelected="1" topLeftCell="E46" workbookViewId="0">
+      <selection activeCell="O80" sqref="O80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7040,7 +7046,9 @@
       </c>
       <c r="M75" s="62"/>
       <c r="N75" s="62"/>
-      <c r="O75" s="62"/>
+      <c r="O75" s="28" t="s">
+        <v>511</v>
+      </c>
       <c r="P75" s="62"/>
       <c r="Q75" s="82" t="s">
         <v>494</v>
@@ -7191,7 +7199,9 @@
       </c>
       <c r="M78" s="62"/>
       <c r="N78" s="62"/>
-      <c r="O78" s="62"/>
+      <c r="O78" s="62" t="s">
+        <v>514</v>
+      </c>
       <c r="P78" s="62"/>
       <c r="Q78" s="68" t="s">
         <v>496</v>
@@ -7241,7 +7251,7 @@
       <c r="M79" s="76"/>
       <c r="N79" s="76"/>
       <c r="O79" s="76" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
       <c r="P79" s="76"/>
       <c r="Q79" s="69" t="s">

</xml_diff>

<commit_message>
Adding VFX parts to disguise 3
Former-commit-id: 5b299ad37efb20eaab3b4fff8f7a0b58ba0eb8bc
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -1571,7 +1571,7 @@
     <t>PF_light_archangel_back;PF_light_archangel_head;PF_light_archangel_lower_jaw;PF_light_archangel_shoulder_left;PF_light_archangel_shoulder_right;PF_light_archangel_staff;PF_light_archangel_waist;FX_PF_LightDragon_Skin04_Wings_Right;FX_PF_LightDragon_Skin04_Wings_Left;FX_PF_LightDragon_Skin04_Head</t>
   </si>
   <si>
-    <t>FX_PF_LightDragon_Skin03_Wings_Right;FX_PF_LightDragon_Skin03_Wings_Left;FX_PF_LightDragon_Skin03_Wand;PF_light_wizard_bear;PF_light_wizard_belt;PF_light_wizard_cape;PF_light_wizard_eyebrows;PF_light_wizard_hood;PF_light_wizard_horns;PF_light_wizard_staff</t>
+    <t>FX_PF_LightDragon_Skin03_Wings_Right;FX_PF_LightDragon_Skin03_Wings_Left;PF_light_wizard_bear;PF_light_wizard_belt;PF_light_wizard_cape_hood;PF_light_wizard_eyebrows;PF_light_wizard_horns;PF_light_wizard_staff</t>
   </si>
 </sst>
 </file>
@@ -3367,8 +3367,8 @@
   </sheetPr>
   <dimension ref="B1:T79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="J83" sqref="J83"/>
+    <sheetView tabSelected="1" topLeftCell="F46" workbookViewId="0">
+      <selection activeCell="O78" sqref="O78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7196,7 +7196,7 @@
       </c>
       <c r="M78" s="62"/>
       <c r="N78" s="62"/>
-      <c r="O78" s="62" t="s">
+      <c r="O78" s="28" t="s">
         <v>515</v>
       </c>
       <c r="P78" s="62"/>

</xml_diff>

<commit_message>
Changes for Skeleton - China
Former-commit-id: 17418f72f113575871c6d424fb09b54a160d1c8b
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -1424,21 +1424,6 @@
     <t>skeletondragon_skin_4</t>
   </si>
   <si>
-    <t>PF_skeleton_body_fire;PF_skeleton_mouth_fire;PF_skeleton_tail_fire</t>
-  </si>
-  <si>
-    <t>PF_skeleton_motu_axe;PF_skeleton_motu_chest;PF_skeleton_motu_hood;PF_skeleton_motu_shin_LF;PF_skeleton_motu_shin_RT;PF_skeleton_motu_shoulder_LF;PF_skeleton_motu_shoulder_RT;PF_skeleton_mouth_fire_blue;PF_skeleton_tail_fire_blue</t>
-  </si>
-  <si>
-    <t>PF_skeleton_termi_wing_LF;PF_skeleton_termi_wing_RT;PF_skeleton_body_fire;PF_skeleton_mouth_fire;PF_skeleton_tail_fire</t>
-  </si>
-  <si>
-    <t>PF_skeleton_mex_guitar;PF_skeleton_mex_hat;PF_skeleton_mex_jacket;PF_skeleton_mex_sleeve_RT;PF_skeleton_mex_sleeve_LF;PF_skeleton_mouth_fire</t>
-  </si>
-  <si>
-    <t>PF_skeleton_viking_necklace;PF_skeleton_viking_axe;PF_skeleton_viking_belt;PF_skeleton_viking_helmet;PF_skeleton_viking_shield;PF_skeleton_viking_shoulder_LF;PF_skeleton_viking_shoulder_RT;PF_skeleton_body_fire_blue;PF_skeleton_mouth_fire_blue;PF_skeleton_tail_fire_blue</t>
-  </si>
-  <si>
     <t>icon_tony_0</t>
   </si>
   <si>
@@ -1572,6 +1557,21 @@
   </si>
   <si>
     <t>FX_PF_LightDragon_Skin03_Wings_Right;FX_PF_LightDragon_Skin03_Wings_Left;PF_light_wizard_bear;PF_light_wizard_belt;PF_light_wizard_cape_hood;PF_light_wizard_eyebrows;PF_light_wizard_horns;PF_light_wizard_staff</t>
+  </si>
+  <si>
+    <t>PF_skeleton_wing_LF_0;PF_skeleton_wing_RT_0;PF_skeleton_facemask_0;PF_skeleton_legpiece_LF_0;PF_skeleton_legpiece_RT_0;PF_skeleton_ribcage_0;PF_skeleton_vertebra_1_0;PF_skeleton_vertebra_2_0;PF_skeleton_vertebra_3_0;PF_skeleton_body_fire;PF_skeleton_mouth_fire;PF_skeleton_tail_fire</t>
+  </si>
+  <si>
+    <t>PF_skeleton_wing_LF_2;PF_skeleton_wing_RT_2;PF_skeleton_facemask_2;PF_skeleton_legpiece_LF_2;PF_skeleton_legpiece_RT_2;PF_skeleton_ribcage_2;PF_skeleton_vertebra_1_2;PF_skeleton_vertebra_2_2;PF_skeleton_vertebra_3_2;PF_skeleton_termi_wing_LF;PF_skeleton_termi_wing_RT;PF_skeleton_body_fire;PF_skeleton_mouth_fire;PF_skeleton_tail_fire</t>
+  </si>
+  <si>
+    <t>PF_skeleton_wing_LF_1;PF_skeleton_wing_RT_1;PF_skeleton_facemask_1;PF_skeleton_legpiece_LF_1;PF_skeleton_legpiece_RT_1;PF_skeleton_ribcage_1;PF_skeleton_vertebra_1_1;PF_skeleton_vertebra_2_1;PF_skeleton_vertebra_3_1; PF_skeleton_motu_axe;PF_skeleton_motu_chest;PF_skeleton_motu_hood;PF_skeleton_motu_shin_LF;PF_skeleton_motu_shin_RT;PF_skeleton_motu_shoulder_LF;PF_skeleton_motu_shoulder_RT;PF_skeleton_mouth_fire_blue;PF_skeleton_tail_fire_blue</t>
+  </si>
+  <si>
+    <t>PF_skeleton_wing_LF_3;PF_skeleton_wing_RT_3;PF_skeleton_facemask_3;PF_skeleton_legpiece_LF_3;PF_skeleton_legpiece_RT_3;PF_skeleton_ribcage_3;PF_skeleton_vertebra_1_3;PF_skeleton_vertebra_2_3;PF_skeleton_vertebra_3_3;PF_skeleton_mex_guitar;PF_skeleton_mex_hat;PF_skeleton_mex_jacket;PF_skeleton_mex_sleeve_RT;PF_skeleton_mex_sleeve_LF;PF_skeleton_mouth_fire</t>
+  </si>
+  <si>
+    <t>PF_skeleton_wing_LF_4;PF_skeleton_wing_RT_4;PF_skeleton_facemask_4;PF_skeleton_legpiece_LF_4;PF_skeleton_legpiece_RT_4;PF_skeleton_ribcage_4;PF_skeleton_vertebra_1_4;PF_skeleton_vertebra_2_4;PF_skeleton_vertebra_3_4;PF_skeleton_viking_necklace;PF_skeleton_viking_axe;PF_skeleton_viking_belt;PF_skeleton_viking_helmet;PF_skeleton_viking_shield;PF_skeleton_viking_shoulder_LF;PF_skeleton_viking_shoulder_RT;PF_skeleton_body_fire_blue;PF_skeleton_mouth_fire_blue;PF_skeleton_tail_fire_blue</t>
   </si>
 </sst>
 </file>
@@ -2011,7 +2011,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
@@ -2281,6 +2281,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3367,8 +3368,8 @@
   </sheetPr>
   <dimension ref="B1:T79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F46" workbookViewId="0">
-      <selection activeCell="O78" sqref="O78"/>
+    <sheetView tabSelected="1" topLeftCell="C46" workbookViewId="0">
+      <selection activeCell="O75" sqref="O75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3910,17 +3911,17 @@
       </c>
       <c r="J13" s="35"/>
       <c r="K13" s="36" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="L13" s="36" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="M13" s="36"/>
       <c r="N13" s="36"/>
       <c r="O13" s="28"/>
       <c r="P13" s="28"/>
       <c r="Q13" s="37" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="R13" s="38" t="s">
         <v>303</v>
@@ -3959,15 +3960,15 @@
       </c>
       <c r="J14" s="35"/>
       <c r="K14" s="36" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="L14" s="36" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="M14" s="36"/>
       <c r="N14" s="36"/>
       <c r="O14" s="28" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="P14" s="28"/>
       <c r="Q14" s="37" t="s">
@@ -4010,15 +4011,15 @@
       </c>
       <c r="J15" s="27"/>
       <c r="K15" s="28" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="L15" s="28" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="M15" s="28"/>
       <c r="N15" s="28"/>
       <c r="O15" s="28" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="P15" s="28"/>
       <c r="Q15" s="58" t="s">
@@ -4061,15 +4062,15 @@
       </c>
       <c r="J16" s="27"/>
       <c r="K16" s="28" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="L16" s="28" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="M16" s="28"/>
       <c r="N16" s="28"/>
       <c r="O16" s="28" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="P16" s="28"/>
       <c r="Q16" s="29" t="s">
@@ -6790,8 +6791,8 @@
       </c>
       <c r="M70" s="62"/>
       <c r="N70" s="62"/>
-      <c r="O70" s="62" t="s">
-        <v>466</v>
+      <c r="O70" s="28" t="s">
+        <v>511</v>
       </c>
       <c r="P70" s="62"/>
       <c r="Q70" s="80" t="s">
@@ -6807,7 +6808,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:20" s="91" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B71" s="65" t="s">
         <v>3</v>
       </c>
@@ -6841,8 +6842,8 @@
       </c>
       <c r="M71" s="62"/>
       <c r="N71" s="62"/>
-      <c r="O71" s="62" t="s">
-        <v>467</v>
+      <c r="O71" s="28" t="s">
+        <v>513</v>
       </c>
       <c r="P71" s="62"/>
       <c r="Q71" s="68" t="s">
@@ -6892,8 +6893,8 @@
       </c>
       <c r="M72" s="62"/>
       <c r="N72" s="62"/>
-      <c r="O72" s="62" t="s">
-        <v>468</v>
+      <c r="O72" s="28" t="s">
+        <v>512</v>
       </c>
       <c r="P72" s="62"/>
       <c r="Q72" s="68" t="s">
@@ -6943,8 +6944,8 @@
       </c>
       <c r="M73" s="62"/>
       <c r="N73" s="62"/>
-      <c r="O73" s="62" t="s">
-        <v>469</v>
+      <c r="O73" s="28" t="s">
+        <v>514</v>
       </c>
       <c r="P73" s="62"/>
       <c r="Q73" s="68" t="s">
@@ -6994,8 +6995,8 @@
       </c>
       <c r="M74" s="86"/>
       <c r="N74" s="86"/>
-      <c r="O74" s="86" t="s">
-        <v>470</v>
+      <c r="O74" s="43" t="s">
+        <v>515</v>
       </c>
       <c r="P74" s="86"/>
       <c r="Q74" s="87" t="s">
@@ -7016,10 +7017,10 @@
         <v>3</v>
       </c>
       <c r="C75" s="78" t="s">
+        <v>478</v>
+      </c>
+      <c r="D75" s="78" t="s">
         <v>483</v>
-      </c>
-      <c r="D75" s="78" t="s">
-        <v>488</v>
       </c>
       <c r="E75" s="77"/>
       <c r="F75" s="64">
@@ -7036,25 +7037,25 @@
       </c>
       <c r="J75" s="61"/>
       <c r="K75" s="28" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="L75" s="28" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="M75" s="62"/>
       <c r="N75" s="62"/>
       <c r="O75" s="28" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="P75" s="62"/>
       <c r="Q75" s="80" t="s">
+        <v>489</v>
+      </c>
+      <c r="R75" s="30" t="s">
         <v>494</v>
       </c>
-      <c r="R75" s="30" t="s">
+      <c r="S75" s="30" t="s">
         <v>499</v>
-      </c>
-      <c r="S75" s="30" t="s">
-        <v>504</v>
       </c>
       <c r="T75" s="70">
         <v>71</v>
@@ -7065,13 +7066,13 @@
         <v>3</v>
       </c>
       <c r="C76" s="66" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="D76" s="66" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="E76" s="89" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="F76" s="64">
         <v>3</v>
@@ -7087,25 +7088,25 @@
       </c>
       <c r="J76" s="61"/>
       <c r="K76" s="28" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="L76" s="28" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="M76" s="62"/>
       <c r="N76" s="62"/>
       <c r="O76" s="62" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="P76" s="62"/>
       <c r="Q76" s="68" t="s">
+        <v>492</v>
+      </c>
+      <c r="R76" s="58" t="s">
         <v>497</v>
       </c>
-      <c r="R76" s="58" t="s">
-        <v>502</v>
-      </c>
       <c r="S76" s="58" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="T76" s="63">
         <v>72</v>
@@ -7116,10 +7117,10 @@
         <v>3</v>
       </c>
       <c r="C77" s="66" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="D77" s="66" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="E77" s="50" t="s">
         <v>247</v>
@@ -7138,25 +7139,25 @@
       </c>
       <c r="J77" s="61"/>
       <c r="K77" s="28" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="L77" s="28" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="M77" s="62"/>
       <c r="N77" s="62"/>
       <c r="O77" s="28" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="P77" s="62"/>
       <c r="Q77" s="68" t="s">
+        <v>490</v>
+      </c>
+      <c r="R77" s="58" t="s">
         <v>495</v>
       </c>
-      <c r="R77" s="58" t="s">
-        <v>500</v>
-      </c>
       <c r="S77" s="58" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="T77" s="63">
         <v>73</v>
@@ -7167,10 +7168,10 @@
         <v>3</v>
       </c>
       <c r="C78" s="66" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="D78" s="66" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="E78" s="50" t="s">
         <v>248</v>
@@ -7189,25 +7190,25 @@
       </c>
       <c r="J78" s="61"/>
       <c r="K78" s="28" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="L78" s="28" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="M78" s="62"/>
       <c r="N78" s="62"/>
       <c r="O78" s="28" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="P78" s="62"/>
       <c r="Q78" s="68" t="s">
+        <v>491</v>
+      </c>
+      <c r="R78" s="58" t="s">
         <v>496</v>
       </c>
-      <c r="R78" s="58" t="s">
-        <v>501</v>
-      </c>
       <c r="S78" s="58" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="T78" s="63">
         <v>74</v>
@@ -7218,13 +7219,13 @@
         <v>3</v>
       </c>
       <c r="C79" s="72" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="D79" s="72" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="E79" s="88" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="F79" s="73">
         <v>4</v>
@@ -7240,25 +7241,25 @@
       </c>
       <c r="J79" s="74"/>
       <c r="K79" s="75" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="L79" s="75" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="M79" s="76"/>
       <c r="N79" s="76"/>
       <c r="O79" s="76" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="P79" s="76"/>
       <c r="Q79" s="69" t="s">
+        <v>493</v>
+      </c>
+      <c r="R79" s="38" t="s">
         <v>498</v>
       </c>
-      <c r="R79" s="38" t="s">
+      <c r="S79" s="38" t="s">
         <v>503</v>
-      </c>
-      <c r="S79" s="38" t="s">
-        <v>508</v>
       </c>
       <c r="T79" s="72">
         <v>75</v>

</xml_diff>

<commit_message>
Updating data for Vampire dragon: progression data
Former-commit-id: 9ad4fb63bae01c2e9f3643ed1032297c675d5f73
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="543">
   <si>
     <t>[sku]</t>
   </si>
@@ -1572,6 +1572,87 @@
   </si>
   <si>
     <t>PF_skeleton_wing_LF_4;PF_skeleton_wing_RT_4;PF_skeleton_facemask_4;PF_skeleton_legpiece_LF_4;PF_skeleton_legpiece_RT_4;PF_skeleton_ribcage_4;PF_skeleton_vertebra_1_4;PF_skeleton_vertebra_2_4;PF_skeleton_vertebra_3_4;PF_skeleton_viking_necklace;PF_skeleton_viking_axe;PF_skeleton_viking_belt;PF_skeleton_viking_helmet;PF_skeleton_viking_shield;PF_skeleton_viking_shoulder_LF;PF_skeleton_viking_shoulder_RT;PF_skeleton_body_fire_blue;PF_skeleton_mouth_fire_blue;PF_skeleton_tail_fire_blue</t>
+  </si>
+  <si>
+    <t>dragon_vampire_0</t>
+  </si>
+  <si>
+    <t>dragon_vampire_4</t>
+  </si>
+  <si>
+    <t>dragon_vampire_3</t>
+  </si>
+  <si>
+    <t>dragon_vampire_2</t>
+  </si>
+  <si>
+    <t>dragon_vampire_1</t>
+  </si>
+  <si>
+    <t>dragon_vampire</t>
+  </si>
+  <si>
+    <t>icon_vampire_0</t>
+  </si>
+  <si>
+    <t>icon_vampire_4</t>
+  </si>
+  <si>
+    <t>icon_vampire_3</t>
+  </si>
+  <si>
+    <t>icon_vampire_2</t>
+  </si>
+  <si>
+    <t>icon_vampire_1</t>
+  </si>
+  <si>
+    <t>PF_vampire_armourplate;PF_vampire_belt;PF_vampire_shoulderpad_L;PF_vampire_shoulderpad_R</t>
+  </si>
+  <si>
+    <t>TID_SKIN_VAMPIRE_0_NAME</t>
+  </si>
+  <si>
+    <t>TID_SKIN_VAMPIRE_3_NAME</t>
+  </si>
+  <si>
+    <t>TID_SKIN_VAMPIRE_1_NAME</t>
+  </si>
+  <si>
+    <t>TID_SKIN_VAMPIRE_2_NAME</t>
+  </si>
+  <si>
+    <t>TID_SKIN_VAMPIRE_4_NAME</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_VAMPIRE_0_DESC</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_VAMPIRE_3_DESC</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_VAMPIRE_1_DESC</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_VAMPIRE_2_DESC</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_VAMPIRE_4_DESC</t>
+  </si>
+  <si>
+    <t>vampiredragon_default</t>
+  </si>
+  <si>
+    <t>vampìredragon_skin_1</t>
+  </si>
+  <si>
+    <t>vampìredragon_skin_2</t>
+  </si>
+  <si>
+    <t>vampìredragon_skin_3</t>
+  </si>
+  <si>
+    <t>vampìredragon_skin_4</t>
   </si>
 </sst>
 </file>
@@ -1716,7 +1797,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1982,17 +2063,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -2011,7 +2081,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
@@ -2215,30 +2285,12 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2272,13 +2324,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -3070,8 +3116,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="disguisesDefinitions6" displayName="disguisesDefinitions6" ref="B4:T79" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19">
-  <autoFilter ref="B4:T79"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="disguisesDefinitions6" displayName="disguisesDefinitions6" ref="B4:T84" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19">
+  <autoFilter ref="B4:T84"/>
   <sortState ref="B5:T46">
     <sortCondition ref="T4:T46"/>
   </sortState>
@@ -3366,10 +3412,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="B1:T79"/>
+  <dimension ref="B1:T84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C46" workbookViewId="0">
-      <selection activeCell="O75" sqref="O75"/>
+    <sheetView tabSelected="1" topLeftCell="O49" workbookViewId="0">
+      <selection activeCell="O86" sqref="O86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6728,7 +6774,7 @@
       <c r="H69" s="42">
         <v>65</v>
       </c>
-      <c r="I69" s="81">
+      <c r="I69" s="75">
         <v>0</v>
       </c>
       <c r="J69" s="42" t="s">
@@ -6760,16 +6806,16 @@
       </c>
     </row>
     <row r="70" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B70" s="79" t="s">
-        <v>3</v>
-      </c>
-      <c r="C70" s="78" t="s">
+      <c r="B70" s="73" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70" s="72" t="s">
         <v>438</v>
       </c>
-      <c r="D70" s="78" t="s">
+      <c r="D70" s="72" t="s">
         <v>443</v>
       </c>
-      <c r="E70" s="77"/>
+      <c r="E70" s="71"/>
       <c r="F70" s="64">
         <v>0</v>
       </c>
@@ -6795,7 +6841,7 @@
         <v>511</v>
       </c>
       <c r="P70" s="62"/>
-      <c r="Q70" s="80" t="s">
+      <c r="Q70" s="74" t="s">
         <v>451</v>
       </c>
       <c r="R70" s="30" t="s">
@@ -6804,11 +6850,11 @@
       <c r="S70" s="30" t="s">
         <v>461</v>
       </c>
-      <c r="T70" s="70">
+      <c r="T70" s="69">
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="2:20" s="91" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:20" s="83" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B71" s="65" t="s">
         <v>3</v>
       </c>
@@ -6962,44 +7008,44 @@
       </c>
     </row>
     <row r="74" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="82" t="s">
-        <v>3</v>
-      </c>
-      <c r="C74" s="83" t="s">
+      <c r="B74" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74" s="77" t="s">
         <v>442</v>
       </c>
-      <c r="D74" s="83" t="s">
+      <c r="D74" s="77" t="s">
         <v>443</v>
       </c>
       <c r="E74" s="54" t="s">
         <v>445</v>
       </c>
-      <c r="F74" s="84">
+      <c r="F74" s="78">
         <v>4</v>
       </c>
-      <c r="G74" s="85">
-        <v>0</v>
-      </c>
-      <c r="H74" s="85">
+      <c r="G74" s="79">
+        <v>0</v>
+      </c>
+      <c r="H74" s="79">
         <v>70</v>
       </c>
-      <c r="I74" s="85">
+      <c r="I74" s="79">
         <v>10</v>
       </c>
-      <c r="J74" s="85"/>
+      <c r="J74" s="79"/>
       <c r="K74" s="43" t="s">
         <v>450</v>
       </c>
       <c r="L74" s="43" t="s">
         <v>442</v>
       </c>
-      <c r="M74" s="86"/>
-      <c r="N74" s="86"/>
+      <c r="M74" s="80"/>
+      <c r="N74" s="80"/>
       <c r="O74" s="43" t="s">
         <v>515</v>
       </c>
-      <c r="P74" s="86"/>
-      <c r="Q74" s="87" t="s">
+      <c r="P74" s="80"/>
+      <c r="Q74" s="81" t="s">
         <v>455</v>
       </c>
       <c r="R74" s="45" t="s">
@@ -7008,21 +7054,21 @@
       <c r="S74" s="44" t="s">
         <v>465</v>
       </c>
-      <c r="T74" s="72">
+      <c r="T74" s="70">
         <v>70</v>
       </c>
     </row>
     <row r="75" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B75" s="79" t="s">
-        <v>3</v>
-      </c>
-      <c r="C75" s="78" t="s">
+      <c r="B75" s="73" t="s">
+        <v>3</v>
+      </c>
+      <c r="C75" s="72" t="s">
         <v>478</v>
       </c>
-      <c r="D75" s="78" t="s">
+      <c r="D75" s="72" t="s">
         <v>483</v>
       </c>
-      <c r="E75" s="77"/>
+      <c r="E75" s="71"/>
       <c r="F75" s="64">
         <v>0</v>
       </c>
@@ -7048,7 +7094,7 @@
         <v>506</v>
       </c>
       <c r="P75" s="62"/>
-      <c r="Q75" s="80" t="s">
+      <c r="Q75" s="74" t="s">
         <v>489</v>
       </c>
       <c r="R75" s="30" t="s">
@@ -7057,7 +7103,7 @@
       <c r="S75" s="30" t="s">
         <v>499</v>
       </c>
-      <c r="T75" s="70">
+      <c r="T75" s="69">
         <v>71</v>
       </c>
     </row>
@@ -7071,7 +7117,7 @@
       <c r="D76" s="66" t="s">
         <v>483</v>
       </c>
-      <c r="E76" s="89" t="s">
+      <c r="E76" s="82" t="s">
         <v>504</v>
       </c>
       <c r="F76" s="64">
@@ -7214,55 +7260,280 @@
         <v>74</v>
       </c>
     </row>
-    <row r="79" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B79" s="71" t="s">
-        <v>3</v>
-      </c>
-      <c r="C79" s="72" t="s">
+    <row r="79" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="C79" s="77" t="s">
         <v>482</v>
       </c>
-      <c r="D79" s="72" t="s">
+      <c r="D79" s="77" t="s">
         <v>483</v>
       </c>
-      <c r="E79" s="88" t="s">
+      <c r="E79" s="54" t="s">
         <v>505</v>
       </c>
-      <c r="F79" s="73">
+      <c r="F79" s="78">
         <v>4</v>
       </c>
-      <c r="G79" s="90">
-        <v>0</v>
-      </c>
-      <c r="H79" s="90">
+      <c r="G79" s="79">
+        <v>0</v>
+      </c>
+      <c r="H79" s="79">
         <v>75</v>
       </c>
-      <c r="I79" s="90">
+      <c r="I79" s="79">
         <v>10</v>
       </c>
-      <c r="J79" s="74"/>
-      <c r="K79" s="75" t="s">
+      <c r="J79" s="79"/>
+      <c r="K79" s="43" t="s">
         <v>488</v>
       </c>
-      <c r="L79" s="75" t="s">
+      <c r="L79" s="43" t="s">
         <v>482</v>
       </c>
-      <c r="M79" s="76"/>
-      <c r="N79" s="76"/>
-      <c r="O79" s="76" t="s">
+      <c r="M79" s="80"/>
+      <c r="N79" s="80"/>
+      <c r="O79" s="43" t="s">
         <v>509</v>
       </c>
-      <c r="P79" s="76"/>
-      <c r="Q79" s="69" t="s">
+      <c r="P79" s="80"/>
+      <c r="Q79" s="81" t="s">
         <v>493</v>
       </c>
-      <c r="R79" s="38" t="s">
+      <c r="R79" s="45" t="s">
         <v>498</v>
       </c>
-      <c r="S79" s="38" t="s">
+      <c r="S79" s="44" t="s">
         <v>503</v>
       </c>
-      <c r="T79" s="72">
+      <c r="T79" s="70">
         <v>75</v>
+      </c>
+    </row>
+    <row r="80" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B80" s="73" t="s">
+        <v>3</v>
+      </c>
+      <c r="C80" s="72" t="s">
+        <v>516</v>
+      </c>
+      <c r="D80" s="72" t="s">
+        <v>521</v>
+      </c>
+      <c r="E80" s="71"/>
+      <c r="F80" s="64">
+        <v>0</v>
+      </c>
+      <c r="G80" s="61"/>
+      <c r="H80" s="61"/>
+      <c r="I80" s="61">
+        <v>0</v>
+      </c>
+      <c r="J80" s="61"/>
+      <c r="K80" s="28" t="s">
+        <v>522</v>
+      </c>
+      <c r="L80" s="28" t="s">
+        <v>516</v>
+      </c>
+      <c r="M80" s="62"/>
+      <c r="N80" s="62"/>
+      <c r="O80" s="28" t="s">
+        <v>527</v>
+      </c>
+      <c r="P80" s="62"/>
+      <c r="Q80" s="74" t="s">
+        <v>528</v>
+      </c>
+      <c r="R80" s="30" t="s">
+        <v>533</v>
+      </c>
+      <c r="S80" s="30" t="s">
+        <v>538</v>
+      </c>
+      <c r="T80" s="69">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="81" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B81" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="C81" s="66" t="s">
+        <v>520</v>
+      </c>
+      <c r="D81" s="66" t="s">
+        <v>521</v>
+      </c>
+      <c r="E81" s="67"/>
+      <c r="F81" s="64">
+        <v>1</v>
+      </c>
+      <c r="G81" s="61"/>
+      <c r="H81" s="61"/>
+      <c r="I81" s="61">
+        <v>1</v>
+      </c>
+      <c r="J81" s="61"/>
+      <c r="K81" s="28" t="s">
+        <v>526</v>
+      </c>
+      <c r="L81" s="28" t="s">
+        <v>520</v>
+      </c>
+      <c r="M81" s="62"/>
+      <c r="N81" s="62"/>
+      <c r="O81" s="28" t="s">
+        <v>527</v>
+      </c>
+      <c r="P81" s="62"/>
+      <c r="Q81" s="68" t="s">
+        <v>529</v>
+      </c>
+      <c r="R81" s="58" t="s">
+        <v>534</v>
+      </c>
+      <c r="S81" s="58" t="s">
+        <v>539</v>
+      </c>
+      <c r="T81" s="63">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="82" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B82" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="C82" s="66" t="s">
+        <v>519</v>
+      </c>
+      <c r="D82" s="66" t="s">
+        <v>521</v>
+      </c>
+      <c r="E82" s="67"/>
+      <c r="F82" s="64">
+        <v>2</v>
+      </c>
+      <c r="G82" s="61"/>
+      <c r="H82" s="61"/>
+      <c r="I82" s="61">
+        <v>4</v>
+      </c>
+      <c r="J82" s="61"/>
+      <c r="K82" s="28" t="s">
+        <v>525</v>
+      </c>
+      <c r="L82" s="28" t="s">
+        <v>519</v>
+      </c>
+      <c r="M82" s="62"/>
+      <c r="N82" s="62"/>
+      <c r="O82" s="28" t="s">
+        <v>527</v>
+      </c>
+      <c r="P82" s="62"/>
+      <c r="Q82" s="68" t="s">
+        <v>530</v>
+      </c>
+      <c r="R82" s="58" t="s">
+        <v>535</v>
+      </c>
+      <c r="S82" s="58" t="s">
+        <v>540</v>
+      </c>
+      <c r="T82" s="63">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="83" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B83" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="C83" s="66" t="s">
+        <v>518</v>
+      </c>
+      <c r="D83" s="66" t="s">
+        <v>521</v>
+      </c>
+      <c r="E83" s="67"/>
+      <c r="F83" s="64">
+        <v>3</v>
+      </c>
+      <c r="G83" s="61"/>
+      <c r="H83" s="61"/>
+      <c r="I83" s="61">
+        <v>7</v>
+      </c>
+      <c r="J83" s="61"/>
+      <c r="K83" s="28" t="s">
+        <v>524</v>
+      </c>
+      <c r="L83" s="28" t="s">
+        <v>518</v>
+      </c>
+      <c r="M83" s="62"/>
+      <c r="N83" s="62"/>
+      <c r="O83" s="28" t="s">
+        <v>527</v>
+      </c>
+      <c r="P83" s="62"/>
+      <c r="Q83" s="68" t="s">
+        <v>531</v>
+      </c>
+      <c r="R83" s="58" t="s">
+        <v>536</v>
+      </c>
+      <c r="S83" s="58" t="s">
+        <v>541</v>
+      </c>
+      <c r="T83" s="63">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="84" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B84" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="C84" s="77" t="s">
+        <v>517</v>
+      </c>
+      <c r="D84" s="77" t="s">
+        <v>521</v>
+      </c>
+      <c r="E84" s="54"/>
+      <c r="F84" s="78">
+        <v>4</v>
+      </c>
+      <c r="G84" s="79"/>
+      <c r="H84" s="79"/>
+      <c r="I84" s="79">
+        <v>10</v>
+      </c>
+      <c r="J84" s="79"/>
+      <c r="K84" s="43" t="s">
+        <v>523</v>
+      </c>
+      <c r="L84" s="43" t="s">
+        <v>517</v>
+      </c>
+      <c r="M84" s="80"/>
+      <c r="N84" s="80"/>
+      <c r="O84" s="43" t="s">
+        <v>527</v>
+      </c>
+      <c r="P84" s="80"/>
+      <c r="Q84" s="81" t="s">
+        <v>532</v>
+      </c>
+      <c r="R84" s="45" t="s">
+        <v>537</v>
+      </c>
+      <c r="S84" s="44" t="s">
+        <v>542</v>
+      </c>
+      <c r="T84" s="70">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added villagers missing in powerup prey_hp_boost_humans Added more Powerups for Disguise Added examples of vampire dragon disguise powers
Former-commit-id: 68d424e5b687676cad115fa33e68fdf47cc9e5a6
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="548">
   <si>
     <t>[sku]</t>
   </si>
@@ -1653,6 +1653,21 @@
   </si>
   <si>
     <t>vampìredragon_skin_4</t>
+  </si>
+  <si>
+    <t>PF_vampire_belt_1;PF_vampire_hair2_1;PF_vampire_neck_1;PF_vampire_shoe_L_1;PF_vampire_shoe_R_1</t>
+  </si>
+  <si>
+    <t>PF_vampire_belt_2;PF_vampire_gears1_LF_2;PF_vampire_gears1_RT_2;PF_vampire_gears2_LF_2;PF_vampire_gears2_RT_2;PF_vampire_hair2_2;PF_vampire_handkerchief_2;PF_vampire_hat_2;PF_vampire_kneepad_LF_2;PF_vampire_kneepad_RT_2</t>
+  </si>
+  <si>
+    <t>disguise_speed_LOW_boost_LOW_disguise_lower_damage_poison</t>
+  </si>
+  <si>
+    <t>disguise_prey_hp_boost_humans_boost</t>
+  </si>
+  <si>
+    <t>disguise_speed_LOW_boost_LOW_prey_hp_boost_humans_boost</t>
   </si>
 </sst>
 </file>
@@ -3414,8 +3429,8 @@
   </sheetPr>
   <dimension ref="B1:T84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O49" workbookViewId="0">
-      <selection activeCell="O86" sqref="O86"/>
+    <sheetView tabSelected="1" topLeftCell="B57" workbookViewId="0">
+      <selection activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3425,7 +3440,7 @@
     <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.28515625" customWidth="1"/>
     <col min="10" max="10" width="17.140625" customWidth="1"/>
@@ -7366,11 +7381,15 @@
       <c r="D81" s="66" t="s">
         <v>521</v>
       </c>
-      <c r="E81" s="67"/>
+      <c r="E81" s="67" t="s">
+        <v>546</v>
+      </c>
       <c r="F81" s="64">
         <v>1</v>
       </c>
-      <c r="G81" s="61"/>
+      <c r="G81" s="61">
+        <v>1200000</v>
+      </c>
       <c r="H81" s="61"/>
       <c r="I81" s="61">
         <v>1</v>
@@ -7385,7 +7404,7 @@
       <c r="M81" s="62"/>
       <c r="N81" s="62"/>
       <c r="O81" s="28" t="s">
-        <v>527</v>
+        <v>543</v>
       </c>
       <c r="P81" s="62"/>
       <c r="Q81" s="68" t="s">
@@ -7411,12 +7430,16 @@
       <c r="D82" s="66" t="s">
         <v>521</v>
       </c>
-      <c r="E82" s="67"/>
+      <c r="E82" s="67" t="s">
+        <v>545</v>
+      </c>
       <c r="F82" s="64">
         <v>2</v>
       </c>
       <c r="G82" s="61"/>
-      <c r="H82" s="61"/>
+      <c r="H82" s="61">
+        <v>70</v>
+      </c>
       <c r="I82" s="61">
         <v>4</v>
       </c>
@@ -7430,7 +7453,7 @@
       <c r="M82" s="62"/>
       <c r="N82" s="62"/>
       <c r="O82" s="28" t="s">
-        <v>527</v>
+        <v>544</v>
       </c>
       <c r="P82" s="62"/>
       <c r="Q82" s="68" t="s">
@@ -7456,12 +7479,16 @@
       <c r="D83" s="66" t="s">
         <v>521</v>
       </c>
-      <c r="E83" s="67"/>
+      <c r="E83" s="67" t="s">
+        <v>547</v>
+      </c>
       <c r="F83" s="64">
         <v>3</v>
       </c>
       <c r="G83" s="61"/>
-      <c r="H83" s="61"/>
+      <c r="H83" s="61">
+        <v>75</v>
+      </c>
       <c r="I83" s="61">
         <v>7</v>
       </c>
@@ -7501,12 +7528,16 @@
       <c r="D84" s="77" t="s">
         <v>521</v>
       </c>
-      <c r="E84" s="54"/>
+      <c r="E84" s="54" t="s">
+        <v>230</v>
+      </c>
       <c r="F84" s="78">
         <v>4</v>
       </c>
-      <c r="G84" s="79"/>
-      <c r="H84" s="79"/>
+      <c r="G84" s="61"/>
+      <c r="H84" s="79">
+        <v>80</v>
+      </c>
       <c r="I84" s="79">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
fixed issues with powers added correct tids, skins, order and new powers
Former-commit-id: 32191f1c954baefc96625465d9781100be7b2698
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="550">
   <si>
     <t>[sku]</t>
   </si>
@@ -1661,20 +1661,26 @@
     <t>PF_vampire_belt_2;PF_vampire_gears1_LF_2;PF_vampire_gears1_RT_2;PF_vampire_gears2_LF_2;PF_vampire_gears2_RT_2;PF_vampire_hair2_2;PF_vampire_handkerchief_2;PF_vampire_hat_2;PF_vampire_kneepad_LF_2;PF_vampire_kneepad_RT_2</t>
   </si>
   <si>
-    <t>disguise_speed_LOW_boost_LOW_disguise_lower_damage_poison</t>
-  </si>
-  <si>
-    <t>disguise_prey_hp_boost_humans_boost</t>
-  </si>
-  <si>
-    <t>disguise_speed_LOW_boost_LOW_prey_hp_boost_humans_boost</t>
+    <t>disguise_speed_LOW_boost_LOW_lower_damage_poison</t>
+  </si>
+  <si>
+    <t>disguise_speed_LOW_boost_LOW</t>
+  </si>
+  <si>
+    <t>disguise_prey_hp_boost_humans</t>
+  </si>
+  <si>
+    <t>PF_vampire_hair_4;PF_vampire_leg_flowers_left_4;PF_vampire_leg_flowers_right_4;PF_vampire_leafs_back_4;PF_vampire_tail_flowers_4;PF_vampire_wing_flower_left_4;PF_vampire_wing_flower_right_4;PF_vampire_neck_4</t>
+  </si>
+  <si>
+    <t>disguise_speed_LOW_hp_LOW</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1729,6 +1735,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1812,7 +1826,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -2092,11 +2106,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
@@ -2343,6 +2387,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3429,8 +3485,8 @@
   </sheetPr>
   <dimension ref="B1:T84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B57" workbookViewId="0">
-      <selection activeCell="E82" sqref="E82"/>
+    <sheetView tabSelected="1" topLeftCell="C46" workbookViewId="0">
+      <selection activeCell="O83" sqref="O83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7381,8 +7437,8 @@
       <c r="D81" s="66" t="s">
         <v>521</v>
       </c>
-      <c r="E81" s="67" t="s">
-        <v>546</v>
+      <c r="E81" s="82" t="s">
+        <v>549</v>
       </c>
       <c r="F81" s="64">
         <v>1</v>
@@ -7390,28 +7446,28 @@
       <c r="G81" s="61">
         <v>1200000</v>
       </c>
-      <c r="H81" s="61"/>
+      <c r="H81" s="86"/>
       <c r="I81" s="61">
         <v>1</v>
       </c>
       <c r="J81" s="61"/>
       <c r="K81" s="28" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="L81" s="28" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="M81" s="62"/>
       <c r="N81" s="62"/>
       <c r="O81" s="28" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="P81" s="62"/>
       <c r="Q81" s="68" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="R81" s="58" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="S81" s="58" t="s">
         <v>539</v>
@@ -7420,7 +7476,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="82" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B82" s="65" t="s">
         <v>3</v>
       </c>
@@ -7430,13 +7486,13 @@
       <c r="D82" s="66" t="s">
         <v>521</v>
       </c>
-      <c r="E82" s="67" t="s">
-        <v>545</v>
+      <c r="E82" s="82" t="s">
+        <v>547</v>
       </c>
       <c r="F82" s="64">
         <v>2</v>
       </c>
-      <c r="G82" s="61"/>
+      <c r="G82" s="85"/>
       <c r="H82" s="61">
         <v>70</v>
       </c>
@@ -7445,15 +7501,15 @@
       </c>
       <c r="J82" s="61"/>
       <c r="K82" s="28" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="L82" s="28" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="M82" s="62"/>
       <c r="N82" s="62"/>
-      <c r="O82" s="28" t="s">
-        <v>544</v>
+      <c r="O82" s="84" t="s">
+        <v>543</v>
       </c>
       <c r="P82" s="62"/>
       <c r="Q82" s="68" t="s">
@@ -7479,8 +7535,8 @@
       <c r="D83" s="66" t="s">
         <v>521</v>
       </c>
-      <c r="E83" s="67" t="s">
-        <v>547</v>
+      <c r="E83" s="87" t="s">
+        <v>546</v>
       </c>
       <c r="F83" s="64">
         <v>3</v>
@@ -7506,10 +7562,10 @@
       </c>
       <c r="P83" s="62"/>
       <c r="Q83" s="68" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="R83" s="58" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="S83" s="58" t="s">
         <v>541</v>
@@ -7529,7 +7585,7 @@
         <v>521</v>
       </c>
       <c r="E84" s="54" t="s">
-        <v>230</v>
+        <v>545</v>
       </c>
       <c r="F84" s="78">
         <v>4</v>
@@ -7551,7 +7607,7 @@
       <c r="M84" s="80"/>
       <c r="N84" s="80"/>
       <c r="O84" s="43" t="s">
-        <v>527</v>
+        <v>548</v>
       </c>
       <c r="P84" s="80"/>
       <c r="Q84" s="81" t="s">

</xml_diff>

<commit_message>
adjustments Dragon vampire min and max health and drain Adjustments Power ups and add 3rd skin to content
Former-commit-id: 5f0e63696af8b882a9759bb87e13616c204220d5
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="551">
   <si>
     <t>[sku]</t>
   </si>
@@ -1670,10 +1670,13 @@
     <t>disguise_prey_hp_boost_humans</t>
   </si>
   <si>
-    <t>PF_vampire_hair_4;PF_vampire_leg_flowers_left_4;PF_vampire_leg_flowers_right_4;PF_vampire_leafs_back_4;PF_vampire_tail_flowers_4;PF_vampire_wing_flower_left_4;PF_vampire_wing_flower_right_4;PF_vampire_neck_4</t>
-  </si>
-  <si>
-    <t>disguise_speed_LOW_hp_LOW</t>
+    <t>disguise_fury_duration_LOW_1</t>
+  </si>
+  <si>
+    <t>PF_vampire_hair_4;PF_vampire_leg_flowers_left_4;PF_vampire_leg_flowers_right_4;PF_vampire_leafs_back_4;PF_vampire_tail_flowers_4;PF_vampire_wing_flower_left_4;PF_vampire_wing_flower_right_4;PF_vampire_neck_4;FX_PF_VampireDragon_Skin04_Wings_Left;FX_PF_VampireDragon_Skin04_Wings_Right</t>
+  </si>
+  <si>
+    <t>PF_vampire_belt_3;PF_vampire_hair_3;PF_vampire_jacket_3;PF_vampire_knee_L_3;PF_vampire_knee_R_3;PF_vampire_neck_3;PF_vampire_skate_L_3;PF_vampire_skate_R_3</t>
   </si>
 </sst>
 </file>
@@ -1740,7 +1743,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3485,7 +3487,7 @@
   </sheetPr>
   <dimension ref="B1:T84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C46" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
       <selection activeCell="O83" sqref="O83"/>
     </sheetView>
   </sheetViews>
@@ -7437,8 +7439,8 @@
       <c r="D81" s="66" t="s">
         <v>521</v>
       </c>
-      <c r="E81" s="82" t="s">
-        <v>549</v>
+      <c r="E81" s="50" t="s">
+        <v>548</v>
       </c>
       <c r="F81" s="64">
         <v>1</v>
@@ -7558,7 +7560,7 @@
       <c r="M83" s="62"/>
       <c r="N83" s="62"/>
       <c r="O83" s="28" t="s">
-        <v>527</v>
+        <v>550</v>
       </c>
       <c r="P83" s="62"/>
       <c r="Q83" s="68" t="s">
@@ -7607,7 +7609,7 @@
       <c r="M84" s="80"/>
       <c r="N84" s="80"/>
       <c r="O84" s="43" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="P84" s="80"/>
       <c r="Q84" s="81" t="s">

</xml_diff>

<commit_message>
Dragonjira content update (tables + disguisesdefinition xml)
Former-commit-id: 8cff3bf6c11298ceb98464be44bab06a4a86d888
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\HD\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="577">
   <si>
     <t>[sku]</t>
   </si>
@@ -1643,18 +1643,6 @@
     <t>vampiredragon_default</t>
   </si>
   <si>
-    <t>vampìredragon_skin_1</t>
-  </si>
-  <si>
-    <t>vampìredragon_skin_2</t>
-  </si>
-  <si>
-    <t>vampìredragon_skin_3</t>
-  </si>
-  <si>
-    <t>vampìredragon_skin_4</t>
-  </si>
-  <si>
     <t>PF_vampire_belt_1;PF_vampire_hair2_1;PF_vampire_neck_1;PF_vampire_shoe_L_1;PF_vampire_shoe_R_1</t>
   </si>
   <si>
@@ -1677,13 +1665,103 @@
   </si>
   <si>
     <t>disguise_fury_duration_LOW_Steam</t>
+  </si>
+  <si>
+    <t>dragon_dragonjira_0</t>
+  </si>
+  <si>
+    <t>dragon_dragonjira_1</t>
+  </si>
+  <si>
+    <t>dragon_dragonjira_2</t>
+  </si>
+  <si>
+    <t>dragon_dragonjira_3</t>
+  </si>
+  <si>
+    <t>dragon_dragonjira_4</t>
+  </si>
+  <si>
+    <t>dragon_dragonjira</t>
+  </si>
+  <si>
+    <t>icon_dragonjira_0</t>
+  </si>
+  <si>
+    <t>icon_dragonjira_1</t>
+  </si>
+  <si>
+    <t>icon_dragonjira_2</t>
+  </si>
+  <si>
+    <t>icon_dragonjira_3</t>
+  </si>
+  <si>
+    <t>icon_dragonjira_4</t>
+  </si>
+  <si>
+    <t>TID_SKIN_DRAGONJIRA_0_NAME</t>
+  </si>
+  <si>
+    <t>TID_SKIN_DRAGONJIRA_1_NAME</t>
+  </si>
+  <si>
+    <t>TID_SKIN_DRAGONJIRA_2_NAME</t>
+  </si>
+  <si>
+    <t>TID_SKIN_DRAGONJIRA_3_NAME</t>
+  </si>
+  <si>
+    <t>TID_SKIN_DRAGONJIRA_4_NAME</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_DRAGONJIRA_0_DESC</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_DRAGONJIRA_1_DESC</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_DRAGONJIRA_2_DESC</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_DRAGONJIRA_3_DESC</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_DRAGONJIRA_4_DESC</t>
+  </si>
+  <si>
+    <t>vampiredragon_skin_4</t>
+  </si>
+  <si>
+    <t>vampiredragon_skin_3</t>
+  </si>
+  <si>
+    <t>vampiredragon_skin_2</t>
+  </si>
+  <si>
+    <t>vampiredragon_skin_1</t>
+  </si>
+  <si>
+    <t>dragonjiradragon_default</t>
+  </si>
+  <si>
+    <t>dragonjiradragon_skin_1</t>
+  </si>
+  <si>
+    <t>dragonjiradragon_skin_2</t>
+  </si>
+  <si>
+    <t>dragonjiradragon_skin_3</t>
+  </si>
+  <si>
+    <t>dragonjiradragon_skin_4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1738,6 +1816,20 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1821,7 +1913,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -2120,14 +2212,25 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top style="thin">
         <color auto="1"/>
-      </right>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2135,7 +2238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
@@ -2385,10 +2488,37 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3086,6 +3216,13 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -3123,13 +3260,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -3179,8 +3309,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="disguisesDefinitions6" displayName="disguisesDefinitions6" ref="B4:T84" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19">
-  <autoFilter ref="B4:T84"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="disguisesDefinitions6" displayName="disguisesDefinitions6" ref="B4:T89" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" headerRowBorderDxfId="19" tableBorderDxfId="20">
+  <autoFilter ref="B4:T89"/>
   <sortState ref="B5:T46">
     <sortCondition ref="T4:T46"/>
   </sortState>
@@ -3475,17 +3605,17 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="B1:T84"/>
+  <dimension ref="B1:T89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="E83" sqref="E83:E84"/>
+    <sheetView tabSelected="1" topLeftCell="O64" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
@@ -3493,7 +3623,7 @@
     <col min="9" max="9" width="12.28515625" customWidth="1"/>
     <col min="10" max="10" width="17.140625" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="73" customWidth="1"/>
     <col min="16" max="16" width="29" bestFit="1" customWidth="1"/>
@@ -7430,15 +7560,15 @@
         <v>521</v>
       </c>
       <c r="E81" s="50" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="F81" s="64">
         <v>1</v>
       </c>
-      <c r="G81" s="61">
+      <c r="G81" s="27">
         <v>1200000</v>
       </c>
-      <c r="H81" s="86"/>
+      <c r="H81" s="27"/>
       <c r="I81" s="61">
         <v>1</v>
       </c>
@@ -7452,7 +7582,7 @@
       <c r="M81" s="62"/>
       <c r="N81" s="62"/>
       <c r="O81" s="28" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="P81" s="62"/>
       <c r="Q81" s="68" t="s">
@@ -7462,13 +7592,13 @@
         <v>536</v>
       </c>
       <c r="S81" s="58" t="s">
-        <v>539</v>
+        <v>571</v>
       </c>
       <c r="T81" s="63">
         <v>77</v>
       </c>
     </row>
-    <row r="82" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B82" s="65" t="s">
         <v>3</v>
       </c>
@@ -7479,13 +7609,13 @@
         <v>521</v>
       </c>
       <c r="E82" s="82" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="F82" s="64">
         <v>2</v>
       </c>
-      <c r="G82" s="85"/>
-      <c r="H82" s="61">
+      <c r="G82" s="27"/>
+      <c r="H82" s="27">
         <v>70</v>
       </c>
       <c r="I82" s="61">
@@ -7501,7 +7631,7 @@
       <c r="M82" s="62"/>
       <c r="N82" s="62"/>
       <c r="O82" s="84" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="P82" s="62"/>
       <c r="Q82" s="68" t="s">
@@ -7511,7 +7641,7 @@
         <v>535</v>
       </c>
       <c r="S82" s="58" t="s">
-        <v>540</v>
+        <v>570</v>
       </c>
       <c r="T82" s="63">
         <v>78</v>
@@ -7528,13 +7658,13 @@
         <v>521</v>
       </c>
       <c r="E83" s="82" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="F83" s="64">
         <v>3</v>
       </c>
-      <c r="G83" s="61"/>
-      <c r="H83" s="61">
+      <c r="G83" s="27"/>
+      <c r="H83" s="27">
         <v>75</v>
       </c>
       <c r="I83" s="61">
@@ -7550,7 +7680,7 @@
       <c r="M83" s="62"/>
       <c r="N83" s="62"/>
       <c r="O83" s="28" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="P83" s="62"/>
       <c r="Q83" s="68" t="s">
@@ -7560,7 +7690,7 @@
         <v>534</v>
       </c>
       <c r="S83" s="58" t="s">
-        <v>541</v>
+        <v>569</v>
       </c>
       <c r="T83" s="63">
         <v>79</v>
@@ -7577,12 +7707,12 @@
         <v>521</v>
       </c>
       <c r="E84" s="82" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="F84" s="78">
         <v>4</v>
       </c>
-      <c r="G84" s="61"/>
+      <c r="G84" s="79"/>
       <c r="H84" s="79">
         <v>80</v>
       </c>
@@ -7599,7 +7729,7 @@
       <c r="M84" s="80"/>
       <c r="N84" s="80"/>
       <c r="O84" s="43" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="P84" s="80"/>
       <c r="Q84" s="81" t="s">
@@ -7609,10 +7739,251 @@
         <v>537</v>
       </c>
       <c r="S84" s="44" t="s">
-        <v>542</v>
+        <v>568</v>
       </c>
       <c r="T84" s="70">
         <v>80</v>
+      </c>
+    </row>
+    <row r="85" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B85" s="72" t="s">
+        <v>3</v>
+      </c>
+      <c r="C85" s="72" t="s">
+        <v>547</v>
+      </c>
+      <c r="D85" s="72" t="s">
+        <v>552</v>
+      </c>
+      <c r="E85" s="85"/>
+      <c r="F85" s="90">
+        <v>0</v>
+      </c>
+      <c r="G85" s="86"/>
+      <c r="H85" s="86"/>
+      <c r="I85" s="86">
+        <v>0</v>
+      </c>
+      <c r="J85" s="86"/>
+      <c r="K85" s="95" t="s">
+        <v>553</v>
+      </c>
+      <c r="L85" s="95" t="s">
+        <v>547</v>
+      </c>
+      <c r="M85" s="87"/>
+      <c r="N85" s="87"/>
+      <c r="O85" s="87" t="s">
+        <v>527</v>
+      </c>
+      <c r="P85" s="87"/>
+      <c r="Q85" s="93" t="s">
+        <v>558</v>
+      </c>
+      <c r="R85" s="94" t="s">
+        <v>563</v>
+      </c>
+      <c r="S85" s="88" t="s">
+        <v>572</v>
+      </c>
+      <c r="T85" s="70">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="86" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B86" s="66" t="s">
+        <v>3</v>
+      </c>
+      <c r="C86" s="66" t="s">
+        <v>548</v>
+      </c>
+      <c r="D86" s="66" t="s">
+        <v>552</v>
+      </c>
+      <c r="E86" s="85" t="s">
+        <v>546</v>
+      </c>
+      <c r="F86" s="90">
+        <v>1</v>
+      </c>
+      <c r="G86" s="86">
+        <v>1200000</v>
+      </c>
+      <c r="H86" s="86"/>
+      <c r="I86" s="86">
+        <v>1</v>
+      </c>
+      <c r="J86" s="86"/>
+      <c r="K86" s="95" t="s">
+        <v>554</v>
+      </c>
+      <c r="L86" s="95" t="s">
+        <v>548</v>
+      </c>
+      <c r="M86" s="87"/>
+      <c r="N86" s="87"/>
+      <c r="O86" s="87" t="s">
+        <v>540</v>
+      </c>
+      <c r="P86" s="87"/>
+      <c r="Q86" s="93" t="s">
+        <v>559</v>
+      </c>
+      <c r="R86" s="94" t="s">
+        <v>564</v>
+      </c>
+      <c r="S86" s="89" t="s">
+        <v>573</v>
+      </c>
+      <c r="T86" s="70">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="87" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B87" s="66" t="s">
+        <v>3</v>
+      </c>
+      <c r="C87" s="66" t="s">
+        <v>549</v>
+      </c>
+      <c r="D87" s="66" t="s">
+        <v>552</v>
+      </c>
+      <c r="E87" s="85" t="s">
+        <v>542</v>
+      </c>
+      <c r="F87" s="90">
+        <v>2</v>
+      </c>
+      <c r="G87" s="86"/>
+      <c r="H87" s="86">
+        <v>70</v>
+      </c>
+      <c r="I87" s="86">
+        <v>4</v>
+      </c>
+      <c r="J87" s="86"/>
+      <c r="K87" s="95" t="s">
+        <v>555</v>
+      </c>
+      <c r="L87" s="95" t="s">
+        <v>549</v>
+      </c>
+      <c r="M87" s="87"/>
+      <c r="N87" s="87"/>
+      <c r="O87" s="87" t="s">
+        <v>539</v>
+      </c>
+      <c r="P87" s="87"/>
+      <c r="Q87" s="93" t="s">
+        <v>560</v>
+      </c>
+      <c r="R87" s="94" t="s">
+        <v>565</v>
+      </c>
+      <c r="S87" s="89" t="s">
+        <v>574</v>
+      </c>
+      <c r="T87" s="70">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="88" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B88" s="66" t="s">
+        <v>3</v>
+      </c>
+      <c r="C88" s="66" t="s">
+        <v>550</v>
+      </c>
+      <c r="D88" s="66" t="s">
+        <v>552</v>
+      </c>
+      <c r="E88" s="85" t="s">
+        <v>541</v>
+      </c>
+      <c r="F88" s="90">
+        <v>3</v>
+      </c>
+      <c r="G88" s="86"/>
+      <c r="H88" s="86">
+        <v>75</v>
+      </c>
+      <c r="I88" s="86">
+        <v>7</v>
+      </c>
+      <c r="J88" s="86"/>
+      <c r="K88" s="95" t="s">
+        <v>556</v>
+      </c>
+      <c r="L88" s="95" t="s">
+        <v>550</v>
+      </c>
+      <c r="M88" s="87"/>
+      <c r="N88" s="87"/>
+      <c r="O88" s="87" t="s">
+        <v>544</v>
+      </c>
+      <c r="P88" s="87"/>
+      <c r="Q88" s="93" t="s">
+        <v>561</v>
+      </c>
+      <c r="R88" s="94" t="s">
+        <v>566</v>
+      </c>
+      <c r="S88" s="89" t="s">
+        <v>575</v>
+      </c>
+      <c r="T88" s="70">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="89" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B89" s="77" t="s">
+        <v>3</v>
+      </c>
+      <c r="C89" s="77" t="s">
+        <v>551</v>
+      </c>
+      <c r="D89" s="77" t="s">
+        <v>552</v>
+      </c>
+      <c r="E89" s="85" t="s">
+        <v>545</v>
+      </c>
+      <c r="F89" s="91">
+        <v>4</v>
+      </c>
+      <c r="G89" s="92"/>
+      <c r="H89" s="92">
+        <v>80</v>
+      </c>
+      <c r="I89" s="86">
+        <v>10</v>
+      </c>
+      <c r="J89" s="86"/>
+      <c r="K89" s="95" t="s">
+        <v>557</v>
+      </c>
+      <c r="L89" s="95" t="s">
+        <v>551</v>
+      </c>
+      <c r="M89" s="87"/>
+      <c r="N89" s="87"/>
+      <c r="O89" s="87" t="s">
+        <v>543</v>
+      </c>
+      <c r="P89" s="87"/>
+      <c r="Q89" s="93" t="s">
+        <v>562</v>
+      </c>
+      <c r="R89" s="94" t="s">
+        <v>567</v>
+      </c>
+      <c r="S89" s="88" t="s">
+        <v>576</v>
+      </c>
+      <c r="T89" s="70">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dragonjira content update (disguisesdefinition parts update)
Former-commit-id: 0af5c4b7c1f3bb483c20ce1ecc32b42f4090d278
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="577">
   <si>
     <t>[sku]</t>
   </si>
@@ -1810,12 +1810,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2497,12 +2499,6 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2519,6 +2515,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3216,13 +3218,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -3260,6 +3255,13 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -3309,7 +3311,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="disguisesDefinitions6" displayName="disguisesDefinitions6" ref="B4:T89" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" headerRowBorderDxfId="19" tableBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="disguisesDefinitions6" displayName="disguisesDefinitions6" ref="B4:T89" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19">
   <autoFilter ref="B4:T89"/>
   <sortState ref="B5:T46">
     <sortCondition ref="T4:T46"/>
@@ -3607,8 +3609,8 @@
   </sheetPr>
   <dimension ref="B1:T89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O64" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="J55" workbookViewId="0">
+      <selection activeCell="P88" sqref="P88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7706,7 +7708,7 @@
       <c r="D84" s="77" t="s">
         <v>521</v>
       </c>
-      <c r="E84" s="82" t="s">
+      <c r="E84" s="54" t="s">
         <v>545</v>
       </c>
       <c r="F84" s="78">
@@ -7755,8 +7757,8 @@
       <c r="D85" s="72" t="s">
         <v>552</v>
       </c>
-      <c r="E85" s="85"/>
-      <c r="F85" s="90">
+      <c r="E85" s="82"/>
+      <c r="F85" s="88">
         <v>0</v>
       </c>
       <c r="G85" s="86"/>
@@ -7765,25 +7767,23 @@
         <v>0</v>
       </c>
       <c r="J85" s="86"/>
-      <c r="K85" s="95" t="s">
+      <c r="K85" s="93" t="s">
         <v>553</v>
       </c>
-      <c r="L85" s="95" t="s">
+      <c r="L85" s="93" t="s">
         <v>547</v>
       </c>
       <c r="M85" s="87"/>
       <c r="N85" s="87"/>
-      <c r="O85" s="87" t="s">
-        <v>527</v>
-      </c>
+      <c r="O85" s="87"/>
       <c r="P85" s="87"/>
-      <c r="Q85" s="93" t="s">
+      <c r="Q85" s="91" t="s">
         <v>558</v>
       </c>
-      <c r="R85" s="94" t="s">
+      <c r="R85" s="92" t="s">
         <v>563</v>
       </c>
-      <c r="S85" s="88" t="s">
+      <c r="S85" s="94" t="s">
         <v>572</v>
       </c>
       <c r="T85" s="70">
@@ -7803,7 +7803,7 @@
       <c r="E86" s="85" t="s">
         <v>546</v>
       </c>
-      <c r="F86" s="90">
+      <c r="F86" s="88">
         <v>1</v>
       </c>
       <c r="G86" s="86">
@@ -7814,25 +7814,23 @@
         <v>1</v>
       </c>
       <c r="J86" s="86"/>
-      <c r="K86" s="95" t="s">
+      <c r="K86" s="93" t="s">
         <v>554</v>
       </c>
-      <c r="L86" s="95" t="s">
+      <c r="L86" s="93" t="s">
         <v>548</v>
       </c>
       <c r="M86" s="87"/>
       <c r="N86" s="87"/>
-      <c r="O86" s="87" t="s">
-        <v>540</v>
-      </c>
+      <c r="O86" s="87"/>
       <c r="P86" s="87"/>
-      <c r="Q86" s="93" t="s">
+      <c r="Q86" s="91" t="s">
         <v>559</v>
       </c>
-      <c r="R86" s="94" t="s">
+      <c r="R86" s="92" t="s">
         <v>564</v>
       </c>
-      <c r="S86" s="89" t="s">
+      <c r="S86" s="95" t="s">
         <v>573</v>
       </c>
       <c r="T86" s="70">
@@ -7852,7 +7850,7 @@
       <c r="E87" s="85" t="s">
         <v>542</v>
       </c>
-      <c r="F87" s="90">
+      <c r="F87" s="88">
         <v>2</v>
       </c>
       <c r="G87" s="86"/>
@@ -7863,25 +7861,23 @@
         <v>4</v>
       </c>
       <c r="J87" s="86"/>
-      <c r="K87" s="95" t="s">
+      <c r="K87" s="93" t="s">
         <v>555</v>
       </c>
-      <c r="L87" s="95" t="s">
+      <c r="L87" s="93" t="s">
         <v>549</v>
       </c>
       <c r="M87" s="87"/>
       <c r="N87" s="87"/>
-      <c r="O87" s="87" t="s">
-        <v>539</v>
-      </c>
+      <c r="O87" s="87"/>
       <c r="P87" s="87"/>
-      <c r="Q87" s="93" t="s">
+      <c r="Q87" s="91" t="s">
         <v>560</v>
       </c>
-      <c r="R87" s="94" t="s">
+      <c r="R87" s="92" t="s">
         <v>565</v>
       </c>
-      <c r="S87" s="89" t="s">
+      <c r="S87" s="95" t="s">
         <v>574</v>
       </c>
       <c r="T87" s="70">
@@ -7901,7 +7897,7 @@
       <c r="E88" s="85" t="s">
         <v>541</v>
       </c>
-      <c r="F88" s="90">
+      <c r="F88" s="88">
         <v>3</v>
       </c>
       <c r="G88" s="86"/>
@@ -7912,25 +7908,23 @@
         <v>7</v>
       </c>
       <c r="J88" s="86"/>
-      <c r="K88" s="95" t="s">
+      <c r="K88" s="93" t="s">
         <v>556</v>
       </c>
-      <c r="L88" s="95" t="s">
+      <c r="L88" s="93" t="s">
         <v>550</v>
       </c>
       <c r="M88" s="87"/>
       <c r="N88" s="87"/>
-      <c r="O88" s="87" t="s">
-        <v>544</v>
-      </c>
+      <c r="O88" s="87"/>
       <c r="P88" s="87"/>
-      <c r="Q88" s="93" t="s">
+      <c r="Q88" s="91" t="s">
         <v>561</v>
       </c>
-      <c r="R88" s="94" t="s">
+      <c r="R88" s="92" t="s">
         <v>566</v>
       </c>
-      <c r="S88" s="89" t="s">
+      <c r="S88" s="95" t="s">
         <v>575</v>
       </c>
       <c r="T88" s="70">
@@ -7950,36 +7944,34 @@
       <c r="E89" s="85" t="s">
         <v>545</v>
       </c>
-      <c r="F89" s="91">
+      <c r="F89" s="89">
         <v>4</v>
       </c>
-      <c r="G89" s="92"/>
-      <c r="H89" s="92">
+      <c r="G89" s="90"/>
+      <c r="H89" s="90">
         <v>80</v>
       </c>
       <c r="I89" s="86">
         <v>10</v>
       </c>
       <c r="J89" s="86"/>
-      <c r="K89" s="95" t="s">
+      <c r="K89" s="93" t="s">
         <v>557</v>
       </c>
-      <c r="L89" s="95" t="s">
+      <c r="L89" s="93" t="s">
         <v>551</v>
       </c>
       <c r="M89" s="87"/>
       <c r="N89" s="87"/>
-      <c r="O89" s="87" t="s">
-        <v>543</v>
-      </c>
+      <c r="O89" s="87"/>
       <c r="P89" s="87"/>
-      <c r="Q89" s="93" t="s">
+      <c r="Q89" s="91" t="s">
         <v>562</v>
       </c>
-      <c r="R89" s="94" t="s">
+      <c r="R89" s="92" t="s">
         <v>567</v>
       </c>
-      <c r="S89" s="88" t="s">
+      <c r="S89" s="94" t="s">
         <v>576</v>
       </c>
       <c r="T89" s="70">

</xml_diff>

<commit_message>
added dragonjira skins and powers
Former-commit-id: b327ef4c9f94b1712a3dddd00e61be7d57b93072
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\HD\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="581">
   <si>
     <t>[sku]</t>
   </si>
@@ -1755,6 +1755,18 @@
   </si>
   <si>
     <t>dragonjiradragon_skin_4</t>
+  </si>
+  <si>
+    <t>disguise_faster_boost_speed_LOWx2</t>
+  </si>
+  <si>
+    <t>disguise_fury_duration_LOW_boost_LOW_dive</t>
+  </si>
+  <si>
+    <t>disguise_transform_gold_LOWx2_boost</t>
+  </si>
+  <si>
+    <t>disguise_transform_gold_LOWx2,5_boost_fury_duration_LOW</t>
   </si>
 </sst>
 </file>
@@ -1821,21 +1833,20 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color theme="9" tint="0.59999389629810485"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1914,8 +1925,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3399"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="26">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -2236,11 +2253,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
@@ -2490,9 +2522,6 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2508,20 +2537,32 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3218,6 +3259,13 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -3255,13 +3303,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -3311,7 +3352,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="disguisesDefinitions6" displayName="disguisesDefinitions6" ref="B4:T89" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="disguisesDefinitions6" displayName="disguisesDefinitions6" ref="B4:T89" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" headerRowBorderDxfId="19" tableBorderDxfId="20">
   <autoFilter ref="B4:T89"/>
   <sortState ref="B5:T46">
     <sortCondition ref="T4:T46"/>
@@ -3609,8 +3650,8 @@
   </sheetPr>
   <dimension ref="B1:T89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J55" workbookViewId="0">
-      <selection activeCell="P88" sqref="P88"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="E89" sqref="E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7758,32 +7799,32 @@
         <v>552</v>
       </c>
       <c r="E85" s="82"/>
-      <c r="F85" s="88">
-        <v>0</v>
-      </c>
-      <c r="G85" s="86"/>
-      <c r="H85" s="86"/>
-      <c r="I85" s="86">
-        <v>0</v>
-      </c>
-      <c r="J85" s="86"/>
-      <c r="K85" s="93" t="s">
+      <c r="F85" s="87">
+        <v>0</v>
+      </c>
+      <c r="G85" s="85"/>
+      <c r="H85" s="85"/>
+      <c r="I85" s="85">
+        <v>0</v>
+      </c>
+      <c r="J85" s="85"/>
+      <c r="K85" s="92" t="s">
         <v>553</v>
       </c>
-      <c r="L85" s="93" t="s">
+      <c r="L85" s="92" t="s">
         <v>547</v>
       </c>
-      <c r="M85" s="87"/>
-      <c r="N85" s="87"/>
-      <c r="O85" s="87"/>
-      <c r="P85" s="87"/>
-      <c r="Q85" s="91" t="s">
+      <c r="M85" s="86"/>
+      <c r="N85" s="86"/>
+      <c r="O85" s="86"/>
+      <c r="P85" s="86"/>
+      <c r="Q85" s="90" t="s">
         <v>558</v>
       </c>
-      <c r="R85" s="92" t="s">
+      <c r="R85" s="91" t="s">
         <v>563</v>
       </c>
-      <c r="S85" s="94" t="s">
+      <c r="S85" s="93" t="s">
         <v>572</v>
       </c>
       <c r="T85" s="70">
@@ -7800,37 +7841,37 @@
       <c r="D86" s="66" t="s">
         <v>552</v>
       </c>
-      <c r="E86" s="85" t="s">
-        <v>546</v>
-      </c>
-      <c r="F86" s="88">
+      <c r="E86" s="97" t="s">
+        <v>577</v>
+      </c>
+      <c r="F86" s="87">
         <v>1</v>
       </c>
-      <c r="G86" s="86">
-        <v>1200000</v>
-      </c>
-      <c r="H86" s="86"/>
-      <c r="I86" s="86">
+      <c r="G86" s="85">
+        <v>1500000</v>
+      </c>
+      <c r="H86" s="85"/>
+      <c r="I86" s="85">
         <v>1</v>
       </c>
-      <c r="J86" s="86"/>
-      <c r="K86" s="93" t="s">
+      <c r="J86" s="85"/>
+      <c r="K86" s="92" t="s">
         <v>554</v>
       </c>
-      <c r="L86" s="93" t="s">
+      <c r="L86" s="92" t="s">
         <v>548</v>
       </c>
-      <c r="M86" s="87"/>
-      <c r="N86" s="87"/>
-      <c r="O86" s="87"/>
-      <c r="P86" s="87"/>
-      <c r="Q86" s="91" t="s">
+      <c r="M86" s="86"/>
+      <c r="N86" s="86"/>
+      <c r="O86" s="86"/>
+      <c r="P86" s="86"/>
+      <c r="Q86" s="90" t="s">
         <v>559</v>
       </c>
-      <c r="R86" s="92" t="s">
+      <c r="R86" s="91" t="s">
         <v>564</v>
       </c>
-      <c r="S86" s="95" t="s">
+      <c r="S86" s="94" t="s">
         <v>573</v>
       </c>
       <c r="T86" s="70">
@@ -7847,37 +7888,37 @@
       <c r="D87" s="66" t="s">
         <v>552</v>
       </c>
-      <c r="E87" s="85" t="s">
-        <v>542</v>
-      </c>
-      <c r="F87" s="88">
+      <c r="E87" s="96" t="s">
+        <v>578</v>
+      </c>
+      <c r="F87" s="87">
         <v>2</v>
       </c>
-      <c r="G87" s="86"/>
-      <c r="H87" s="86">
-        <v>70</v>
-      </c>
-      <c r="I87" s="86">
+      <c r="G87" s="85"/>
+      <c r="H87" s="85">
+        <v>75</v>
+      </c>
+      <c r="I87" s="85">
         <v>4</v>
       </c>
-      <c r="J87" s="86"/>
-      <c r="K87" s="93" t="s">
+      <c r="J87" s="85"/>
+      <c r="K87" s="92" t="s">
         <v>555</v>
       </c>
-      <c r="L87" s="93" t="s">
+      <c r="L87" s="92" t="s">
         <v>549</v>
       </c>
-      <c r="M87" s="87"/>
-      <c r="N87" s="87"/>
-      <c r="O87" s="87"/>
-      <c r="P87" s="87"/>
-      <c r="Q87" s="91" t="s">
+      <c r="M87" s="86"/>
+      <c r="N87" s="86"/>
+      <c r="O87" s="86"/>
+      <c r="P87" s="86"/>
+      <c r="Q87" s="90" t="s">
         <v>560</v>
       </c>
-      <c r="R87" s="92" t="s">
+      <c r="R87" s="91" t="s">
         <v>565</v>
       </c>
-      <c r="S87" s="95" t="s">
+      <c r="S87" s="94" t="s">
         <v>574</v>
       </c>
       <c r="T87" s="70">
@@ -7894,37 +7935,37 @@
       <c r="D88" s="66" t="s">
         <v>552</v>
       </c>
-      <c r="E88" s="85" t="s">
-        <v>541</v>
-      </c>
-      <c r="F88" s="88">
-        <v>3</v>
-      </c>
-      <c r="G88" s="86"/>
-      <c r="H88" s="86">
-        <v>75</v>
-      </c>
-      <c r="I88" s="86">
+      <c r="E88" s="95" t="s">
+        <v>579</v>
+      </c>
+      <c r="F88" s="87">
+        <v>3</v>
+      </c>
+      <c r="G88" s="85"/>
+      <c r="H88" s="85">
+        <v>80</v>
+      </c>
+      <c r="I88" s="85">
         <v>7</v>
       </c>
-      <c r="J88" s="86"/>
-      <c r="K88" s="93" t="s">
+      <c r="J88" s="85"/>
+      <c r="K88" s="92" t="s">
         <v>556</v>
       </c>
-      <c r="L88" s="93" t="s">
+      <c r="L88" s="92" t="s">
         <v>550</v>
       </c>
-      <c r="M88" s="87"/>
-      <c r="N88" s="87"/>
-      <c r="O88" s="87"/>
-      <c r="P88" s="87"/>
-      <c r="Q88" s="91" t="s">
+      <c r="M88" s="86"/>
+      <c r="N88" s="86"/>
+      <c r="O88" s="86"/>
+      <c r="P88" s="86"/>
+      <c r="Q88" s="90" t="s">
         <v>561</v>
       </c>
-      <c r="R88" s="92" t="s">
+      <c r="R88" s="91" t="s">
         <v>566</v>
       </c>
-      <c r="S88" s="95" t="s">
+      <c r="S88" s="94" t="s">
         <v>575</v>
       </c>
       <c r="T88" s="70">
@@ -7941,37 +7982,37 @@
       <c r="D89" s="77" t="s">
         <v>552</v>
       </c>
-      <c r="E89" s="85" t="s">
-        <v>545</v>
-      </c>
-      <c r="F89" s="89">
+      <c r="E89" s="98" t="s">
+        <v>580</v>
+      </c>
+      <c r="F89" s="88">
         <v>4</v>
       </c>
-      <c r="G89" s="90"/>
-      <c r="H89" s="90">
-        <v>80</v>
-      </c>
-      <c r="I89" s="86">
+      <c r="G89" s="89"/>
+      <c r="H89" s="89">
+        <v>85</v>
+      </c>
+      <c r="I89" s="85">
         <v>10</v>
       </c>
-      <c r="J89" s="86"/>
-      <c r="K89" s="93" t="s">
+      <c r="J89" s="85"/>
+      <c r="K89" s="92" t="s">
         <v>557</v>
       </c>
-      <c r="L89" s="93" t="s">
+      <c r="L89" s="92" t="s">
         <v>551</v>
       </c>
-      <c r="M89" s="87"/>
-      <c r="N89" s="87"/>
-      <c r="O89" s="87"/>
-      <c r="P89" s="87"/>
-      <c r="Q89" s="91" t="s">
+      <c r="M89" s="86"/>
+      <c r="N89" s="86"/>
+      <c r="O89" s="86"/>
+      <c r="P89" s="86"/>
+      <c r="Q89" s="90" t="s">
         <v>562</v>
       </c>
-      <c r="R89" s="92" t="s">
+      <c r="R89" s="91" t="s">
         <v>567</v>
       </c>
-      <c r="S89" s="94" t="s">
+      <c r="S89" s="93" t="s">
         <v>576</v>
       </c>
       <c r="T89" s="70">

</xml_diff>

<commit_message>
fixed body parts 0, 3 and 4
Former-commit-id: 0cc170ba140b0fe904b57b5d06a5a6c589d919d0
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="586">
   <si>
     <t>[sku]</t>
   </si>
@@ -1767,13 +1767,28 @@
   </si>
   <si>
     <t>disguise_transform_gold_LOWx2,5_boost_fury_duration_LOW</t>
+  </si>
+  <si>
+    <t>FX_PF_Dragonjira_ElectricBody_Skin00;FX_PF_Dragonjira_Chest_Skin00;FX_PF_Dragonjira_Neck_Skin00;FX_PF_Dragonjira_Tail_Skin00</t>
+  </si>
+  <si>
+    <t>FX_PF_Dragonjira_ElectricBody_Skin01;FX_PF_Dragonjira_Chest_Skin01;FX_PF_Dragonjira_Neck_Skin01;FX_PF_Dragonjira_Tail_Skin01</t>
+  </si>
+  <si>
+    <t>PF_spartan_hand;PF_spartan_chest;PF_spartan_spine;PF_spartan_head;PF_spartan_shield;PF_spartan_shield_china;PF_spartan_arm_R;PF_spartan_knee_L;PF_spartan_knee_R;FX_PF_Dragonjira_Neck_Skin04;FX_PF_Dragonjira_Tail_Skin04</t>
+  </si>
+  <si>
+    <t>FX_PF_Dragonjira_ElectricBody_Skin03;FX_PF_Dragonjira_Chest_Skin03;FX_PF_Dragonjira_Tail_Skin03;PF_kawaii_hand;PF_kawaii_head;PF_kawaii_neck;PF_kawaii_tail;PF_kawaii_tail_04;PF_kawaii_torax</t>
+  </si>
+  <si>
+    <t>FX_PF_Dragonjira_ElectricBody_Skin02;FX_PF_Dragonjira_Chest_Skin02;FX_PF_Dragonjira_Neck_Skin02;FX_PF_Dragonjira_Tail_Skin02</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1843,6 +1858,12 @@
       <color theme="9" tint="0.59999389629810485"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -2272,7 +2293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
@@ -2563,6 +2584,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3650,8 +3674,8 @@
   </sheetPr>
   <dimension ref="B1:T89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="E89" sqref="E89"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93:XFD97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7816,7 +7840,9 @@
       </c>
       <c r="M85" s="86"/>
       <c r="N85" s="86"/>
-      <c r="O85" s="86"/>
+      <c r="O85" s="99" t="s">
+        <v>581</v>
+      </c>
       <c r="P85" s="86"/>
       <c r="Q85" s="90" t="s">
         <v>558</v>
@@ -7863,7 +7889,9 @@
       </c>
       <c r="M86" s="86"/>
       <c r="N86" s="86"/>
-      <c r="O86" s="86"/>
+      <c r="O86" s="86" t="s">
+        <v>582</v>
+      </c>
       <c r="P86" s="86"/>
       <c r="Q86" s="90" t="s">
         <v>559</v>
@@ -7910,7 +7938,9 @@
       </c>
       <c r="M87" s="86"/>
       <c r="N87" s="86"/>
-      <c r="O87" s="86"/>
+      <c r="O87" s="99" t="s">
+        <v>585</v>
+      </c>
       <c r="P87" s="86"/>
       <c r="Q87" s="90" t="s">
         <v>560</v>
@@ -7957,7 +7987,9 @@
       </c>
       <c r="M88" s="86"/>
       <c r="N88" s="86"/>
-      <c r="O88" s="86"/>
+      <c r="O88" s="86" t="s">
+        <v>584</v>
+      </c>
       <c r="P88" s="86"/>
       <c r="Q88" s="90" t="s">
         <v>561</v>
@@ -8004,7 +8036,9 @@
       </c>
       <c r="M89" s="86"/>
       <c r="N89" s="86"/>
-      <c r="O89" s="86"/>
+      <c r="O89" s="86" t="s">
+        <v>583</v>
+      </c>
       <c r="P89" s="86"/>
       <c r="Q89" s="90" t="s">
         <v>562</v>

</xml_diff>

<commit_message>
Jade disguises definition updated
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\client_lfs\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="610">
   <si>
     <t>[sku]</t>
   </si>
@@ -1782,6 +1782,78 @@
   </si>
   <si>
     <t>FX_PF_Dragonjira_ElectricBody_Skin02;FX_PF_Dragonjira_Chest_Skin02;FX_PF_Dragonjira_Neck_Skin02;FX_PF_Dragonjira_Tail_Skin02</t>
+  </si>
+  <si>
+    <t>dragon_jade_0</t>
+  </si>
+  <si>
+    <t>dragon_jade_1</t>
+  </si>
+  <si>
+    <t>dragon_jade_2</t>
+  </si>
+  <si>
+    <t>dragon_jade_3</t>
+  </si>
+  <si>
+    <t>dragon_jade</t>
+  </si>
+  <si>
+    <t>disguise_boost_LOW_faster_boost</t>
+  </si>
+  <si>
+    <t>disguise_speed_fury_duration_LOW</t>
+  </si>
+  <si>
+    <t>disguise_speed_LOW_boost_LOW_free_revive</t>
+  </si>
+  <si>
+    <t>icon_jade_0</t>
+  </si>
+  <si>
+    <t>icon_jade_2</t>
+  </si>
+  <si>
+    <t>icon_jade_1</t>
+  </si>
+  <si>
+    <t>icon_jade_3</t>
+  </si>
+  <si>
+    <t>jadedragon_default</t>
+  </si>
+  <si>
+    <t>jadedragon_skin_1</t>
+  </si>
+  <si>
+    <t>jadedragon_skin_2</t>
+  </si>
+  <si>
+    <t>jadedragon_skin_3</t>
+  </si>
+  <si>
+    <t>TID_SKIN_JADE_0_NAME</t>
+  </si>
+  <si>
+    <t>TID_SKIN_JADE_2_NAME</t>
+  </si>
+  <si>
+    <t>TID_SKIN_JADE_1_NAME</t>
+  </si>
+  <si>
+    <t>TID_SKIN_JADE_3_NAME</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_JADE_0_DESC</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_JADE_1_DESC</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_JADE_2_DESC</t>
+  </si>
+  <si>
+    <t>TID_DRAGON_JADE_3_DESC</t>
   </si>
 </sst>
 </file>
@@ -1953,7 +2025,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -2289,11 +2361,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
@@ -2586,6 +2701,45 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3672,10 +3826,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="B1:T89"/>
+  <dimension ref="B1:T93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A93" sqref="A93:XFD97"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="G91" sqref="G91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3685,7 +3839,7 @@
     <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.28515625" customWidth="1"/>
     <col min="10" max="10" width="17.140625" customWidth="1"/>
@@ -7813,7 +7967,7 @@
       </c>
     </row>
     <row r="85" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="72" t="s">
+      <c r="B85" s="107" t="s">
         <v>3</v>
       </c>
       <c r="C85" s="72" t="s">
@@ -7858,7 +8012,7 @@
       </c>
     </row>
     <row r="86" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="66" t="s">
+      <c r="B86" s="108" t="s">
         <v>3</v>
       </c>
       <c r="C86" s="66" t="s">
@@ -7907,7 +8061,7 @@
       </c>
     </row>
     <row r="87" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="66" t="s">
+      <c r="B87" s="108" t="s">
         <v>3</v>
       </c>
       <c r="C87" s="66" t="s">
@@ -7956,7 +8110,7 @@
       </c>
     </row>
     <row r="88" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="66" t="s">
+      <c r="B88" s="108" t="s">
         <v>3</v>
       </c>
       <c r="C88" s="66" t="s">
@@ -8005,7 +8159,7 @@
       </c>
     </row>
     <row r="89" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="77" t="s">
+      <c r="B89" s="109" t="s">
         <v>3</v>
       </c>
       <c r="C89" s="77" t="s">
@@ -8051,6 +8205,190 @@
       </c>
       <c r="T89" s="70">
         <v>85</v>
+      </c>
+    </row>
+    <row r="90" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B90" s="105" t="s">
+        <v>3</v>
+      </c>
+      <c r="C90" s="23" t="s">
+        <v>586</v>
+      </c>
+      <c r="D90" s="23" t="s">
+        <v>590</v>
+      </c>
+      <c r="E90" s="82"/>
+      <c r="F90" s="64">
+        <v>0</v>
+      </c>
+      <c r="G90" s="61"/>
+      <c r="H90" s="61"/>
+      <c r="I90" s="61">
+        <v>0</v>
+      </c>
+      <c r="J90" s="61"/>
+      <c r="K90" s="28" t="s">
+        <v>594</v>
+      </c>
+      <c r="L90" s="28" t="s">
+        <v>594</v>
+      </c>
+      <c r="M90" s="62"/>
+      <c r="N90" s="62"/>
+      <c r="O90" s="28"/>
+      <c r="P90" s="62"/>
+      <c r="Q90" s="74" t="s">
+        <v>602</v>
+      </c>
+      <c r="R90" s="30" t="s">
+        <v>606</v>
+      </c>
+      <c r="S90" s="30" t="s">
+        <v>598</v>
+      </c>
+      <c r="T90" s="102">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="91" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B91" s="106" t="s">
+        <v>3</v>
+      </c>
+      <c r="C91" s="59" t="s">
+        <v>587</v>
+      </c>
+      <c r="D91" s="23" t="s">
+        <v>590</v>
+      </c>
+      <c r="E91" s="82" t="s">
+        <v>591</v>
+      </c>
+      <c r="F91" s="111">
+        <v>1</v>
+      </c>
+      <c r="G91" s="100">
+        <v>1800000</v>
+      </c>
+      <c r="H91" s="100"/>
+      <c r="I91" s="61">
+        <v>1</v>
+      </c>
+      <c r="J91" s="61"/>
+      <c r="K91" s="28" t="s">
+        <v>595</v>
+      </c>
+      <c r="L91" s="28" t="s">
+        <v>595</v>
+      </c>
+      <c r="M91" s="62"/>
+      <c r="N91" s="62"/>
+      <c r="O91" s="28"/>
+      <c r="P91" s="62"/>
+      <c r="Q91" s="68" t="s">
+        <v>603</v>
+      </c>
+      <c r="R91" s="58" t="s">
+        <v>607</v>
+      </c>
+      <c r="S91" s="58" t="s">
+        <v>599</v>
+      </c>
+      <c r="T91" s="103">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="92" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B92" s="106" t="s">
+        <v>3</v>
+      </c>
+      <c r="C92" s="59" t="s">
+        <v>588</v>
+      </c>
+      <c r="D92" s="23" t="s">
+        <v>590</v>
+      </c>
+      <c r="E92" s="82" t="s">
+        <v>592</v>
+      </c>
+      <c r="F92" s="64">
+        <v>2</v>
+      </c>
+      <c r="G92" s="27"/>
+      <c r="H92" s="100">
+        <v>75</v>
+      </c>
+      <c r="I92" s="61">
+        <v>4</v>
+      </c>
+      <c r="J92" s="61"/>
+      <c r="K92" s="28" t="s">
+        <v>596</v>
+      </c>
+      <c r="L92" s="28" t="s">
+        <v>596</v>
+      </c>
+      <c r="M92" s="62"/>
+      <c r="N92" s="62"/>
+      <c r="O92" s="110"/>
+      <c r="P92" s="62"/>
+      <c r="Q92" s="68" t="s">
+        <v>604</v>
+      </c>
+      <c r="R92" s="68" t="s">
+        <v>608</v>
+      </c>
+      <c r="S92" s="68" t="s">
+        <v>600</v>
+      </c>
+      <c r="T92" s="103">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="93" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B93" s="112" t="s">
+        <v>3</v>
+      </c>
+      <c r="C93" s="77" t="s">
+        <v>589</v>
+      </c>
+      <c r="D93" s="77" t="s">
+        <v>590</v>
+      </c>
+      <c r="E93" s="54" t="s">
+        <v>593</v>
+      </c>
+      <c r="F93" s="78">
+        <v>3</v>
+      </c>
+      <c r="G93" s="79"/>
+      <c r="H93" s="101">
+        <v>80</v>
+      </c>
+      <c r="I93" s="79">
+        <v>7</v>
+      </c>
+      <c r="J93" s="79"/>
+      <c r="K93" s="43" t="s">
+        <v>597</v>
+      </c>
+      <c r="L93" s="43" t="s">
+        <v>597</v>
+      </c>
+      <c r="M93" s="80"/>
+      <c r="N93" s="80"/>
+      <c r="O93" s="43"/>
+      <c r="P93" s="80"/>
+      <c r="Q93" s="81" t="s">
+        <v>605</v>
+      </c>
+      <c r="R93" s="45" t="s">
+        <v>609</v>
+      </c>
+      <c r="S93" s="44" t="s">
+        <v>601</v>
+      </c>
+      <c r="T93" s="104">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed content excel's format
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -1927,19 +1927,19 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="9" tint="0.59999389629810485"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2018,14 +2018,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF3399"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="30">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -2350,65 +2344,18 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top style="thin">
         <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
@@ -2661,18 +2608,6 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2688,40 +2623,7 @@
     <xf numFmtId="0" fontId="8" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2733,13 +2635,37 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3530,8 +3456,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="disguisesDefinitions6" displayName="disguisesDefinitions6" ref="B4:T89" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" headerRowBorderDxfId="19" tableBorderDxfId="20">
-  <autoFilter ref="B4:T89"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="disguisesDefinitions6" displayName="disguisesDefinitions6" ref="B4:T93" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" headerRowBorderDxfId="19" tableBorderDxfId="20">
+  <autoFilter ref="B4:T93"/>
   <sortState ref="B5:T46">
     <sortCondition ref="T4:T46"/>
   </sortState>
@@ -3828,8 +3754,8 @@
   </sheetPr>
   <dimension ref="B1:T93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="G91" sqref="G91"/>
+    <sheetView tabSelected="1" topLeftCell="L64" workbookViewId="0">
+      <selection activeCell="Q91" sqref="Q91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3999,7 +3925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
         <v>3</v>
       </c>
@@ -4495,7 +4421,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="24" t="s">
         <v>3</v>
       </c>
@@ -4695,7 +4621,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="24" t="s">
         <v>3</v>
       </c>
@@ -4897,7 +4823,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="24" t="s">
         <v>3</v>
       </c>
@@ -5250,7 +5176,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="24" t="s">
         <v>3</v>
       </c>
@@ -6358,7 +6284,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B53" s="31" t="s">
         <v>3</v>
       </c>
@@ -7967,7 +7893,7 @@
       </c>
     </row>
     <row r="85" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="107" t="s">
+      <c r="B85" s="92" t="s">
         <v>3</v>
       </c>
       <c r="C85" s="72" t="s">
@@ -7976,35 +7902,35 @@
       <c r="D85" s="72" t="s">
         <v>552</v>
       </c>
-      <c r="E85" s="82"/>
-      <c r="F85" s="87">
-        <v>0</v>
-      </c>
-      <c r="G85" s="85"/>
-      <c r="H85" s="85"/>
-      <c r="I85" s="85">
+      <c r="E85" s="71"/>
+      <c r="F85" s="64">
+        <v>0</v>
+      </c>
+      <c r="G85" s="61"/>
+      <c r="H85" s="61"/>
+      <c r="I85" s="61">
         <v>0</v>
       </c>
       <c r="J85" s="85"/>
-      <c r="K85" s="92" t="s">
+      <c r="K85" s="88" t="s">
         <v>553</v>
       </c>
-      <c r="L85" s="92" t="s">
+      <c r="L85" s="88" t="s">
         <v>547</v>
       </c>
-      <c r="M85" s="86"/>
-      <c r="N85" s="86"/>
-      <c r="O85" s="99" t="s">
+      <c r="M85" s="62"/>
+      <c r="N85" s="62"/>
+      <c r="O85" s="28" t="s">
         <v>581</v>
       </c>
-      <c r="P85" s="86"/>
-      <c r="Q85" s="90" t="s">
+      <c r="P85" s="62"/>
+      <c r="Q85" s="86" t="s">
         <v>558</v>
       </c>
-      <c r="R85" s="91" t="s">
+      <c r="R85" s="87" t="s">
         <v>563</v>
       </c>
-      <c r="S85" s="93" t="s">
+      <c r="S85" s="89" t="s">
         <v>572</v>
       </c>
       <c r="T85" s="70">
@@ -8012,7 +7938,7 @@
       </c>
     </row>
     <row r="86" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="108" t="s">
+      <c r="B86" s="93" t="s">
         <v>3</v>
       </c>
       <c r="C86" s="66" t="s">
@@ -8021,39 +7947,39 @@
       <c r="D86" s="66" t="s">
         <v>552</v>
       </c>
-      <c r="E86" s="97" t="s">
+      <c r="E86" s="50" t="s">
         <v>577</v>
       </c>
-      <c r="F86" s="87">
+      <c r="F86" s="64">
         <v>1</v>
       </c>
-      <c r="G86" s="85">
+      <c r="G86" s="27">
         <v>1500000</v>
       </c>
-      <c r="H86" s="85"/>
-      <c r="I86" s="85">
+      <c r="H86" s="27"/>
+      <c r="I86" s="61">
         <v>1</v>
       </c>
       <c r="J86" s="85"/>
-      <c r="K86" s="92" t="s">
+      <c r="K86" s="88" t="s">
         <v>554</v>
       </c>
-      <c r="L86" s="92" t="s">
+      <c r="L86" s="88" t="s">
         <v>548</v>
       </c>
-      <c r="M86" s="86"/>
-      <c r="N86" s="86"/>
-      <c r="O86" s="86" t="s">
+      <c r="M86" s="62"/>
+      <c r="N86" s="62"/>
+      <c r="O86" s="28" t="s">
         <v>582</v>
       </c>
-      <c r="P86" s="86"/>
-      <c r="Q86" s="90" t="s">
+      <c r="P86" s="62"/>
+      <c r="Q86" s="86" t="s">
         <v>559</v>
       </c>
-      <c r="R86" s="91" t="s">
+      <c r="R86" s="87" t="s">
         <v>564</v>
       </c>
-      <c r="S86" s="94" t="s">
+      <c r="S86" s="90" t="s">
         <v>573</v>
       </c>
       <c r="T86" s="70">
@@ -8061,7 +7987,7 @@
       </c>
     </row>
     <row r="87" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="108" t="s">
+      <c r="B87" s="93" t="s">
         <v>3</v>
       </c>
       <c r="C87" s="66" t="s">
@@ -8070,39 +7996,39 @@
       <c r="D87" s="66" t="s">
         <v>552</v>
       </c>
-      <c r="E87" s="96" t="s">
+      <c r="E87" s="82" t="s">
         <v>578</v>
       </c>
-      <c r="F87" s="87">
+      <c r="F87" s="64">
         <v>2</v>
       </c>
-      <c r="G87" s="85"/>
-      <c r="H87" s="85">
+      <c r="G87" s="27"/>
+      <c r="H87" s="27">
         <v>75</v>
       </c>
-      <c r="I87" s="85">
+      <c r="I87" s="61">
         <v>4</v>
       </c>
       <c r="J87" s="85"/>
-      <c r="K87" s="92" t="s">
+      <c r="K87" s="88" t="s">
         <v>555</v>
       </c>
-      <c r="L87" s="92" t="s">
+      <c r="L87" s="88" t="s">
         <v>549</v>
       </c>
-      <c r="M87" s="86"/>
-      <c r="N87" s="86"/>
-      <c r="O87" s="99" t="s">
+      <c r="M87" s="62"/>
+      <c r="N87" s="62"/>
+      <c r="O87" s="84" t="s">
         <v>585</v>
       </c>
-      <c r="P87" s="86"/>
-      <c r="Q87" s="90" t="s">
+      <c r="P87" s="62"/>
+      <c r="Q87" s="86" t="s">
         <v>560</v>
       </c>
-      <c r="R87" s="91" t="s">
+      <c r="R87" s="87" t="s">
         <v>565</v>
       </c>
-      <c r="S87" s="94" t="s">
+      <c r="S87" s="90" t="s">
         <v>574</v>
       </c>
       <c r="T87" s="70">
@@ -8110,7 +8036,7 @@
       </c>
     </row>
     <row r="88" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="108" t="s">
+      <c r="B88" s="93" t="s">
         <v>3</v>
       </c>
       <c r="C88" s="66" t="s">
@@ -8119,39 +8045,39 @@
       <c r="D88" s="66" t="s">
         <v>552</v>
       </c>
-      <c r="E88" s="95" t="s">
+      <c r="E88" s="82" t="s">
         <v>579</v>
       </c>
-      <c r="F88" s="87">
-        <v>3</v>
-      </c>
-      <c r="G88" s="85"/>
-      <c r="H88" s="85">
+      <c r="F88" s="64">
+        <v>3</v>
+      </c>
+      <c r="G88" s="27"/>
+      <c r="H88" s="27">
         <v>80</v>
       </c>
-      <c r="I88" s="85">
+      <c r="I88" s="61">
         <v>7</v>
       </c>
       <c r="J88" s="85"/>
-      <c r="K88" s="92" t="s">
+      <c r="K88" s="88" t="s">
         <v>556</v>
       </c>
-      <c r="L88" s="92" t="s">
+      <c r="L88" s="88" t="s">
         <v>550</v>
       </c>
-      <c r="M88" s="86"/>
-      <c r="N88" s="86"/>
-      <c r="O88" s="86" t="s">
+      <c r="M88" s="62"/>
+      <c r="N88" s="62"/>
+      <c r="O88" s="28" t="s">
         <v>584</v>
       </c>
-      <c r="P88" s="86"/>
-      <c r="Q88" s="90" t="s">
+      <c r="P88" s="62"/>
+      <c r="Q88" s="86" t="s">
         <v>561</v>
       </c>
-      <c r="R88" s="91" t="s">
+      <c r="R88" s="87" t="s">
         <v>566</v>
       </c>
-      <c r="S88" s="94" t="s">
+      <c r="S88" s="90" t="s">
         <v>575</v>
       </c>
       <c r="T88" s="70">
@@ -8159,7 +8085,7 @@
       </c>
     </row>
     <row r="89" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="109" t="s">
+      <c r="B89" s="94" t="s">
         <v>3</v>
       </c>
       <c r="C89" s="77" t="s">
@@ -8168,226 +8094,226 @@
       <c r="D89" s="77" t="s">
         <v>552</v>
       </c>
-      <c r="E89" s="98" t="s">
+      <c r="E89" s="54" t="s">
         <v>580</v>
       </c>
-      <c r="F89" s="88">
+      <c r="F89" s="78">
         <v>4</v>
       </c>
-      <c r="G89" s="89"/>
-      <c r="H89" s="89">
+      <c r="G89" s="79"/>
+      <c r="H89" s="79">
         <v>85</v>
       </c>
-      <c r="I89" s="85">
+      <c r="I89" s="79">
         <v>10</v>
       </c>
-      <c r="J89" s="85"/>
-      <c r="K89" s="92" t="s">
+      <c r="J89" s="79"/>
+      <c r="K89" s="43" t="s">
         <v>557</v>
       </c>
-      <c r="L89" s="92" t="s">
+      <c r="L89" s="43" t="s">
         <v>551</v>
       </c>
-      <c r="M89" s="86"/>
-      <c r="N89" s="86"/>
-      <c r="O89" s="86" t="s">
+      <c r="M89" s="80"/>
+      <c r="N89" s="80"/>
+      <c r="O89" s="43" t="s">
         <v>583</v>
       </c>
-      <c r="P89" s="86"/>
-      <c r="Q89" s="90" t="s">
+      <c r="P89" s="80"/>
+      <c r="Q89" s="86" t="s">
         <v>562</v>
       </c>
-      <c r="R89" s="91" t="s">
+      <c r="R89" s="87" t="s">
         <v>567</v>
       </c>
-      <c r="S89" s="93" t="s">
+      <c r="S89" s="44" t="s">
         <v>576</v>
       </c>
       <c r="T89" s="70">
         <v>85</v>
       </c>
     </row>
-    <row r="90" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B90" s="105" t="s">
-        <v>3</v>
-      </c>
-      <c r="C90" s="23" t="s">
+    <row r="90" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B90" s="73" t="s">
+        <v>3</v>
+      </c>
+      <c r="C90" s="72" t="s">
         <v>586</v>
       </c>
-      <c r="D90" s="23" t="s">
+      <c r="D90" s="72" t="s">
         <v>590</v>
       </c>
-      <c r="E90" s="82"/>
+      <c r="E90" s="95"/>
       <c r="F90" s="64">
         <v>0</v>
       </c>
       <c r="G90" s="61"/>
       <c r="H90" s="61"/>
-      <c r="I90" s="61">
-        <v>0</v>
-      </c>
-      <c r="J90" s="61"/>
-      <c r="K90" s="28" t="s">
+      <c r="I90" s="96">
+        <v>0</v>
+      </c>
+      <c r="J90" s="96"/>
+      <c r="K90" s="91" t="s">
         <v>594</v>
       </c>
-      <c r="L90" s="28" t="s">
+      <c r="L90" s="91" t="s">
         <v>594</v>
       </c>
-      <c r="M90" s="62"/>
-      <c r="N90" s="62"/>
-      <c r="O90" s="28"/>
-      <c r="P90" s="62"/>
-      <c r="Q90" s="74" t="s">
+      <c r="M90" s="91"/>
+      <c r="N90" s="91"/>
+      <c r="O90" s="91"/>
+      <c r="P90" s="91"/>
+      <c r="Q90" s="97" t="s">
         <v>602</v>
       </c>
-      <c r="R90" s="30" t="s">
+      <c r="R90" s="98" t="s">
         <v>606</v>
       </c>
-      <c r="S90" s="30" t="s">
+      <c r="S90" s="100" t="s">
         <v>598</v>
       </c>
-      <c r="T90" s="102">
+      <c r="T90" s="103">
         <v>86</v>
       </c>
     </row>
-    <row r="91" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B91" s="106" t="s">
-        <v>3</v>
-      </c>
-      <c r="C91" s="59" t="s">
+    <row r="91" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B91" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="C91" s="66" t="s">
         <v>587</v>
       </c>
-      <c r="D91" s="23" t="s">
+      <c r="D91" s="66" t="s">
         <v>590</v>
       </c>
-      <c r="E91" s="82" t="s">
+      <c r="E91" s="95" t="s">
         <v>591</v>
       </c>
-      <c r="F91" s="111">
+      <c r="F91" s="64">
         <v>1</v>
       </c>
-      <c r="G91" s="100">
+      <c r="G91" s="27">
         <v>1800000</v>
       </c>
-      <c r="H91" s="100"/>
-      <c r="I91" s="61">
+      <c r="H91" s="27"/>
+      <c r="I91" s="96">
         <v>1</v>
       </c>
-      <c r="J91" s="61"/>
-      <c r="K91" s="28" t="s">
+      <c r="J91" s="96"/>
+      <c r="K91" s="91" t="s">
         <v>595</v>
       </c>
-      <c r="L91" s="28" t="s">
+      <c r="L91" s="91" t="s">
         <v>595</v>
       </c>
-      <c r="M91" s="62"/>
-      <c r="N91" s="62"/>
-      <c r="O91" s="28"/>
-      <c r="P91" s="62"/>
-      <c r="Q91" s="68" t="s">
+      <c r="M91" s="91"/>
+      <c r="N91" s="91"/>
+      <c r="O91" s="91"/>
+      <c r="P91" s="91"/>
+      <c r="Q91" s="97" t="s">
         <v>603</v>
       </c>
-      <c r="R91" s="58" t="s">
+      <c r="R91" s="98" t="s">
         <v>607</v>
       </c>
-      <c r="S91" s="58" t="s">
+      <c r="S91" s="101" t="s">
         <v>599</v>
       </c>
       <c r="T91" s="103">
         <v>87</v>
       </c>
     </row>
-    <row r="92" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B92" s="106" t="s">
-        <v>3</v>
-      </c>
-      <c r="C92" s="59" t="s">
+    <row r="92" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B92" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="C92" s="66" t="s">
         <v>588</v>
       </c>
-      <c r="D92" s="23" t="s">
+      <c r="D92" s="66" t="s">
         <v>590</v>
       </c>
-      <c r="E92" s="82" t="s">
+      <c r="E92" s="95" t="s">
         <v>592</v>
       </c>
       <c r="F92" s="64">
         <v>2</v>
       </c>
       <c r="G92" s="27"/>
-      <c r="H92" s="100">
+      <c r="H92" s="27">
         <v>75</v>
       </c>
-      <c r="I92" s="61">
+      <c r="I92" s="96">
         <v>4</v>
       </c>
-      <c r="J92" s="61"/>
-      <c r="K92" s="28" t="s">
+      <c r="J92" s="96"/>
+      <c r="K92" s="91" t="s">
         <v>596</v>
       </c>
-      <c r="L92" s="28" t="s">
+      <c r="L92" s="91" t="s">
         <v>596</v>
       </c>
-      <c r="M92" s="62"/>
-      <c r="N92" s="62"/>
-      <c r="O92" s="110"/>
-      <c r="P92" s="62"/>
-      <c r="Q92" s="68" t="s">
+      <c r="M92" s="91"/>
+      <c r="N92" s="91"/>
+      <c r="O92" s="91"/>
+      <c r="P92" s="91"/>
+      <c r="Q92" s="97" t="s">
         <v>604</v>
       </c>
-      <c r="R92" s="68" t="s">
+      <c r="R92" s="99" t="s">
         <v>608</v>
       </c>
-      <c r="S92" s="68" t="s">
+      <c r="S92" s="102" t="s">
         <v>600</v>
       </c>
       <c r="T92" s="103">
         <v>88</v>
       </c>
     </row>
-    <row r="93" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="112" t="s">
-        <v>3</v>
-      </c>
-      <c r="C93" s="77" t="s">
+    <row r="93" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B93" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="C93" s="66" t="s">
         <v>589</v>
       </c>
-      <c r="D93" s="77" t="s">
+      <c r="D93" s="66" t="s">
         <v>590</v>
       </c>
-      <c r="E93" s="54" t="s">
+      <c r="E93" s="95" t="s">
         <v>593</v>
       </c>
-      <c r="F93" s="78">
-        <v>3</v>
-      </c>
-      <c r="G93" s="79"/>
-      <c r="H93" s="101">
+      <c r="F93" s="64">
+        <v>3</v>
+      </c>
+      <c r="G93" s="27"/>
+      <c r="H93" s="27">
         <v>80</v>
       </c>
-      <c r="I93" s="79">
+      <c r="I93" s="96">
         <v>7</v>
       </c>
-      <c r="J93" s="79"/>
-      <c r="K93" s="43" t="s">
+      <c r="J93" s="96"/>
+      <c r="K93" s="91" t="s">
         <v>597</v>
       </c>
-      <c r="L93" s="43" t="s">
+      <c r="L93" s="91" t="s">
         <v>597</v>
       </c>
-      <c r="M93" s="80"/>
-      <c r="N93" s="80"/>
-      <c r="O93" s="43"/>
-      <c r="P93" s="80"/>
-      <c r="Q93" s="81" t="s">
+      <c r="M93" s="91"/>
+      <c r="N93" s="91"/>
+      <c r="O93" s="91"/>
+      <c r="P93" s="91"/>
+      <c r="Q93" s="104" t="s">
         <v>605</v>
       </c>
-      <c r="R93" s="45" t="s">
+      <c r="R93" s="105" t="s">
         <v>609</v>
       </c>
-      <c r="S93" s="44" t="s">
+      <c r="S93" s="100" t="s">
         <v>601</v>
       </c>
-      <c r="T93" s="104">
+      <c r="T93" s="103">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed Dragonjira disguises body parts
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\client_lfs\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\clientlfs\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="610">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="614">
   <si>
     <t>[sku]</t>
   </si>
@@ -1772,18 +1772,12 @@
     <t>FX_PF_Dragonjira_ElectricBody_Skin00;FX_PF_Dragonjira_Chest_Skin00;FX_PF_Dragonjira_Neck_Skin00;FX_PF_Dragonjira_Tail_Skin00</t>
   </si>
   <si>
-    <t>FX_PF_Dragonjira_ElectricBody_Skin01;FX_PF_Dragonjira_Chest_Skin01;FX_PF_Dragonjira_Neck_Skin01;FX_PF_Dragonjira_Tail_Skin01</t>
-  </si>
-  <si>
     <t>PF_spartan_hand;PF_spartan_chest;PF_spartan_spine;PF_spartan_head;PF_spartan_shield;PF_spartan_shield_china;PF_spartan_arm_R;PF_spartan_knee_L;PF_spartan_knee_R;FX_PF_Dragonjira_Neck_Skin04;FX_PF_Dragonjira_Tail_Skin04</t>
   </si>
   <si>
     <t>FX_PF_Dragonjira_ElectricBody_Skin03;FX_PF_Dragonjira_Chest_Skin03;FX_PF_Dragonjira_Tail_Skin03;PF_kawaii_hand;PF_kawaii_head;PF_kawaii_neck;PF_kawaii_tail;PF_kawaii_tail_04;PF_kawaii_torax</t>
   </si>
   <si>
-    <t>FX_PF_Dragonjira_ElectricBody_Skin02;FX_PF_Dragonjira_Chest_Skin02;FX_PF_Dragonjira_Neck_Skin02;FX_PF_Dragonjira_Tail_Skin02</t>
-  </si>
-  <si>
     <t>dragon_jade_0</t>
   </si>
   <si>
@@ -1854,6 +1848,24 @@
   </si>
   <si>
     <t>TID_DRAGON_JADE_3_DESC</t>
+  </si>
+  <si>
+    <t>PF_baseball_head;PF_baseball_hand;PF_baseball_ankle_LF;PF_baseball_ankle_RT;FX_PF_Dragonjira_ElectricBody_Skin01;FX_PF_Dragonjira_Chest_Skin01;FX_PF_Dragonjira_Neck_Skin01;FX_PF_Dragonjira_Tail_Skin01</t>
+  </si>
+  <si>
+    <t>PF_super_head;PF_super_chest;PF_super_torax;PF_super_tail_04;PF_super_arm_LF;PF_super_arm_RT;PF_super_tail_06;FX_PF_Dragonjira_ElectricBody_Skin02;FX_PF_Dragonjira_Neck_Skin02;FX_PF_Dragonjira_Tail_Skin02</t>
+  </si>
+  <si>
+    <t>FX_PF_JadeDragon_Skin00_Orb;PF_jade_0_bracelet_LF;PF_jade_0_bracelet_RT;PF_jade_0_chain;PF_jade_0_feet_LF;PF_jade_0_feet_RT;PF_jade_0_jacket;PF_jade_0_shoulder_LF;PF_jade_0_shoulder_RT;PF_jade_0_tail</t>
+  </si>
+  <si>
+    <t>FX_PF_JadeDragon_Skin01_Paper;PF_jade_1_shoulder_LF;PF_jade_1_shoulder_RT;PF_jade_1_belt;PF_jade_1_necklace</t>
+  </si>
+  <si>
+    <t>FX_PF_JadeDragon_Skin02_Smoke;FX_PF_JadeDragon_Skin02_Sparks_Left;FX_PF_JadeDragon_Skin02_Sparks_Right</t>
+  </si>
+  <si>
+    <t>FX_PF_JadeDragon_Skin03_Clouds;FX_PF_JadeDragon_Skin03_Sparks</t>
   </si>
 </sst>
 </file>
@@ -3363,13 +3375,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -3407,6 +3412,13 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -3456,7 +3468,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="disguisesDefinitions6" displayName="disguisesDefinitions6" ref="B4:T93" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" headerRowBorderDxfId="19" tableBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="disguisesDefinitions6" displayName="disguisesDefinitions6" ref="B4:T93" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19">
   <autoFilter ref="B4:T93"/>
   <sortState ref="B5:T46">
     <sortCondition ref="T4:T46"/>
@@ -3754,8 +3766,8 @@
   </sheetPr>
   <dimension ref="B1:T93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L64" workbookViewId="0">
-      <selection activeCell="Q91" sqref="Q91"/>
+    <sheetView tabSelected="1" topLeftCell="H64" workbookViewId="0">
+      <selection activeCell="O96" sqref="O96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7970,7 +7982,7 @@
       <c r="M86" s="62"/>
       <c r="N86" s="62"/>
       <c r="O86" s="28" t="s">
-        <v>582</v>
+        <v>608</v>
       </c>
       <c r="P86" s="62"/>
       <c r="Q86" s="86" t="s">
@@ -8019,7 +8031,7 @@
       <c r="M87" s="62"/>
       <c r="N87" s="62"/>
       <c r="O87" s="84" t="s">
-        <v>585</v>
+        <v>609</v>
       </c>
       <c r="P87" s="62"/>
       <c r="Q87" s="86" t="s">
@@ -8068,7 +8080,7 @@
       <c r="M88" s="62"/>
       <c r="N88" s="62"/>
       <c r="O88" s="28" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="P88" s="62"/>
       <c r="Q88" s="86" t="s">
@@ -8117,7 +8129,7 @@
       <c r="M89" s="80"/>
       <c r="N89" s="80"/>
       <c r="O89" s="43" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="P89" s="80"/>
       <c r="Q89" s="86" t="s">
@@ -8138,10 +8150,10 @@
         <v>3</v>
       </c>
       <c r="C90" s="72" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="D90" s="72" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="E90" s="95"/>
       <c r="F90" s="64">
@@ -8154,23 +8166,25 @@
       </c>
       <c r="J90" s="96"/>
       <c r="K90" s="91" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="L90" s="91" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="M90" s="91"/>
       <c r="N90" s="91"/>
-      <c r="O90" s="91"/>
+      <c r="O90" s="91" t="s">
+        <v>610</v>
+      </c>
       <c r="P90" s="91"/>
       <c r="Q90" s="97" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="R90" s="98" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="S90" s="100" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="T90" s="103">
         <v>86</v>
@@ -8181,13 +8195,13 @@
         <v>3</v>
       </c>
       <c r="C91" s="66" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="D91" s="66" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="E91" s="95" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="F91" s="64">
         <v>1</v>
@@ -8201,23 +8215,25 @@
       </c>
       <c r="J91" s="96"/>
       <c r="K91" s="91" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="L91" s="91" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="M91" s="91"/>
       <c r="N91" s="91"/>
-      <c r="O91" s="91"/>
+      <c r="O91" s="91" t="s">
+        <v>611</v>
+      </c>
       <c r="P91" s="91"/>
       <c r="Q91" s="97" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="R91" s="98" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="S91" s="101" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="T91" s="103">
         <v>87</v>
@@ -8228,13 +8244,13 @@
         <v>3</v>
       </c>
       <c r="C92" s="66" t="s">
+        <v>586</v>
+      </c>
+      <c r="D92" s="66" t="s">
         <v>588</v>
       </c>
-      <c r="D92" s="66" t="s">
+      <c r="E92" s="95" t="s">
         <v>590</v>
-      </c>
-      <c r="E92" s="95" t="s">
-        <v>592</v>
       </c>
       <c r="F92" s="64">
         <v>2</v>
@@ -8248,23 +8264,25 @@
       </c>
       <c r="J92" s="96"/>
       <c r="K92" s="91" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="L92" s="91" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="M92" s="91"/>
       <c r="N92" s="91"/>
-      <c r="O92" s="91"/>
+      <c r="O92" s="91" t="s">
+        <v>612</v>
+      </c>
       <c r="P92" s="91"/>
       <c r="Q92" s="97" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="R92" s="99" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="S92" s="102" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="T92" s="103">
         <v>88</v>
@@ -8275,13 +8293,13 @@
         <v>3</v>
       </c>
       <c r="C93" s="66" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="D93" s="66" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="E93" s="95" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="F93" s="64">
         <v>3</v>
@@ -8295,23 +8313,25 @@
       </c>
       <c r="J93" s="96"/>
       <c r="K93" s="91" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="L93" s="91" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="M93" s="91"/>
       <c r="N93" s="91"/>
-      <c r="O93" s="91"/>
+      <c r="O93" s="91" t="s">
+        <v>613</v>
+      </c>
       <c r="P93" s="91"/>
       <c r="Q93" s="104" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="R93" s="105" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="S93" s="100" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="T93" s="103">
         <v>89</v>

</xml_diff>

<commit_message>
Jade content disguises smoke added
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -1856,9 +1856,6 @@
     <t>PF_super_head;PF_super_chest;PF_super_torax;PF_super_tail_04;PF_super_arm_LF;PF_super_arm_RT;PF_super_tail_06;FX_PF_Dragonjira_ElectricBody_Skin02;FX_PF_Dragonjira_Neck_Skin02;FX_PF_Dragonjira_Tail_Skin02</t>
   </si>
   <si>
-    <t>FX_PF_JadeDragon_Skin00_Orb;PF_jade_0_bracelet_LF;PF_jade_0_bracelet_RT;PF_jade_0_chain;PF_jade_0_feet_LF;PF_jade_0_feet_RT;PF_jade_0_jacket;PF_jade_0_shoulder_LF;PF_jade_0_shoulder_RT;PF_jade_0_tail</t>
-  </si>
-  <si>
     <t>FX_PF_JadeDragon_Skin01_Paper;PF_jade_1_shoulder_LF;PF_jade_1_shoulder_RT;PF_jade_1_belt;PF_jade_1_necklace</t>
   </si>
   <si>
@@ -1866,6 +1863,9 @@
   </si>
   <si>
     <t>FX_PF_JadeDragon_Skin03_Clouds;FX_PF_JadeDragon_Skin03_Sparks</t>
+  </si>
+  <si>
+    <t>FX_PF_JadeDragon_Skin00_Orb;PF_jade_0_bracelet_LF;PF_jade_0_bracelet_RT;PF_jade_0_chain;PF_jade_0_feet_LF;PF_jade_0_feet_RT;PF_jade_0_jacket;PF_jade_0_shoulder_LF;PF_jade_0_shoulder_RT;PF_jade_0_tail;FX_PF_JadeDragon_Skin00_Smoke</t>
   </si>
 </sst>
 </file>
@@ -3766,8 +3766,8 @@
   </sheetPr>
   <dimension ref="B1:T93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="Q97" sqref="Q97"/>
+    <sheetView tabSelected="1" topLeftCell="G73" workbookViewId="0">
+      <selection activeCell="O90" sqref="O90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8174,7 +8174,7 @@
       <c r="M90" s="91"/>
       <c r="N90" s="91"/>
       <c r="O90" s="91" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="P90" s="91"/>
       <c r="Q90" s="97" t="s">
@@ -8223,7 +8223,7 @@
       <c r="M91" s="91"/>
       <c r="N91" s="91"/>
       <c r="O91" s="91" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="P91" s="91"/>
       <c r="Q91" s="97" t="s">
@@ -8272,7 +8272,7 @@
       <c r="M92" s="91"/>
       <c r="N92" s="91"/>
       <c r="O92" s="91" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="P92" s="91"/>
       <c r="Q92" s="97" t="s">
@@ -8321,7 +8321,7 @@
       <c r="M93" s="91"/>
       <c r="N93" s="91"/>
       <c r="O93" s="91" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="P93" s="91"/>
       <c r="Q93" s="104" t="s">

</xml_diff>

<commit_message>
JAde content disguises update (excel)
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -1859,13 +1859,13 @@
     <t>FX_PF_JadeDragon_Skin01_Paper;PF_jade_1_shoulder_LF;PF_jade_1_shoulder_RT;PF_jade_1_belt;PF_jade_1_necklace</t>
   </si>
   <si>
-    <t>FX_PF_JadeDragon_Skin02_Smoke;FX_PF_JadeDragon_Skin02_Sparks_Left;FX_PF_JadeDragon_Skin02_Sparks_Right</t>
-  </si>
-  <si>
-    <t>FX_PF_JadeDragon_Skin03_Clouds;FX_PF_JadeDragon_Skin03_Sparks</t>
-  </si>
-  <si>
     <t>FX_PF_JadeDragon_Skin00_Orb;PF_jade_0_bracelet_LF;PF_jade_0_bracelet_RT;PF_jade_0_chain;PF_jade_0_feet_LF;PF_jade_0_feet_RT;PF_jade_0_jacket;PF_jade_0_shoulder_LF;PF_jade_0_shoulder_RT;PF_jade_0_tail;FX_PF_JadeDragon_Skin00_Smoke</t>
+  </si>
+  <si>
+    <t>PF_jade_3_fringes;PF_jade_3_helmet;PF_jade_3_shinguard_LF;PF_jade_3_shinguard_RT;PF_jade_3_shoulderpad_LF;PF_jade_3_shoulderpad_RT;PF_jade_3_skirt;PF_jade_3_stick;PF_jade_3_tailpads;FX_PF_JadeDragon_Skin03_Clouds;FX_PF_JadeDragon_Skin03_Sparks</t>
+  </si>
+  <si>
+    <t>PF_jade_2_backspine1;PF_jade_2_backspine2;PF_jade_2_backspine3;PF_jade_2_bracelet_LF;PF_jade_2_bracelet_RT;PF_jade_2_feet_LF;PF_jade_2_feet_RT;PF_jade_2_horns;PF_jade_2_sidebuns;FX_PF_JadeDragon_Skin02_Smoke;FX_PF_JadeDragon_Skin02_Sparks_Left;FX_PF_JadeDragon_Skin02_Sparks_Right</t>
   </si>
 </sst>
 </file>
@@ -3767,7 +3767,7 @@
   <dimension ref="B1:T93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G73" workbookViewId="0">
-      <selection activeCell="O90" sqref="O90"/>
+      <selection activeCell="O92" sqref="O92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8173,8 +8173,8 @@
       </c>
       <c r="M90" s="91"/>
       <c r="N90" s="91"/>
-      <c r="O90" s="91" t="s">
-        <v>613</v>
+      <c r="O90" s="28" t="s">
+        <v>611</v>
       </c>
       <c r="P90" s="91"/>
       <c r="Q90" s="97" t="s">
@@ -8222,7 +8222,7 @@
       </c>
       <c r="M91" s="91"/>
       <c r="N91" s="91"/>
-      <c r="O91" s="91" t="s">
+      <c r="O91" s="28" t="s">
         <v>610</v>
       </c>
       <c r="P91" s="91"/>
@@ -8271,8 +8271,8 @@
       </c>
       <c r="M92" s="91"/>
       <c r="N92" s="91"/>
-      <c r="O92" s="91" t="s">
-        <v>611</v>
+      <c r="O92" s="28" t="s">
+        <v>613</v>
       </c>
       <c r="P92" s="91"/>
       <c r="Q92" s="97" t="s">
@@ -8320,7 +8320,7 @@
       </c>
       <c r="M93" s="91"/>
       <c r="N93" s="91"/>
-      <c r="O93" s="91" t="s">
+      <c r="O93" s="28" t="s">
         <v>612</v>
       </c>
       <c r="P93" s="91"/>

</xml_diff>

<commit_message>
Jade disguises content update (excel)
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_Disguises.xlsx
+++ b/Docs/Content/HungryDragonContent_Disguises.xlsx
@@ -1862,10 +1862,10 @@
     <t>FX_PF_JadeDragon_Skin00_Orb;PF_jade_0_bracelet_LF;PF_jade_0_bracelet_RT;PF_jade_0_chain;PF_jade_0_feet_LF;PF_jade_0_feet_RT;PF_jade_0_jacket;PF_jade_0_shoulder_LF;PF_jade_0_shoulder_RT;PF_jade_0_tail;FX_PF_JadeDragon_Skin00_Smoke</t>
   </si>
   <si>
-    <t>PF_jade_3_fringes;PF_jade_3_helmet;PF_jade_3_shinguard_LF;PF_jade_3_shinguard_RT;PF_jade_3_shoulderpad_LF;PF_jade_3_shoulderpad_RT;PF_jade_3_skirt;PF_jade_3_stick;PF_jade_3_tailpads;FX_PF_JadeDragon_Skin03_Clouds;FX_PF_JadeDragon_Skin03_Sparks</t>
-  </si>
-  <si>
     <t>PF_jade_2_backspine1;PF_jade_2_backspine2;PF_jade_2_backspine3;PF_jade_2_bracelet_LF;PF_jade_2_bracelet_RT;PF_jade_2_feet_LF;PF_jade_2_feet_RT;PF_jade_2_horns;PF_jade_2_sidebuns;FX_PF_JadeDragon_Skin02_Smoke;FX_PF_JadeDragon_Skin02_Sparks_Left;FX_PF_JadeDragon_Skin02_Sparks_Right</t>
+  </si>
+  <si>
+    <t>PF_jade_3_fringes;PF_jade_3_helmet;PF_jade_3_shinguard_LF;PF_jade_3_shinguard_RT;PF_jade_3_shoulderpad_LF;PF_jade_3_shoulderpad_RT;PF_jade_3_skirt;PF_jade_3_stick;PF_jade_3_tailpads;FX_PF_JadeDragon_Skin03_Clouds</t>
   </si>
 </sst>
 </file>
@@ -3767,7 +3767,7 @@
   <dimension ref="B1:T93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G73" workbookViewId="0">
-      <selection activeCell="O92" sqref="O92"/>
+      <selection activeCell="O93" sqref="O93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8272,7 +8272,7 @@
       <c r="M92" s="91"/>
       <c r="N92" s="91"/>
       <c r="O92" s="28" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="P92" s="91"/>
       <c r="Q92" s="97" t="s">
@@ -8321,7 +8321,7 @@
       <c r="M93" s="91"/>
       <c r="N93" s="91"/>
       <c r="O93" s="28" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="P93" s="91"/>
       <c r="Q93" s="104" t="s">

</xml_diff>